<commit_message>
GDE-7195 script changes to handle v1 and v2 endpoint for SBLC Issuance
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="5400" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="13" activeTab="17" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="13" activeTab="13" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -2417,9 +2417,9 @@
   </sheetPr>
   <dimension ref="A1:BQ7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC3_13092020190018</t>
+          <t>COMSEE_SC3_14092020203358</t>
         </is>
       </c>
       <c r="F2" s="38" t="inlineStr">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="BI2" s="1" t="inlineStr">
         <is>
-          <t>15-Oct-2021</t>
+          <t>16-Oct-2021</t>
         </is>
       </c>
       <c r="BJ2" s="41" t="inlineStr">
@@ -3168,6 +3168,341 @@
         </is>
       </c>
       <c r="BQ2" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_03</t>
+        </is>
+      </c>
+      <c r="C3" s="30" t="inlineStr">
+        <is>
+          <t>COMSEE_SC3_</t>
+        </is>
+      </c>
+      <c r="D3" s="30" t="inlineStr">
+        <is>
+          <t>CS3</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC3_14092020211728</t>
+        </is>
+      </c>
+      <c r="F3" s="38" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="G3" s="38" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="H3" s="38" t="inlineStr">
+        <is>
+          <t>Sales Group 1</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="J3" s="41" t="inlineStr">
+        <is>
+          <t>BLOGGS</t>
+        </is>
+      </c>
+      <c r="K3" s="75" t="inlineStr">
+        <is>
+          <t>Melbourne, VIC,Australia</t>
+        </is>
+      </c>
+      <c r="L3" s="41" t="inlineStr">
+        <is>
+          <t>Bloggs,  John</t>
+        </is>
+      </c>
+      <c r="M3" s="41" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="N3" s="38" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="O3" s="38" t="inlineStr">
+        <is>
+          <t>GCP</t>
+        </is>
+      </c>
+      <c r="P3" s="38" t="inlineStr">
+        <is>
+          <t>General Corp Purpose</t>
+        </is>
+      </c>
+      <c r="Q3" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="R3" s="40" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="S3" s="38" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="T3" s="38" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="U3" s="38" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="V3" s="38" t="inlineStr">
+        <is>
+          <t>CBA OBU AUD</t>
+        </is>
+      </c>
+      <c r="W3" s="38" t="inlineStr">
+        <is>
+          <t>CBA OBU USD</t>
+        </is>
+      </c>
+      <c r="X3" s="38" t="n"/>
+      <c r="Y3" s="38" t="inlineStr">
+        <is>
+          <t>1,000,000.00</t>
+        </is>
+      </c>
+      <c r="Z3" s="38" t="inlineStr">
+        <is>
+          <t>BG_COL</t>
+        </is>
+      </c>
+      <c r="AA3" s="38" t="inlineStr">
+        <is>
+          <t>Sydney, Australia</t>
+        </is>
+      </c>
+      <c r="AB3" s="40" t="inlineStr">
+        <is>
+          <t>BBSW - Mid</t>
+        </is>
+      </c>
+      <c r="AC3" s="40" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="AD3" s="41" t="inlineStr">
+        <is>
+          <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
+        </is>
+      </c>
+      <c r="AE3" s="38" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AF3" s="38" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AG3" s="38" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AH3" s="41" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AI3" s="41" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AJ3" s="41" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AK3" s="41" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AL3" s="38" t="inlineStr">
+        <is>
+          <t>Start of current cycle</t>
+        </is>
+      </c>
+      <c r="AM3" s="30" t="inlineStr">
+        <is>
+          <t>Start of next interest cycle</t>
+        </is>
+      </c>
+      <c r="AN3" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO3" s="38" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="AP3" s="38" t="inlineStr">
+        <is>
+          <t>Effective date of change</t>
+        </is>
+      </c>
+      <c r="AQ3" s="38" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AR3" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS3" s="30" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="AT3" s="38" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="AU3" s="38" t="inlineStr">
+        <is>
+          <t>BG_COL</t>
+        </is>
+      </c>
+      <c r="AV3" s="38" t="inlineStr">
+        <is>
+          <t>Corporate Lending</t>
+        </is>
+      </c>
+      <c r="AW3" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="AX3" s="38" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="AY3" s="38" t="inlineStr">
+        <is>
+          <t>IT_COL</t>
+        </is>
+      </c>
+      <c r="AZ3" s="30" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="BA3" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="BB3" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="BC3" s="30" t="inlineStr">
+        <is>
+          <t>CBA as Primary Lender</t>
+        </is>
+      </c>
+      <c r="BD3" s="38" t="inlineStr">
+        <is>
+          <t>Business Verification,${SPACE}${SPACE}BVT</t>
+        </is>
+      </c>
+      <c r="BE3" s="30" t="inlineStr">
+        <is>
+          <t>OL</t>
+        </is>
+      </c>
+      <c r="BF3" s="38" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="BG3" s="38" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="BH3" s="38" t="inlineStr">
+        <is>
+          <t>1,000,000.00</t>
+        </is>
+      </c>
+      <c r="BI3" s="1" t="inlineStr">
+        <is>
+          <t>16-Oct-2021</t>
+        </is>
+      </c>
+      <c r="BJ3" s="41" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="BK3" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="BL3" s="41" t="inlineStr">
+        <is>
+          <t>Loan,${SPACE}${SPACE}Operations</t>
+        </is>
+      </c>
+      <c r="BM3" s="41" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="BN3" s="41" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="BO3" s="41" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="BP3" s="41" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="BQ3" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
@@ -3205,13 +3540,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3345,12 +3680,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC3_13092020190018</t>
+          <t>COMSEE_SC3_14092020203358</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>COMSEEFACBG_13092020190727</t>
+          <t>COMSEEFACBG_14092020204147</t>
         </is>
       </c>
       <c r="E2" s="30" t="inlineStr">
@@ -3424,6 +3759,103 @@
         </is>
       </c>
       <c r="S2" s="40" t="inlineStr">
+        <is>
+          <t>US Dollar</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_03</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC3_14092020211728</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEEFACBG_14092020212610</t>
+        </is>
+      </c>
+      <c r="E3" s="30" t="inlineStr">
+        <is>
+          <t>COMSEEFACBG_</t>
+        </is>
+      </c>
+      <c r="F3" s="30" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="G3" s="40" t="inlineStr">
+        <is>
+          <t>Bank Guarantee</t>
+        </is>
+      </c>
+      <c r="H3" s="47" t="inlineStr">
+        <is>
+          <t>1,000,000.00</t>
+        </is>
+      </c>
+      <c r="I3" s="40" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="J3" s="47" t="inlineStr">
+        <is>
+          <t>08-May-2018</t>
+        </is>
+      </c>
+      <c r="K3" s="30" t="inlineStr">
+        <is>
+          <t>31-Jan-2019</t>
+        </is>
+      </c>
+      <c r="L3" s="47" t="inlineStr">
+        <is>
+          <t>08-May-2019</t>
+        </is>
+      </c>
+      <c r="M3" s="47" t="inlineStr">
+        <is>
+          <t>08-May-2019</t>
+        </is>
+      </c>
+      <c r="N3" s="40" t="inlineStr">
+        <is>
+          <t>Financial Letter of Credit</t>
+        </is>
+      </c>
+      <c r="O3" s="38" t="inlineStr">
+        <is>
+          <t>Acquisition</t>
+        </is>
+      </c>
+      <c r="P3" s="47" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="Q3" s="40" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="R3" s="47" t="inlineStr">
+        <is>
+          <t>Australian Dollar</t>
+        </is>
+      </c>
+      <c r="S3" s="40" t="inlineStr">
         <is>
           <t>US Dollar</t>
         </is>
@@ -3442,13 +3874,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3634,6 +4066,88 @@
         </is>
       </c>
     </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_03</t>
+        </is>
+      </c>
+      <c r="C3" s="40" t="inlineStr">
+        <is>
+          <t>Fee on Lender Shares</t>
+        </is>
+      </c>
+      <c r="D3" s="40" t="inlineStr">
+        <is>
+          <t>Issuance Fee (BG/LC)</t>
+        </is>
+      </c>
+      <c r="E3" s="38" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="F3" s="38" t="inlineStr">
+        <is>
+          <t>FormulaCategory</t>
+        </is>
+      </c>
+      <c r="G3" s="47" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="H3" s="47" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="I3" s="47" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="J3" s="47" t="inlineStr">
+        <is>
+          <t>4.000000</t>
+        </is>
+      </c>
+      <c r="K3" s="38" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+      <c r="L3" s="30" t="inlineStr">
+        <is>
+          <t>Option</t>
+        </is>
+      </c>
+      <c r="M3" s="38" t="inlineStr">
+        <is>
+          <t>BBSW - Mid</t>
+        </is>
+      </c>
+      <c r="N3" s="30" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="O3" s="30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="P3" s="30" t="inlineStr">
+        <is>
+          <t>BBSW</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -3647,11 +4161,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY5"/>
+  <dimension ref="A1:AZ5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X2" sqref="X2"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3659,47 +4173,47 @@
     <col width="6.140625" customWidth="1" style="30" min="1" max="1"/>
     <col width="38.140625" customWidth="1" style="30" min="2" max="2"/>
     <col width="40.7109375" customWidth="1" style="30" min="3" max="3"/>
-    <col width="15" customWidth="1" style="30" min="4" max="4"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="30" min="4" max="4"/>
     <col width="8.28515625" customWidth="1" style="30" min="5" max="5"/>
-    <col width="19.42578125" customWidth="1" style="30" min="6" max="7"/>
-    <col width="21" customWidth="1" style="30" min="8" max="9"/>
-    <col width="23.85546875" customWidth="1" style="30" min="10" max="11"/>
-    <col width="28.7109375" customWidth="1" style="30" min="12" max="12"/>
-    <col width="27.85546875" customWidth="1" style="30" min="13" max="13"/>
-    <col width="36.140625" customWidth="1" style="30" min="14" max="14"/>
-    <col width="31.42578125" customWidth="1" style="30" min="15" max="17"/>
-    <col width="21.42578125" customWidth="1" style="30" min="18" max="19"/>
-    <col width="25.140625" customWidth="1" style="30" min="20" max="20"/>
-    <col width="26" customWidth="1" style="30" min="21" max="21"/>
-    <col width="33.140625" customWidth="1" style="30" min="22" max="22"/>
-    <col width="30.7109375" customWidth="1" style="30" min="23" max="23"/>
-    <col width="36.28515625" bestFit="1" customWidth="1" style="30" min="24" max="24"/>
-    <col width="28" customWidth="1" style="30" min="25" max="25"/>
-    <col width="34" customWidth="1" style="30" min="26" max="26"/>
-    <col width="33.28515625" customWidth="1" style="30" min="27" max="27"/>
-    <col width="31.85546875" customWidth="1" style="30" min="28" max="28"/>
-    <col width="26.28515625" customWidth="1" style="30" min="29" max="29"/>
-    <col width="26.42578125" customWidth="1" style="30" min="30" max="30"/>
-    <col width="30.42578125" customWidth="1" style="30" min="31" max="31"/>
-    <col width="25.85546875" customWidth="1" style="30" min="32" max="32"/>
-    <col width="19.42578125" customWidth="1" style="30" min="33" max="33"/>
-    <col width="21.5703125" customWidth="1" style="30" min="34" max="34"/>
-    <col width="27.5703125" customWidth="1" style="30" min="35" max="35"/>
-    <col width="11.42578125" customWidth="1" style="30" min="36" max="36"/>
-    <col width="36" customWidth="1" style="30" min="37" max="37"/>
-    <col width="20.85546875" customWidth="1" style="30" min="38" max="38"/>
-    <col width="18.85546875" customWidth="1" style="30" min="39" max="39"/>
-    <col width="23.42578125" customWidth="1" style="30" min="40" max="40"/>
-    <col width="22.42578125" customWidth="1" style="30" min="41" max="41"/>
-    <col width="16.7109375" customWidth="1" style="30" min="42" max="42"/>
-    <col width="17" customWidth="1" style="30" min="43" max="43"/>
-    <col width="18.85546875" customWidth="1" style="30" min="44" max="44"/>
-    <col width="17.5703125" customWidth="1" style="30" min="45" max="45"/>
-    <col width="17.28515625" customWidth="1" style="30" min="46" max="46"/>
-    <col width="23.42578125" customWidth="1" style="30" min="47" max="47"/>
-    <col width="36.7109375" customWidth="1" style="30" min="48" max="48"/>
-    <col width="35.85546875" customWidth="1" style="30" min="49" max="49"/>
-    <col width="26.5703125" customWidth="1" style="30" min="50" max="51"/>
+    <col width="19.42578125" customWidth="1" style="30" min="6" max="8"/>
+    <col width="21" customWidth="1" style="30" min="9" max="10"/>
+    <col width="23.85546875" customWidth="1" style="30" min="11" max="12"/>
+    <col width="28.7109375" customWidth="1" style="30" min="13" max="13"/>
+    <col width="27.85546875" customWidth="1" style="30" min="14" max="14"/>
+    <col width="36.140625" customWidth="1" style="30" min="15" max="15"/>
+    <col width="31.42578125" customWidth="1" style="30" min="16" max="18"/>
+    <col width="21.42578125" customWidth="1" style="30" min="19" max="20"/>
+    <col width="25.140625" customWidth="1" style="30" min="21" max="21"/>
+    <col width="26" customWidth="1" style="30" min="22" max="22"/>
+    <col width="33.140625" customWidth="1" style="30" min="23" max="23"/>
+    <col width="30.7109375" customWidth="1" style="30" min="24" max="24"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="30" min="25" max="25"/>
+    <col width="28" customWidth="1" style="30" min="26" max="26"/>
+    <col width="34" customWidth="1" style="30" min="27" max="27"/>
+    <col width="33.28515625" customWidth="1" style="30" min="28" max="28"/>
+    <col width="31.85546875" customWidth="1" style="30" min="29" max="29"/>
+    <col width="26.28515625" customWidth="1" style="30" min="30" max="30"/>
+    <col width="26.42578125" customWidth="1" style="30" min="31" max="31"/>
+    <col width="30.42578125" customWidth="1" style="30" min="32" max="32"/>
+    <col width="25.85546875" customWidth="1" style="30" min="33" max="33"/>
+    <col width="19.42578125" customWidth="1" style="30" min="34" max="34"/>
+    <col width="21.5703125" customWidth="1" style="30" min="35" max="35"/>
+    <col width="27.5703125" customWidth="1" style="30" min="36" max="36"/>
+    <col width="11.42578125" customWidth="1" style="30" min="37" max="37"/>
+    <col width="36" customWidth="1" style="30" min="38" max="38"/>
+    <col width="20.85546875" customWidth="1" style="30" min="39" max="39"/>
+    <col width="18.85546875" customWidth="1" style="30" min="40" max="40"/>
+    <col width="23.42578125" customWidth="1" style="30" min="41" max="41"/>
+    <col width="22.42578125" customWidth="1" style="30" min="42" max="42"/>
+    <col width="16.7109375" customWidth="1" style="30" min="43" max="43"/>
+    <col width="17" customWidth="1" style="30" min="44" max="44"/>
+    <col width="18.85546875" customWidth="1" style="30" min="45" max="45"/>
+    <col width="17.5703125" customWidth="1" style="30" min="46" max="46"/>
+    <col width="17.28515625" customWidth="1" style="30" min="47" max="47"/>
+    <col width="23.42578125" customWidth="1" style="30" min="48" max="48"/>
+    <col width="36.7109375" customWidth="1" style="30" min="49" max="49"/>
+    <col width="35.85546875" customWidth="1" style="30" min="50" max="50"/>
+    <col width="26.5703125" customWidth="1" style="30" min="51" max="52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="150">
@@ -3735,225 +4249,230 @@
       </c>
       <c r="G1" s="56" t="inlineStr">
         <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="H1" s="56" t="inlineStr">
+        <is>
           <t>Fee_Name</t>
         </is>
       </c>
-      <c r="H1" s="56" t="inlineStr">
+      <c r="I1" s="56" t="inlineStr">
         <is>
           <t>Fee_FeeAlias</t>
         </is>
       </c>
-      <c r="I1" s="56" t="inlineStr">
+      <c r="J1" s="56" t="inlineStr">
         <is>
           <t>Fee_Status</t>
         </is>
       </c>
-      <c r="J1" s="56" t="inlineStr">
+      <c r="K1" s="56" t="inlineStr">
         <is>
           <t>Fee_Type</t>
         </is>
       </c>
-      <c r="K1" s="56" t="inlineStr">
+      <c r="L1" s="56" t="inlineStr">
         <is>
           <t>Fee_Currency</t>
         </is>
       </c>
-      <c r="L1" s="56" t="inlineStr">
+      <c r="M1" s="56" t="inlineStr">
         <is>
           <t>Fee_CurrentRate</t>
         </is>
       </c>
-      <c r="M1" s="56" t="inlineStr">
+      <c r="N1" s="56" t="inlineStr">
         <is>
           <t>Fee_EffectiveDate</t>
         </is>
       </c>
-      <c r="N1" s="56" t="inlineStr">
+      <c r="O1" s="56" t="inlineStr">
         <is>
           <t>Fee_ExpiryDate</t>
         </is>
       </c>
-      <c r="O1" s="56" t="inlineStr">
+      <c r="P1" s="56" t="inlineStr">
         <is>
           <t>Fee_DueDate</t>
         </is>
       </c>
-      <c r="P1" s="56" t="inlineStr">
+      <c r="Q1" s="56" t="inlineStr">
         <is>
           <t>Fee_AccruedToDate</t>
         </is>
       </c>
-      <c r="Q1" s="56" t="inlineStr">
+      <c r="R1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Alias</t>
         </is>
       </c>
-      <c r="R1" s="56" t="inlineStr">
+      <c r="S1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RiskType</t>
         </is>
       </c>
-      <c r="S1" s="56" t="inlineStr">
+      <c r="T1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="T1" s="56" t="inlineStr">
+      <c r="U1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_EffectiveDate</t>
         </is>
       </c>
-      <c r="U1" s="56" t="inlineStr">
+      <c r="V1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetAmount</t>
         </is>
       </c>
-      <c r="V1" s="56" t="inlineStr">
+      <c r="W1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetFacCCYAmount</t>
         </is>
       </c>
-      <c r="W1" s="56" t="inlineStr">
+      <c r="X1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_MaturityExpiryDate</t>
         </is>
       </c>
-      <c r="X1" s="77" t="inlineStr">
+      <c r="Y1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Favouree</t>
         </is>
       </c>
-      <c r="Y1" s="56" t="inlineStr">
+      <c r="Z1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBGrossAmount</t>
         </is>
       </c>
-      <c r="Z1" s="56" t="inlineStr">
+      <c r="AA1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalOriginalAmount</t>
         </is>
       </c>
-      <c r="AA1" s="56" t="inlineStr">
+      <c r="AB1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalCurrentAmount</t>
         </is>
       </c>
-      <c r="AB1" s="56" t="inlineStr">
+      <c r="AC1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingFrequency</t>
         </is>
       </c>
-      <c r="AC1" s="56" t="inlineStr">
+      <c r="AD1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingDate</t>
         </is>
       </c>
-      <c r="AD1" s="56" t="inlineStr">
+      <c r="AE1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PaymentMode</t>
         </is>
       </c>
-      <c r="AE1" s="56" t="inlineStr">
+      <c r="AF1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="AF1" s="56" t="inlineStr">
+      <c r="AG1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PricingOption</t>
         </is>
       </c>
-      <c r="AG1" s="56" t="inlineStr">
+      <c r="AH1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Margin</t>
         </is>
       </c>
-      <c r="AH1" s="56" t="inlineStr">
+      <c r="AI1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AllInRate</t>
         </is>
       </c>
-      <c r="AI1" s="56" t="inlineStr">
+      <c r="AJ1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AccruedInterest</t>
         </is>
       </c>
-      <c r="AJ1" s="78" t="inlineStr">
+      <c r="AK1" s="78" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="AK1" s="77" t="inlineStr">
+      <c r="AL1" s="77" t="inlineStr">
         <is>
           <t>OutstandingSelect_Type</t>
         </is>
       </c>
-      <c r="AL1" s="78" t="inlineStr">
+      <c r="AM1" s="78" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="AM1" s="77" t="inlineStr">
+      <c r="AN1" s="77" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
       </c>
-      <c r="AN1" s="77" t="inlineStr">
+      <c r="AO1" s="77" t="inlineStr">
         <is>
           <t>Amount_Requested</t>
         </is>
       </c>
-      <c r="AO1" s="77" t="inlineStr">
+      <c r="AP1" s="77" t="inlineStr">
         <is>
           <t>Issuance_Fee</t>
         </is>
       </c>
-      <c r="AP1" s="77" t="inlineStr">
+      <c r="AQ1" s="77" t="inlineStr">
         <is>
           <t>SBLC_Status</t>
         </is>
       </c>
-      <c r="AQ1" s="77" t="inlineStr">
+      <c r="AR1" s="77" t="inlineStr">
         <is>
           <t>Cycle_Frequency</t>
         </is>
       </c>
-      <c r="AR1" s="77" t="inlineStr">
+      <c r="AS1" s="77" t="inlineStr">
         <is>
           <t>SBLC_ExpiryDate</t>
         </is>
       </c>
-      <c r="AS1" s="77" t="inlineStr">
+      <c r="AT1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Alias</t>
         </is>
       </c>
-      <c r="AT1" s="77" t="inlineStr">
+      <c r="AU1" s="77" t="inlineStr">
         <is>
           <t>Cycle_Number</t>
         </is>
       </c>
-      <c r="AU1" s="77" t="inlineStr">
+      <c r="AV1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Type</t>
         </is>
       </c>
-      <c r="AV1" s="77" t="inlineStr">
+      <c r="AW1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Type</t>
         </is>
       </c>
-      <c r="AW1" s="77" t="inlineStr">
+      <c r="AX1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Status_Awaiting_Approval</t>
         </is>
       </c>
-      <c r="AX1" s="77" t="inlineStr">
+      <c r="AY1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Status_Awaiting_Release</t>
         </is>
       </c>
-      <c r="AY1" s="150" t="inlineStr">
+      <c r="AZ1" s="150" t="inlineStr">
         <is>
           <t>AccrualRule_PayInAdvance</t>
         </is>
@@ -3977,12 +4496,12 @@
       </c>
       <c r="D2" s="10" t="inlineStr">
         <is>
-          <t>COM_RES_03</t>
+          <t>COM_RES_03_V1</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>3000652</t>
+          <t>3000670</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -3992,177 +4511,390 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>60000764</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>60000786</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>Issuance Fee (BG/LC)</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>2020-10-15</t>
-        </is>
-      </c>
       <c r="N2" s="1" t="inlineStr">
         <is>
-          <t>2020-10-21</t>
+          <t>2020-10-16</t>
         </is>
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>2020-10-15</t>
+          <t>2020-10-22</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
+          <t>2020-10-16</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
+      <c r="S2" s="1" t="inlineStr">
         <is>
           <t>Financial Letter of Credit</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
-        <is>
-          <t>2020-10-15</t>
-        </is>
-      </c>
       <c r="U2" s="1" t="inlineStr">
         <is>
+          <t>2020-10-16</t>
+        </is>
+      </c>
+      <c r="V2" s="1" t="inlineStr">
+        <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
-        <is>
-          <t>2021-10-15</t>
-        </is>
-      </c>
-      <c r="X2" s="38" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
+        <is>
+          <t>2021-10-18</t>
+        </is>
+      </c>
+      <c r="Y2" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="Z2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AA2" s="1" t="inlineStr">
+      <c r="AB2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AB2" s="79" t="n"/>
       <c r="AC2" s="79" t="n"/>
-      <c r="AJ2" s="1" t="inlineStr">
-        <is>
-          <t>COMSEE_SC3_13092020190018</t>
-        </is>
-      </c>
-      <c r="AK2" s="40" t="inlineStr">
+      <c r="AD2" s="79" t="n"/>
+      <c r="AK2" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC3_14092020203358</t>
+        </is>
+      </c>
+      <c r="AL2" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AL2" s="1" t="inlineStr">
-        <is>
-          <t>COMSEEFACBG_13092020190727</t>
-        </is>
-      </c>
-      <c r="AM2" s="40" t="inlineStr">
+      <c r="AM2" s="1" t="inlineStr">
+        <is>
+          <t>COMSEEFACBG_14092020204147</t>
+        </is>
+      </c>
+      <c r="AN2" s="40" t="inlineStr">
         <is>
           <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
         </is>
       </c>
-      <c r="AN2" s="40" t="n">
+      <c r="AO2" s="40" t="n">
         <v>1000</v>
       </c>
-      <c r="AO2" s="40" t="inlineStr">
+      <c r="AP2" s="40" t="inlineStr">
         <is>
           <t>Outstandings  X Rate (4%)</t>
         </is>
       </c>
-      <c r="AP2" s="40" t="inlineStr">
+      <c r="AQ2" s="40" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
       </c>
-      <c r="AQ2" s="40" t="inlineStr">
+      <c r="AR2" s="40" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="AR2" s="1" t="inlineStr">
-        <is>
-          <t>15-Oct-2021</t>
-        </is>
-      </c>
-      <c r="AS2" s="30" t="inlineStr">
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>16-Oct-2021</t>
+        </is>
+      </c>
+      <c r="AT2" s="30" t="inlineStr">
         <is>
           <t>ESPS11112500003</t>
         </is>
       </c>
-      <c r="AT2" s="30" t="inlineStr">
+      <c r="AU2" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AU2" s="40" t="inlineStr">
+      <c r="AV2" s="40" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AV2" s="40" t="inlineStr">
+      <c r="AW2" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee Issuance</t>
         </is>
       </c>
-      <c r="AW2" s="40" t="inlineStr">
+      <c r="AX2" s="40" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AX2" s="40" t="inlineStr">
+      <c r="AY2" s="40" t="inlineStr">
         <is>
           <t>Awaiting Release</t>
         </is>
       </c>
-      <c r="AY2" s="40" t="inlineStr">
+      <c r="AZ2" s="40" t="inlineStr">
         <is>
           <t>Pay In Advance</t>
         </is>
       </c>
     </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_03</t>
+        </is>
+      </c>
+      <c r="C3" s="10" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>COM_RES_03_V2</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>3000671</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>60000787</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>Issuance Fee (BG/LC)</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-16</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-22</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-16</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>Financial Letter of Credit</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-16</t>
+        </is>
+      </c>
+      <c r="V3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="W3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="X3" s="1" t="inlineStr">
+        <is>
+          <t>2021-10-18</t>
+        </is>
+      </c>
+      <c r="Y3" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="Z3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="AA3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="AB3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="AC3" s="79" t="n"/>
+      <c r="AD3" s="79" t="n"/>
+      <c r="AK3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC3_14092020211728</t>
+        </is>
+      </c>
+      <c r="AL3" s="40" t="inlineStr">
+        <is>
+          <t>SBLC/Guarantee</t>
+        </is>
+      </c>
+      <c r="AM3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEEFACBG_14092020212610</t>
+        </is>
+      </c>
+      <c r="AN3" s="40" t="inlineStr">
+        <is>
+          <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
+        </is>
+      </c>
+      <c r="AO3" s="40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AP3" s="40" t="inlineStr">
+        <is>
+          <t>Outstandings  X Rate (4%)</t>
+        </is>
+      </c>
+      <c r="AQ3" s="40" t="inlineStr">
+        <is>
+          <t>Awaiting release</t>
+        </is>
+      </c>
+      <c r="AR3" s="40" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="AS3" s="1" t="inlineStr">
+        <is>
+          <t>16-Oct-2021</t>
+        </is>
+      </c>
+      <c r="AT3" s="30" t="inlineStr">
+        <is>
+          <t>ESPS11112500003</t>
+        </is>
+      </c>
+      <c r="AU3" s="30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AV3" s="40" t="inlineStr">
+        <is>
+          <t>Outstandings</t>
+        </is>
+      </c>
+      <c r="AW3" s="40" t="inlineStr">
+        <is>
+          <t>SBLC/Guarantee Issuance</t>
+        </is>
+      </c>
+      <c r="AX3" s="40" t="inlineStr">
+        <is>
+          <t>Awaiting Approval</t>
+        </is>
+      </c>
+      <c r="AY3" s="40" t="inlineStr">
+        <is>
+          <t>Awaiting Release</t>
+        </is>
+      </c>
+      <c r="AZ3" s="40" t="inlineStr">
+        <is>
+          <t>Pay In Advance</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
     <row r="5">
-      <c r="AQ5" s="49" t="n"/>
+      <c r="AR5" s="49" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -4177,11 +4909,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EO2"/>
+  <dimension ref="A1:EP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AW2" sqref="AW2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4191,135 +4923,135 @@
     <col width="36.42578125" customWidth="1" style="30" min="3" max="3"/>
     <col width="15" customWidth="1" style="30" min="4" max="4"/>
     <col width="8.140625" customWidth="1" style="30" min="5" max="5"/>
-    <col width="19.7109375" customWidth="1" style="30" min="6" max="7"/>
-    <col width="17.42578125" customWidth="1" style="30" min="8" max="9"/>
-    <col width="9.85546875" customWidth="1" style="30" min="10" max="10"/>
-    <col width="13.7109375" customWidth="1" style="30" min="11" max="11"/>
-    <col width="18" customWidth="1" style="30" min="12" max="12"/>
-    <col width="17.5703125" customWidth="1" style="30" min="13" max="13"/>
-    <col width="15.42578125" customWidth="1" style="30" min="14" max="14"/>
-    <col width="13.28515625" customWidth="1" style="30" min="15" max="15"/>
-    <col width="19.5703125" customWidth="1" style="30" min="16" max="17"/>
-    <col width="21.42578125" customWidth="1" style="30" min="18" max="19"/>
-    <col width="25.140625" customWidth="1" style="30" min="20" max="20"/>
-    <col width="26" customWidth="1" style="30" min="21" max="21"/>
-    <col width="33.140625" customWidth="1" style="30" min="22" max="22"/>
-    <col width="30.7109375" customWidth="1" style="30" min="23" max="23"/>
-    <col width="21.85546875" customWidth="1" style="30" min="24" max="24"/>
-    <col width="28" customWidth="1" style="30" min="25" max="25"/>
-    <col width="34" customWidth="1" style="30" min="26" max="26"/>
-    <col width="33.28515625" customWidth="1" style="30" min="27" max="27"/>
-    <col width="31.85546875" customWidth="1" style="30" min="28" max="28"/>
-    <col width="26.28515625" customWidth="1" style="30" min="29" max="29"/>
-    <col width="26.42578125" customWidth="1" style="30" min="30" max="30"/>
-    <col width="30.42578125" customWidth="1" style="30" min="31" max="31"/>
-    <col width="25.85546875" customWidth="1" style="30" min="32" max="32"/>
-    <col width="19.42578125" customWidth="1" style="30" min="33" max="33"/>
-    <col width="21.5703125" customWidth="1" style="30" min="34" max="34"/>
-    <col width="27.5703125" customWidth="1" style="30" min="35" max="35"/>
-    <col width="34.7109375" customWidth="1" style="30" min="36" max="36"/>
-    <col width="33.85546875" customWidth="1" style="30" min="37" max="38"/>
-    <col width="21.42578125" customWidth="1" style="30" min="39" max="39"/>
-    <col width="29.140625" customWidth="1" style="30" min="40" max="40"/>
-    <col width="34" customWidth="1" style="30" min="41" max="41"/>
-    <col width="31.5703125" customWidth="1" style="30" min="42" max="42"/>
-    <col width="15.140625" customWidth="1" style="30" min="43" max="43"/>
-    <col width="11.28515625" customWidth="1" style="30" min="44" max="44"/>
-    <col width="18" customWidth="1" style="30" min="45" max="45"/>
-    <col width="15.5703125" customWidth="1" style="30" min="46" max="46"/>
-    <col width="15.7109375" customWidth="1" style="30" min="47" max="47"/>
-    <col width="16.5703125" customWidth="1" style="30" min="48" max="48"/>
-    <col width="41.85546875" customWidth="1" style="30" min="49" max="49"/>
-    <col width="22.140625" customWidth="1" style="30" min="50" max="50"/>
-    <col width="21.85546875" customWidth="1" style="30" min="51" max="51"/>
-    <col width="25.140625" customWidth="1" style="30" min="52" max="52"/>
-    <col width="22.42578125" customWidth="1" style="30" min="53" max="53"/>
-    <col width="27.5703125" customWidth="1" style="30" min="54" max="54"/>
-    <col width="23.42578125" customWidth="1" style="30" min="55" max="55"/>
-    <col width="29.140625" customWidth="1" style="30" min="56" max="56"/>
-    <col width="39.7109375" customWidth="1" style="30" min="57" max="57"/>
-    <col width="19" customWidth="1" style="30" min="58" max="58"/>
-    <col width="32.42578125" customWidth="1" style="30" min="59" max="59"/>
-    <col width="17.28515625" customWidth="1" style="30" min="60" max="60"/>
-    <col width="28.7109375" customWidth="1" style="30" min="61" max="61"/>
-    <col width="23.5703125" customWidth="1" style="30" min="62" max="62"/>
-    <col width="45.28515625" customWidth="1" style="30" min="63" max="63"/>
-    <col width="29.85546875" customWidth="1" style="30" min="64" max="64"/>
-    <col width="14.28515625" customWidth="1" style="30" min="65" max="65"/>
-    <col width="23" customWidth="1" style="30" min="66" max="66"/>
-    <col width="19.85546875" customWidth="1" style="30" min="67" max="70"/>
-    <col width="24.7109375" customWidth="1" style="30" min="71" max="72"/>
-    <col width="25" customWidth="1" style="30" min="73" max="73"/>
-    <col width="24.42578125" customWidth="1" style="30" min="74" max="74"/>
-    <col width="30.42578125" customWidth="1" style="30" min="75" max="75"/>
-    <col width="36" customWidth="1" style="30" min="76" max="76"/>
-    <col width="34.42578125" customWidth="1" style="30" min="77" max="77"/>
-    <col width="26.7109375" customWidth="1" style="30" min="78" max="78"/>
-    <col width="17.28515625" customWidth="1" style="30" min="79" max="80"/>
-    <col width="34.140625" customWidth="1" style="30" min="81" max="81"/>
-    <col width="28.42578125" customWidth="1" style="30" min="82" max="82"/>
-    <col width="24.7109375" customWidth="1" style="30" min="83" max="83"/>
-    <col width="30.28515625" customWidth="1" style="30" min="84" max="84"/>
-    <col width="17.5703125" customWidth="1" style="30" min="85" max="85"/>
-    <col width="20.28515625" customWidth="1" style="30" min="86" max="86"/>
-    <col width="12.140625" customWidth="1" style="30" min="87" max="87"/>
-    <col width="21.42578125" customWidth="1" style="30" min="88" max="88"/>
-    <col width="24.140625" customWidth="1" style="30" min="89" max="89"/>
-    <col width="16" customWidth="1" style="30" min="90" max="90"/>
-    <col width="14" customWidth="1" style="30" min="91" max="91"/>
-    <col width="16.7109375" customWidth="1" style="30" min="92" max="92"/>
-    <col width="10" customWidth="1" style="30" min="93" max="93"/>
-    <col width="8.5703125" customWidth="1" style="30" min="94" max="94"/>
-    <col width="19.140625" customWidth="1" style="30" min="95" max="95"/>
-    <col width="37.7109375" customWidth="1" style="30" min="96" max="96"/>
-    <col width="15.85546875" customWidth="1" style="30" min="97" max="97"/>
-    <col width="9.28515625" customWidth="1" style="30" min="98" max="98"/>
-    <col width="16.7109375" customWidth="1" style="30" min="99" max="100"/>
-    <col width="12.85546875" customWidth="1" style="30" min="101" max="101"/>
-    <col width="32.42578125" customWidth="1" style="30" min="102" max="102"/>
-    <col width="11.7109375" customWidth="1" style="30" min="103" max="103"/>
-    <col width="35" customWidth="1" style="30" min="104" max="104"/>
-    <col width="18.140625" customWidth="1" style="30" min="105" max="105"/>
-    <col width="15.7109375" customWidth="1" style="30" min="106" max="106"/>
-    <col width="24" customWidth="1" style="30" min="107" max="107"/>
-    <col width="11.5703125" customWidth="1" style="30" min="108" max="108"/>
-    <col width="8.28515625" customWidth="1" style="30" min="109" max="109"/>
-    <col width="16.5703125" customWidth="1" style="30" min="110" max="110"/>
-    <col width="32.85546875" customWidth="1" style="30" min="111" max="111"/>
-    <col width="18.7109375" customWidth="1" style="30" min="112" max="112"/>
-    <col width="18.28515625" customWidth="1" style="30" min="113" max="113"/>
-    <col width="10.42578125" customWidth="1" style="30" min="114" max="114"/>
-    <col width="9.7109375" customWidth="1" style="30" min="115" max="115"/>
-    <col width="12.7109375" customWidth="1" style="30" min="116" max="116"/>
-    <col width="11.7109375" customWidth="1" style="30" min="117" max="117"/>
-    <col width="24" customWidth="1" style="30" min="118" max="118"/>
-    <col width="43.7109375" customWidth="1" style="30" min="119" max="119"/>
-    <col width="44.85546875" customWidth="1" style="30" min="120" max="120"/>
-    <col width="30.140625" customWidth="1" style="30" min="121" max="121"/>
-    <col width="29.42578125" customWidth="1" style="30" min="122" max="122"/>
-    <col width="25.28515625" customWidth="1" style="30" min="123" max="123"/>
-    <col width="9.5703125" customWidth="1" style="30" min="124" max="124"/>
-    <col width="25.7109375" customWidth="1" style="30" min="125" max="125"/>
-    <col width="19.7109375" customWidth="1" style="30" min="126" max="126"/>
-    <col width="28.5703125" customWidth="1" style="30" min="127" max="127"/>
-    <col width="21.140625" customWidth="1" style="30" min="128" max="128"/>
-    <col width="14.5703125" customWidth="1" style="30" min="129" max="129"/>
-    <col width="20.5703125" customWidth="1" style="30" min="130" max="130"/>
-    <col width="18.28515625" customWidth="1" style="30" min="131" max="131"/>
-    <col width="18.85546875" customWidth="1" style="30" min="132" max="132"/>
-    <col width="35" customWidth="1" style="30" min="133" max="133"/>
-    <col width="20" customWidth="1" style="30" min="134" max="134"/>
-    <col width="32.42578125" customWidth="1" style="30" min="135" max="135"/>
-    <col width="21.5703125" customWidth="1" style="30" min="136" max="136"/>
-    <col width="13.5703125" customWidth="1" style="30" min="137" max="137"/>
-    <col width="26.28515625" customWidth="1" style="30" min="138" max="138"/>
-    <col width="19.140625" customWidth="1" style="30" min="139" max="139"/>
-    <col width="44" customWidth="1" style="30" min="140" max="140"/>
-    <col width="23.5703125" customWidth="1" style="30" min="141" max="141"/>
-    <col width="26.28515625" customWidth="1" style="30" min="142" max="142"/>
-    <col width="34.85546875" customWidth="1" style="30" min="143" max="143"/>
-    <col width="9.140625" customWidth="1" style="30" min="144" max="144"/>
-    <col width="15.85546875" customWidth="1" style="30" min="145" max="145"/>
+    <col width="19.7109375" customWidth="1" style="30" min="6" max="8"/>
+    <col width="17.42578125" customWidth="1" style="30" min="9" max="10"/>
+    <col width="9.85546875" customWidth="1" style="30" min="11" max="11"/>
+    <col width="13.7109375" customWidth="1" style="30" min="12" max="12"/>
+    <col width="18" customWidth="1" style="30" min="13" max="13"/>
+    <col width="17.5703125" customWidth="1" style="30" min="14" max="14"/>
+    <col width="15.42578125" customWidth="1" style="30" min="15" max="15"/>
+    <col width="13.28515625" customWidth="1" style="30" min="16" max="16"/>
+    <col width="19.5703125" customWidth="1" style="30" min="17" max="18"/>
+    <col width="21.42578125" customWidth="1" style="30" min="19" max="20"/>
+    <col width="25.140625" customWidth="1" style="30" min="21" max="21"/>
+    <col width="26" customWidth="1" style="30" min="22" max="22"/>
+    <col width="33.140625" customWidth="1" style="30" min="23" max="23"/>
+    <col width="30.7109375" customWidth="1" style="30" min="24" max="24"/>
+    <col width="21.85546875" customWidth="1" style="30" min="25" max="25"/>
+    <col width="28" customWidth="1" style="30" min="26" max="26"/>
+    <col width="34" customWidth="1" style="30" min="27" max="27"/>
+    <col width="33.28515625" customWidth="1" style="30" min="28" max="28"/>
+    <col width="31.85546875" customWidth="1" style="30" min="29" max="29"/>
+    <col width="26.28515625" customWidth="1" style="30" min="30" max="30"/>
+    <col width="26.42578125" customWidth="1" style="30" min="31" max="31"/>
+    <col width="30.42578125" customWidth="1" style="30" min="32" max="32"/>
+    <col width="25.85546875" customWidth="1" style="30" min="33" max="33"/>
+    <col width="19.42578125" customWidth="1" style="30" min="34" max="34"/>
+    <col width="21.5703125" customWidth="1" style="30" min="35" max="35"/>
+    <col width="27.5703125" customWidth="1" style="30" min="36" max="36"/>
+    <col width="34.7109375" customWidth="1" style="30" min="37" max="37"/>
+    <col width="33.85546875" customWidth="1" style="30" min="38" max="39"/>
+    <col width="21.42578125" customWidth="1" style="30" min="40" max="40"/>
+    <col width="29.140625" customWidth="1" style="30" min="41" max="41"/>
+    <col width="34" customWidth="1" style="30" min="42" max="42"/>
+    <col width="31.5703125" customWidth="1" style="30" min="43" max="43"/>
+    <col width="15.140625" customWidth="1" style="30" min="44" max="44"/>
+    <col width="11.28515625" customWidth="1" style="30" min="45" max="45"/>
+    <col width="18" customWidth="1" style="30" min="46" max="46"/>
+    <col width="15.5703125" customWidth="1" style="30" min="47" max="47"/>
+    <col width="15.7109375" customWidth="1" style="30" min="48" max="48"/>
+    <col width="16.5703125" customWidth="1" style="30" min="49" max="49"/>
+    <col width="41.85546875" customWidth="1" style="30" min="50" max="50"/>
+    <col width="22.140625" customWidth="1" style="30" min="51" max="51"/>
+    <col width="21.85546875" customWidth="1" style="30" min="52" max="52"/>
+    <col width="25.140625" customWidth="1" style="30" min="53" max="53"/>
+    <col width="22.42578125" customWidth="1" style="30" min="54" max="54"/>
+    <col width="27.5703125" customWidth="1" style="30" min="55" max="55"/>
+    <col width="23.42578125" customWidth="1" style="30" min="56" max="56"/>
+    <col width="29.140625" customWidth="1" style="30" min="57" max="57"/>
+    <col width="39.7109375" customWidth="1" style="30" min="58" max="58"/>
+    <col width="19" customWidth="1" style="30" min="59" max="59"/>
+    <col width="32.42578125" customWidth="1" style="30" min="60" max="60"/>
+    <col width="17.28515625" customWidth="1" style="30" min="61" max="61"/>
+    <col width="28.7109375" customWidth="1" style="30" min="62" max="62"/>
+    <col width="23.5703125" customWidth="1" style="30" min="63" max="63"/>
+    <col width="45.28515625" customWidth="1" style="30" min="64" max="64"/>
+    <col width="29.85546875" customWidth="1" style="30" min="65" max="65"/>
+    <col width="14.28515625" customWidth="1" style="30" min="66" max="66"/>
+    <col width="23" customWidth="1" style="30" min="67" max="67"/>
+    <col width="19.85546875" customWidth="1" style="30" min="68" max="71"/>
+    <col width="24.7109375" customWidth="1" style="30" min="72" max="73"/>
+    <col width="25" customWidth="1" style="30" min="74" max="74"/>
+    <col width="24.42578125" customWidth="1" style="30" min="75" max="75"/>
+    <col width="30.42578125" customWidth="1" style="30" min="76" max="76"/>
+    <col width="36" customWidth="1" style="30" min="77" max="77"/>
+    <col width="34.42578125" customWidth="1" style="30" min="78" max="78"/>
+    <col width="26.7109375" customWidth="1" style="30" min="79" max="79"/>
+    <col width="17.28515625" customWidth="1" style="30" min="80" max="81"/>
+    <col width="34.140625" customWidth="1" style="30" min="82" max="82"/>
+    <col width="28.42578125" customWidth="1" style="30" min="83" max="83"/>
+    <col width="24.7109375" customWidth="1" style="30" min="84" max="84"/>
+    <col width="30.28515625" customWidth="1" style="30" min="85" max="85"/>
+    <col width="17.5703125" customWidth="1" style="30" min="86" max="86"/>
+    <col width="20.28515625" customWidth="1" style="30" min="87" max="87"/>
+    <col width="12.140625" customWidth="1" style="30" min="88" max="88"/>
+    <col width="21.42578125" customWidth="1" style="30" min="89" max="89"/>
+    <col width="24.140625" customWidth="1" style="30" min="90" max="90"/>
+    <col width="16" customWidth="1" style="30" min="91" max="91"/>
+    <col width="14" customWidth="1" style="30" min="92" max="92"/>
+    <col width="16.7109375" customWidth="1" style="30" min="93" max="93"/>
+    <col width="10" customWidth="1" style="30" min="94" max="94"/>
+    <col width="8.5703125" customWidth="1" style="30" min="95" max="95"/>
+    <col width="19.140625" customWidth="1" style="30" min="96" max="96"/>
+    <col width="37.7109375" customWidth="1" style="30" min="97" max="97"/>
+    <col width="15.85546875" customWidth="1" style="30" min="98" max="98"/>
+    <col width="9.28515625" customWidth="1" style="30" min="99" max="99"/>
+    <col width="16.7109375" customWidth="1" style="30" min="100" max="101"/>
+    <col width="12.85546875" customWidth="1" style="30" min="102" max="102"/>
+    <col width="32.42578125" customWidth="1" style="30" min="103" max="103"/>
+    <col width="11.7109375" customWidth="1" style="30" min="104" max="104"/>
+    <col width="35" customWidth="1" style="30" min="105" max="105"/>
+    <col width="18.140625" customWidth="1" style="30" min="106" max="106"/>
+    <col width="15.7109375" customWidth="1" style="30" min="107" max="107"/>
+    <col width="24" customWidth="1" style="30" min="108" max="108"/>
+    <col width="11.5703125" customWidth="1" style="30" min="109" max="109"/>
+    <col width="8.28515625" customWidth="1" style="30" min="110" max="110"/>
+    <col width="16.5703125" customWidth="1" style="30" min="111" max="111"/>
+    <col width="32.85546875" customWidth="1" style="30" min="112" max="112"/>
+    <col width="18.7109375" customWidth="1" style="30" min="113" max="113"/>
+    <col width="18.28515625" customWidth="1" style="30" min="114" max="114"/>
+    <col width="10.42578125" customWidth="1" style="30" min="115" max="115"/>
+    <col width="9.7109375" customWidth="1" style="30" min="116" max="116"/>
+    <col width="12.7109375" customWidth="1" style="30" min="117" max="117"/>
+    <col width="11.7109375" customWidth="1" style="30" min="118" max="118"/>
+    <col width="24" customWidth="1" style="30" min="119" max="119"/>
+    <col width="43.7109375" customWidth="1" style="30" min="120" max="120"/>
+    <col width="44.85546875" customWidth="1" style="30" min="121" max="121"/>
+    <col width="30.140625" customWidth="1" style="30" min="122" max="122"/>
+    <col width="29.42578125" customWidth="1" style="30" min="123" max="123"/>
+    <col width="25.28515625" customWidth="1" style="30" min="124" max="124"/>
+    <col width="9.5703125" customWidth="1" style="30" min="125" max="125"/>
+    <col width="25.7109375" customWidth="1" style="30" min="126" max="126"/>
+    <col width="19.7109375" customWidth="1" style="30" min="127" max="127"/>
+    <col width="28.5703125" customWidth="1" style="30" min="128" max="128"/>
+    <col width="21.140625" customWidth="1" style="30" min="129" max="129"/>
+    <col width="14.5703125" customWidth="1" style="30" min="130" max="130"/>
+    <col width="20.5703125" customWidth="1" style="30" min="131" max="131"/>
+    <col width="18.28515625" customWidth="1" style="30" min="132" max="132"/>
+    <col width="18.85546875" customWidth="1" style="30" min="133" max="133"/>
+    <col width="35" customWidth="1" style="30" min="134" max="134"/>
+    <col width="20" customWidth="1" style="30" min="135" max="135"/>
+    <col width="32.42578125" customWidth="1" style="30" min="136" max="136"/>
+    <col width="21.5703125" customWidth="1" style="30" min="137" max="137"/>
+    <col width="13.5703125" customWidth="1" style="30" min="138" max="138"/>
+    <col width="26.28515625" customWidth="1" style="30" min="139" max="139"/>
+    <col width="19.140625" customWidth="1" style="30" min="140" max="140"/>
+    <col width="44" customWidth="1" style="30" min="141" max="141"/>
+    <col width="23.5703125" customWidth="1" style="30" min="142" max="142"/>
+    <col width="26.28515625" customWidth="1" style="30" min="143" max="143"/>
+    <col width="34.85546875" customWidth="1" style="30" min="144" max="144"/>
+    <col width="9.140625" customWidth="1" style="30" min="145" max="145"/>
+    <col width="15.85546875" customWidth="1" style="30" min="146" max="146"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="50" thickBot="1">
@@ -4355,261 +5087,265 @@
       </c>
       <c r="G1" s="56" t="inlineStr">
         <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="H1" s="56" t="inlineStr">
+        <is>
           <t>Fee_Name</t>
         </is>
       </c>
-      <c r="H1" s="56" t="inlineStr">
+      <c r="I1" s="56" t="inlineStr">
         <is>
           <t>Fee_FeeAlias</t>
         </is>
       </c>
-      <c r="I1" s="56" t="inlineStr">
+      <c r="J1" s="56" t="inlineStr">
         <is>
           <t>Fee_Status</t>
         </is>
       </c>
-      <c r="J1" s="56" t="inlineStr">
+      <c r="K1" s="56" t="inlineStr">
         <is>
           <t>Fee_Type</t>
         </is>
       </c>
-      <c r="K1" s="56" t="inlineStr">
+      <c r="L1" s="56" t="inlineStr">
         <is>
           <t>Fee_Currency</t>
         </is>
       </c>
-      <c r="L1" s="56" t="inlineStr">
+      <c r="M1" s="56" t="inlineStr">
         <is>
           <t>Fee_CurrentRate</t>
         </is>
       </c>
-      <c r="M1" s="56" t="inlineStr">
+      <c r="N1" s="56" t="inlineStr">
         <is>
           <t>Fee_EffectiveDate</t>
         </is>
       </c>
-      <c r="N1" s="56" t="inlineStr">
+      <c r="O1" s="56" t="inlineStr">
         <is>
           <t>Fee_ExpiryDate</t>
         </is>
       </c>
-      <c r="O1" s="56" t="inlineStr">
+      <c r="P1" s="56" t="inlineStr">
         <is>
           <t>Fee_DueDate</t>
         </is>
       </c>
-      <c r="P1" s="56" t="inlineStr">
+      <c r="Q1" s="56" t="inlineStr">
         <is>
           <t>Fee_AccruedToDate</t>
         </is>
       </c>
-      <c r="Q1" s="56" t="inlineStr">
+      <c r="R1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Alias</t>
         </is>
       </c>
-      <c r="R1" s="56" t="inlineStr">
+      <c r="S1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RiskType</t>
         </is>
       </c>
-      <c r="S1" s="56" t="inlineStr">
+      <c r="T1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="T1" s="56" t="inlineStr">
+      <c r="U1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_EffectiveDate</t>
         </is>
       </c>
-      <c r="U1" s="56" t="inlineStr">
+      <c r="V1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetAmount</t>
         </is>
       </c>
-      <c r="V1" s="56" t="inlineStr">
+      <c r="W1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetFacCCYAmount</t>
         </is>
       </c>
-      <c r="W1" s="56" t="inlineStr">
+      <c r="X1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_MaturityExpiryDate</t>
         </is>
       </c>
-      <c r="X1" s="77" t="inlineStr">
+      <c r="Y1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Favouree</t>
         </is>
       </c>
-      <c r="Y1" s="56" t="inlineStr">
+      <c r="Z1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBGrossAmount</t>
         </is>
       </c>
-      <c r="Z1" s="56" t="inlineStr">
+      <c r="AA1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalOriginalAmount</t>
         </is>
       </c>
-      <c r="AA1" s="56" t="inlineStr">
+      <c r="AB1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalCurrentAmount</t>
         </is>
       </c>
-      <c r="AB1" s="56" t="inlineStr">
+      <c r="AC1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingFrequency</t>
         </is>
       </c>
-      <c r="AC1" s="56" t="inlineStr">
+      <c r="AD1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingDate</t>
         </is>
       </c>
-      <c r="AD1" s="56" t="inlineStr">
+      <c r="AE1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PaymentMode</t>
         </is>
       </c>
-      <c r="AE1" s="56" t="inlineStr">
+      <c r="AF1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="AF1" s="56" t="inlineStr">
+      <c r="AG1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PricingOption</t>
         </is>
       </c>
-      <c r="AG1" s="56" t="inlineStr">
+      <c r="AH1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Margin</t>
         </is>
       </c>
-      <c r="AH1" s="56" t="inlineStr">
+      <c r="AI1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AllInRate</t>
         </is>
       </c>
-      <c r="AI1" s="56" t="inlineStr">
+      <c r="AJ1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AccruedInterest</t>
         </is>
       </c>
-      <c r="AJ1" s="77" t="inlineStr">
+      <c r="AK1" s="77" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="AK1" s="77" t="inlineStr">
+      <c r="AL1" s="77" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="AL1" s="77" t="inlineStr">
+      <c r="AM1" s="77" t="inlineStr">
         <is>
           <t>OutstandingSelect_Type</t>
         </is>
       </c>
-      <c r="AM1" s="77" t="inlineStr">
+      <c r="AN1" s="77" t="inlineStr">
         <is>
           <t>Borrower1_ShortName</t>
         </is>
       </c>
-      <c r="AN1" s="77" t="inlineStr">
+      <c r="AO1" s="77" t="inlineStr">
         <is>
           <t>Computed_ProjectedCycleDue</t>
         </is>
       </c>
-      <c r="AO1" s="77" t="inlineStr">
+      <c r="AP1" s="77" t="inlineStr">
         <is>
           <t>IssuanceFeePayment_EffectiveDate</t>
         </is>
       </c>
-      <c r="AP1" s="77" t="inlineStr">
+      <c r="AQ1" s="77" t="inlineStr">
         <is>
           <t>SBLCFeePayment_NoticeMethod</t>
         </is>
       </c>
-      <c r="AQ1" s="81" t="inlineStr">
+      <c r="AR1" s="81" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="AR1" s="81" t="inlineStr">
+      <c r="AS1" s="81" t="inlineStr">
         <is>
           <t>Search_By</t>
         </is>
       </c>
-      <c r="AS1" s="77" t="inlineStr">
+      <c r="AT1" s="77" t="inlineStr">
         <is>
           <t>CycleNumber</t>
         </is>
       </c>
-      <c r="AT1" s="44" t="inlineStr">
+      <c r="AU1" s="44" t="inlineStr">
         <is>
           <t>Workflow_Item</t>
         </is>
       </c>
-      <c r="AU1" s="44" t="inlineStr">
+      <c r="AV1" s="44" t="inlineStr">
         <is>
           <t>LIQCustomer_ID</t>
         </is>
       </c>
-      <c r="AV1" s="44" t="inlineStr">
+      <c r="AW1" s="44" t="inlineStr">
         <is>
           <t>Borrower_Profile</t>
         </is>
       </c>
-      <c r="AW1" s="71" t="inlineStr">
+      <c r="AX1" s="71" t="inlineStr">
         <is>
           <t>RemittanceInstruction_RTGSDescriptionAUD</t>
         </is>
       </c>
-      <c r="AX1" s="71" t="inlineStr">
+      <c r="AY1" s="71" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
       </c>
-      <c r="AY1" s="44" t="inlineStr">
+      <c r="AZ1" s="44" t="inlineStr">
         <is>
           <t>HostBankSharePct</t>
         </is>
       </c>
-      <c r="AZ1" s="44" t="inlineStr">
+      <c r="BA1" s="44" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="BA1" s="44" t="inlineStr">
+      <c r="BB1" s="44" t="inlineStr">
         <is>
           <t>Servicing_Alias</t>
         </is>
       </c>
-      <c r="BB1" s="44" t="inlineStr">
+      <c r="BC1" s="44" t="inlineStr">
         <is>
           <t>Servicing_Name</t>
         </is>
       </c>
-      <c r="BC1" s="44" t="inlineStr">
+      <c r="BD1" s="44" t="inlineStr">
         <is>
           <t>Servicing_Location</t>
         </is>
       </c>
-      <c r="BD1" s="71" t="inlineStr">
+      <c r="BE1" s="71" t="inlineStr">
         <is>
           <t>Computed_ProjectedCycleDue</t>
         </is>
       </c>
-      <c r="BE1" s="71" t="inlineStr">
+      <c r="BF1" s="71" t="inlineStr">
         <is>
           <t>Host_Bank</t>
         </is>
       </c>
-      <c r="BH1" s="150" t="n"/>
-      <c r="CP1" s="80" t="n"/>
+      <c r="BI1" s="150" t="n"/>
       <c r="CQ1" s="80" t="n"/>
       <c r="CR1" s="80" t="n"/>
       <c r="CS1" s="80" t="n"/>
@@ -4661,6 +5397,7 @@
       <c r="EM1" s="80" t="n"/>
       <c r="EN1" s="80" t="n"/>
       <c r="EO1" s="80" t="n"/>
+      <c r="EP1" s="80" t="n"/>
     </row>
     <row r="2" ht="15" customFormat="1" customHeight="1" s="82">
       <c r="A2" s="30" t="inlineStr">
@@ -4680,12 +5417,12 @@
       </c>
       <c r="D2" s="10" t="inlineStr">
         <is>
-          <t>COM_RES_PAY_03</t>
+          <t>COM_RES_PAY_03_V1</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>3000652</t>
+          <t>3000670</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -4695,102 +5432,106 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>60000764</t>
-        </is>
-      </c>
-      <c r="H2" s="30" t="n"/>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>60000786</t>
+        </is>
+      </c>
       <c r="I2" s="30" t="n"/>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="J2" s="30" t="n"/>
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>Issuance Fee (BG/LC)</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>2020-10-15</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>2020-10-21</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>2020-10-15</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>0.11</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>60000764</t>
-        </is>
-      </c>
       <c r="R2" s="1" t="inlineStr">
         <is>
+          <t>60000786</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
           <t>Financial Letter of Credit</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>2020-10-15</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>2021-10-15</t>
         </is>
       </c>
-      <c r="X2" s="38" t="inlineStr">
+      <c r="Y2" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="Z2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AA2" s="1" t="inlineStr">
+      <c r="AB2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AB2" s="30" t="n"/>
       <c r="AC2" s="30" t="n"/>
       <c r="AD2" s="30" t="n"/>
       <c r="AE2" s="30" t="n"/>
@@ -4798,113 +5539,113 @@
       <c r="AG2" s="30" t="n"/>
       <c r="AH2" s="30" t="n"/>
       <c r="AI2" s="30" t="n"/>
-      <c r="AJ2" s="1" t="inlineStr">
-        <is>
-          <t>COMSEE_SC3_13092020190018</t>
-        </is>
-      </c>
+      <c r="AJ2" s="30" t="n"/>
       <c r="AK2" s="1" t="inlineStr">
         <is>
-          <t>COMSEEFACBG_13092020190727</t>
+          <t>COMSEE_SC3_14092020203358</t>
         </is>
       </c>
       <c r="AL2" s="1" t="inlineStr">
         <is>
+          <t>COMSEEFACBG_14092020204147</t>
+        </is>
+      </c>
+      <c r="AM2" s="1" t="inlineStr">
+        <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AM2" s="1" t="inlineStr">
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>BORROWER1111</t>
         </is>
       </c>
-      <c r="AN2" s="1" t="n">
+      <c r="AO2" s="1" t="n">
         <v>0.11</v>
       </c>
-      <c r="AO2" s="30" t="inlineStr">
+      <c r="AP2" s="30" t="inlineStr">
         <is>
           <t>17-Sep-2018</t>
         </is>
       </c>
-      <c r="AP2" s="82" t="inlineStr">
+      <c r="AQ2" s="82" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="AQ2" s="82" t="inlineStr">
+      <c r="AR2" s="82" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AR2" s="82" t="inlineStr">
+      <c r="AS2" s="82" t="inlineStr">
         <is>
           <t>Deal/Facility</t>
         </is>
       </c>
-      <c r="AS2" s="83" t="inlineStr">
+      <c r="AT2" s="83" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AT2" s="30" t="inlineStr">
+      <c r="AU2" s="30" t="inlineStr">
         <is>
           <t>Create Cashflows</t>
         </is>
       </c>
-      <c r="AU2" s="30" t="inlineStr">
+      <c r="AV2" s="30" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="AV2" s="30" t="inlineStr">
+      <c r="AW2" s="30" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="AW2" s="1" t="inlineStr">
+      <c r="AX2" s="1" t="inlineStr">
         <is>
           <t>RTGS1</t>
         </is>
       </c>
-      <c r="AX2" s="1" t="inlineStr">
+      <c r="AY2" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AY2" s="30" t="inlineStr">
+      <c r="AZ2" s="30" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="AZ2" s="30" t="inlineStr">
+      <c r="BA2" s="30" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="BA2" s="30" t="inlineStr">
+      <c r="BB2" s="30" t="inlineStr">
         <is>
           <t>JB</t>
         </is>
       </c>
-      <c r="BB2" s="30" t="inlineStr">
+      <c r="BC2" s="30" t="inlineStr">
         <is>
           <t>BLOGGS</t>
         </is>
       </c>
-      <c r="BC2" s="30" t="inlineStr">
+      <c r="BD2" s="30" t="inlineStr">
         <is>
           <t>Melbourne, VIC,Australia</t>
         </is>
       </c>
-      <c r="BD2" s="30" t="n">
+      <c r="BE2" s="30" t="n">
         <v>0.33</v>
       </c>
-      <c r="BE2" s="30" t="inlineStr">
+      <c r="BF2" s="30" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/IT_AKD</t>
         </is>
       </c>
-      <c r="BF2" s="83" t="n"/>
       <c r="BG2" s="83" t="n"/>
       <c r="BH2" s="83" t="n"/>
       <c r="BI2" s="83" t="n"/>
@@ -4912,21 +5653,21 @@
       <c r="BK2" s="83" t="n"/>
       <c r="BL2" s="83" t="n"/>
       <c r="BM2" s="83" t="n"/>
-      <c r="BO2" s="83" t="n"/>
+      <c r="BN2" s="83" t="n"/>
       <c r="BP2" s="83" t="n"/>
       <c r="BQ2" s="83" t="n"/>
-      <c r="BS2" s="83" t="n"/>
+      <c r="BR2" s="83" t="n"/>
       <c r="BT2" s="83" t="n"/>
       <c r="BU2" s="83" t="n"/>
       <c r="BV2" s="83" t="n"/>
       <c r="BW2" s="83" t="n"/>
       <c r="BX2" s="83" t="n"/>
-      <c r="CA2" s="83" t="n"/>
-      <c r="CC2" s="83" t="n"/>
+      <c r="BY2" s="83" t="n"/>
+      <c r="CB2" s="83" t="n"/>
       <c r="CD2" s="83" t="n"/>
-      <c r="CI2" s="83" t="n"/>
-      <c r="CL2" s="83" t="n"/>
-      <c r="CO2" s="83" t="n"/>
+      <c r="CE2" s="83" t="n"/>
+      <c r="CJ2" s="83" t="n"/>
+      <c r="CM2" s="83" t="n"/>
       <c r="CP2" s="83" t="n"/>
       <c r="CQ2" s="83" t="n"/>
       <c r="CR2" s="83" t="n"/>
@@ -4936,7 +5677,7 @@
       <c r="CV2" s="83" t="n"/>
       <c r="CW2" s="83" t="n"/>
       <c r="CX2" s="83" t="n"/>
-      <c r="CZ2" s="83" t="n"/>
+      <c r="CY2" s="83" t="n"/>
       <c r="DA2" s="83" t="n"/>
       <c r="DB2" s="83" t="n"/>
       <c r="DC2" s="83" t="n"/>
@@ -4948,7 +5689,7 @@
       <c r="DI2" s="83" t="n"/>
       <c r="DJ2" s="83" t="n"/>
       <c r="DK2" s="83" t="n"/>
-      <c r="DN2" s="83" t="n"/>
+      <c r="DL2" s="83" t="n"/>
       <c r="DO2" s="83" t="n"/>
       <c r="DP2" s="83" t="n"/>
       <c r="DQ2" s="83" t="n"/>
@@ -4959,8 +5700,8 @@
       <c r="DV2" s="83" t="n"/>
       <c r="DW2" s="83" t="n"/>
       <c r="DX2" s="83" t="n"/>
-      <c r="EB2" s="83" t="n"/>
-      <c r="ED2" s="83" t="n"/>
+      <c r="DY2" s="83" t="n"/>
+      <c r="EC2" s="83" t="n"/>
       <c r="EE2" s="83" t="n"/>
       <c r="EF2" s="83" t="n"/>
       <c r="EG2" s="83" t="n"/>
@@ -4972,6 +5713,245 @@
       <c r="EM2" s="83" t="n"/>
       <c r="EN2" s="83" t="n"/>
       <c r="EO2" s="83" t="n"/>
+      <c r="EP2" s="83" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_03</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>COM_RES_PAY_03_V2</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>3000671</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>60000787</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>Issuance Fee (BG/LC)</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-15</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-15</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="R3" s="1" t="inlineStr">
+        <is>
+          <t>60000787</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>Financial Letter of Credit</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>2020-10-15</t>
+        </is>
+      </c>
+      <c r="V3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="W3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="X3" s="1" t="inlineStr">
+        <is>
+          <t>2021-10-15</t>
+        </is>
+      </c>
+      <c r="Y3" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="Z3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="AA3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="AB3" s="1" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="AK3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC3_14092020211728</t>
+        </is>
+      </c>
+      <c r="AL3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEEFACBG_14092020212610</t>
+        </is>
+      </c>
+      <c r="AM3" s="1" t="inlineStr">
+        <is>
+          <t>SBLC/Guarantee</t>
+        </is>
+      </c>
+      <c r="AN3" s="1" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="AO3" s="1" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="AP3" s="30" t="inlineStr">
+        <is>
+          <t>17-Sep-2018</t>
+        </is>
+      </c>
+      <c r="AQ3" s="82" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="AR3" s="82" t="inlineStr">
+        <is>
+          <t>SBLC/Guarantee</t>
+        </is>
+      </c>
+      <c r="AS3" s="82" t="inlineStr">
+        <is>
+          <t>Deal/Facility</t>
+        </is>
+      </c>
+      <c r="AT3" s="83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AU3" s="30" t="inlineStr">
+        <is>
+          <t>Create Cashflows</t>
+        </is>
+      </c>
+      <c r="AV3" s="30" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AW3" s="30" t="inlineStr">
+        <is>
+          <t>Borrower</t>
+        </is>
+      </c>
+      <c r="AX3" s="1" t="inlineStr">
+        <is>
+          <t>RTGS1</t>
+        </is>
+      </c>
+      <c r="AY3" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="AZ3" s="30" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="BA3" s="30" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BB3" s="30" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="BC3" s="30" t="inlineStr">
+        <is>
+          <t>BLOGGS</t>
+        </is>
+      </c>
+      <c r="BD3" s="30" t="inlineStr">
+        <is>
+          <t>Melbourne, VIC,Australia</t>
+        </is>
+      </c>
+      <c r="BE3" s="30" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="BF3" s="30" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_AKD</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -17589,8 +18569,8 @@
   </sheetPr>
   <dimension ref="A1:CE3"/>
   <sheetViews>
-    <sheetView topLeftCell="BC1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BH2" sqref="BH2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
GDE-7335 script for CommSee fees endpoing of SBLC
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -4536,22 +4536,22 @@
       </c>
       <c r="N2" s="1" t="inlineStr">
         <is>
-          <t>2020-10-16</t>
+          <t>2020-11-13</t>
         </is>
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>2020-10-22</t>
+          <t>2020-11-19</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t>2020-10-16</t>
+          <t>2020-11-13</t>
         </is>
       </c>
       <c r="Q2" s="1" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>3.41</t>
         </is>
       </c>
       <c r="S2" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-7338 Script for V2 endpoint of outstanding for SBLC Issuance
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="13" activeTab="13" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="13" activeTab="16" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -2417,8 +2417,8 @@
   </sheetPr>
   <dimension ref="A1:BQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AP1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4161,11 +4161,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ5"/>
+  <dimension ref="A1:BA5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4181,39 +4181,39 @@
     <col width="28.7109375" customWidth="1" style="30" min="13" max="13"/>
     <col width="27.85546875" customWidth="1" style="30" min="14" max="14"/>
     <col width="36.140625" customWidth="1" style="30" min="15" max="15"/>
-    <col width="31.42578125" customWidth="1" style="30" min="16" max="18"/>
-    <col width="21.42578125" customWidth="1" style="30" min="19" max="20"/>
-    <col width="25.140625" customWidth="1" style="30" min="21" max="21"/>
-    <col width="26" customWidth="1" style="30" min="22" max="22"/>
-    <col width="33.140625" customWidth="1" style="30" min="23" max="23"/>
-    <col width="30.7109375" customWidth="1" style="30" min="24" max="24"/>
-    <col width="36.28515625" bestFit="1" customWidth="1" style="30" min="25" max="25"/>
-    <col width="28" customWidth="1" style="30" min="26" max="26"/>
-    <col width="34" customWidth="1" style="30" min="27" max="27"/>
-    <col width="33.28515625" customWidth="1" style="30" min="28" max="28"/>
-    <col width="31.85546875" customWidth="1" style="30" min="29" max="29"/>
-    <col width="26.28515625" customWidth="1" style="30" min="30" max="30"/>
-    <col width="26.42578125" customWidth="1" style="30" min="31" max="31"/>
-    <col width="30.42578125" customWidth="1" style="30" min="32" max="32"/>
-    <col width="25.85546875" customWidth="1" style="30" min="33" max="33"/>
-    <col width="19.42578125" customWidth="1" style="30" min="34" max="34"/>
-    <col width="21.5703125" customWidth="1" style="30" min="35" max="35"/>
-    <col width="27.5703125" customWidth="1" style="30" min="36" max="36"/>
-    <col width="11.42578125" customWidth="1" style="30" min="37" max="37"/>
-    <col width="36" customWidth="1" style="30" min="38" max="38"/>
-    <col width="20.85546875" customWidth="1" style="30" min="39" max="39"/>
-    <col width="18.85546875" customWidth="1" style="30" min="40" max="40"/>
-    <col width="23.42578125" customWidth="1" style="30" min="41" max="41"/>
-    <col width="22.42578125" customWidth="1" style="30" min="42" max="42"/>
-    <col width="16.7109375" customWidth="1" style="30" min="43" max="43"/>
-    <col width="17" customWidth="1" style="30" min="44" max="44"/>
-    <col width="18.85546875" customWidth="1" style="30" min="45" max="45"/>
-    <col width="17.5703125" customWidth="1" style="30" min="46" max="46"/>
-    <col width="17.28515625" customWidth="1" style="30" min="47" max="47"/>
-    <col width="23.42578125" customWidth="1" style="30" min="48" max="48"/>
-    <col width="36.7109375" customWidth="1" style="30" min="49" max="49"/>
-    <col width="35.85546875" customWidth="1" style="30" min="50" max="50"/>
-    <col width="26.5703125" customWidth="1" style="30" min="51" max="52"/>
+    <col width="31.42578125" customWidth="1" style="30" min="16" max="19"/>
+    <col width="21.42578125" customWidth="1" style="30" min="20" max="21"/>
+    <col width="25.140625" customWidth="1" style="30" min="22" max="22"/>
+    <col width="26" customWidth="1" style="30" min="23" max="23"/>
+    <col width="33.140625" customWidth="1" style="30" min="24" max="24"/>
+    <col width="30.7109375" customWidth="1" style="30" min="25" max="25"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="30" min="26" max="26"/>
+    <col width="28" customWidth="1" style="30" min="27" max="27"/>
+    <col width="34" customWidth="1" style="30" min="28" max="28"/>
+    <col width="33.28515625" customWidth="1" style="30" min="29" max="29"/>
+    <col width="31.85546875" customWidth="1" style="30" min="30" max="30"/>
+    <col width="26.28515625" customWidth="1" style="30" min="31" max="31"/>
+    <col width="26.42578125" customWidth="1" style="30" min="32" max="32"/>
+    <col width="30.42578125" customWidth="1" style="30" min="33" max="33"/>
+    <col width="25.85546875" customWidth="1" style="30" min="34" max="34"/>
+    <col width="19.42578125" customWidth="1" style="30" min="35" max="35"/>
+    <col width="21.5703125" customWidth="1" style="30" min="36" max="36"/>
+    <col width="27.5703125" customWidth="1" style="30" min="37" max="37"/>
+    <col width="11.42578125" customWidth="1" style="30" min="38" max="38"/>
+    <col width="36" customWidth="1" style="30" min="39" max="39"/>
+    <col width="20.85546875" customWidth="1" style="30" min="40" max="40"/>
+    <col width="18.85546875" customWidth="1" style="30" min="41" max="41"/>
+    <col width="23.42578125" customWidth="1" style="30" min="42" max="42"/>
+    <col width="22.42578125" customWidth="1" style="30" min="43" max="43"/>
+    <col width="16.7109375" customWidth="1" style="30" min="44" max="44"/>
+    <col width="17" customWidth="1" style="30" min="45" max="45"/>
+    <col width="18.85546875" customWidth="1" style="30" min="46" max="46"/>
+    <col width="17.5703125" customWidth="1" style="30" min="47" max="47"/>
+    <col width="17.28515625" customWidth="1" style="30" min="48" max="48"/>
+    <col width="23.42578125" customWidth="1" style="30" min="49" max="49"/>
+    <col width="36.7109375" customWidth="1" style="30" min="50" max="50"/>
+    <col width="35.85546875" customWidth="1" style="30" min="51" max="51"/>
+    <col width="26.5703125" customWidth="1" style="30" min="52" max="53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="150">
@@ -4304,175 +4304,180 @@
       </c>
       <c r="R1" s="56" t="inlineStr">
         <is>
+          <t>Fee_PaidToDate</t>
+        </is>
+      </c>
+      <c r="S1" s="56" t="inlineStr">
+        <is>
           <t>Outstanding_Alias</t>
         </is>
       </c>
-      <c r="S1" s="56" t="inlineStr">
+      <c r="T1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RiskType</t>
         </is>
       </c>
-      <c r="T1" s="56" t="inlineStr">
+      <c r="U1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="U1" s="56" t="inlineStr">
+      <c r="V1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_EffectiveDate</t>
         </is>
       </c>
-      <c r="V1" s="56" t="inlineStr">
+      <c r="W1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetAmount</t>
         </is>
       </c>
-      <c r="W1" s="56" t="inlineStr">
+      <c r="X1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetFacCCYAmount</t>
         </is>
       </c>
-      <c r="X1" s="56" t="inlineStr">
+      <c r="Y1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_MaturityExpiryDate</t>
         </is>
       </c>
-      <c r="Y1" s="77" t="inlineStr">
+      <c r="Z1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Favouree</t>
         </is>
       </c>
-      <c r="Z1" s="56" t="inlineStr">
+      <c r="AA1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBGrossAmount</t>
         </is>
       </c>
-      <c r="AA1" s="56" t="inlineStr">
+      <c r="AB1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalOriginalAmount</t>
         </is>
       </c>
-      <c r="AB1" s="56" t="inlineStr">
+      <c r="AC1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalCurrentAmount</t>
         </is>
       </c>
-      <c r="AC1" s="56" t="inlineStr">
+      <c r="AD1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingFrequency</t>
         </is>
       </c>
-      <c r="AD1" s="56" t="inlineStr">
+      <c r="AE1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingDate</t>
         </is>
       </c>
-      <c r="AE1" s="56" t="inlineStr">
+      <c r="AF1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PaymentMode</t>
         </is>
       </c>
-      <c r="AF1" s="56" t="inlineStr">
+      <c r="AG1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="AG1" s="56" t="inlineStr">
+      <c r="AH1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PricingOption</t>
         </is>
       </c>
-      <c r="AH1" s="56" t="inlineStr">
+      <c r="AI1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Margin</t>
         </is>
       </c>
-      <c r="AI1" s="56" t="inlineStr">
+      <c r="AJ1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AllInRate</t>
         </is>
       </c>
-      <c r="AJ1" s="56" t="inlineStr">
+      <c r="AK1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AccruedInterest</t>
         </is>
       </c>
-      <c r="AK1" s="78" t="inlineStr">
+      <c r="AL1" s="78" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="AL1" s="77" t="inlineStr">
+      <c r="AM1" s="77" t="inlineStr">
         <is>
           <t>OutstandingSelect_Type</t>
         </is>
       </c>
-      <c r="AM1" s="78" t="inlineStr">
+      <c r="AN1" s="78" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="AN1" s="77" t="inlineStr">
+      <c r="AO1" s="77" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
       </c>
-      <c r="AO1" s="77" t="inlineStr">
+      <c r="AP1" s="77" t="inlineStr">
         <is>
           <t>Amount_Requested</t>
         </is>
       </c>
-      <c r="AP1" s="77" t="inlineStr">
+      <c r="AQ1" s="77" t="inlineStr">
         <is>
           <t>Issuance_Fee</t>
         </is>
       </c>
-      <c r="AQ1" s="77" t="inlineStr">
+      <c r="AR1" s="77" t="inlineStr">
         <is>
           <t>SBLC_Status</t>
         </is>
       </c>
-      <c r="AR1" s="77" t="inlineStr">
+      <c r="AS1" s="77" t="inlineStr">
         <is>
           <t>Cycle_Frequency</t>
         </is>
       </c>
-      <c r="AS1" s="77" t="inlineStr">
+      <c r="AT1" s="77" t="inlineStr">
         <is>
           <t>SBLC_ExpiryDate</t>
         </is>
       </c>
-      <c r="AT1" s="77" t="inlineStr">
+      <c r="AU1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Alias</t>
         </is>
       </c>
-      <c r="AU1" s="77" t="inlineStr">
+      <c r="AV1" s="77" t="inlineStr">
         <is>
           <t>Cycle_Number</t>
         </is>
       </c>
-      <c r="AV1" s="77" t="inlineStr">
+      <c r="AW1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Type</t>
         </is>
       </c>
-      <c r="AW1" s="77" t="inlineStr">
+      <c r="AX1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Type</t>
         </is>
       </c>
-      <c r="AX1" s="77" t="inlineStr">
+      <c r="AY1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Status_Awaiting_Approval</t>
         </is>
       </c>
-      <c r="AY1" s="77" t="inlineStr">
+      <c r="AZ1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Status_Awaiting_Release</t>
         </is>
       </c>
-      <c r="AZ1" s="150" t="inlineStr">
+      <c r="BA1" s="150" t="inlineStr">
         <is>
           <t>AccrualRule_PayInAdvance</t>
         </is>
@@ -4551,135 +4556,140 @@
       </c>
       <c r="Q2" s="1" t="inlineStr">
         <is>
-          <t>3.41</t>
-        </is>
-      </c>
-      <c r="S2" s="1" t="inlineStr">
+          <t>3.52</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>Financial Letter of Credit</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>2020-10-16</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="inlineStr">
         <is>
           <t>2021-10-18</t>
         </is>
       </c>
-      <c r="Y2" s="38" t="inlineStr">
+      <c r="Z2" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="Z2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AA2" s="1" t="inlineStr">
+      <c r="AB2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AB2" s="1" t="inlineStr">
+      <c r="AC2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AC2" s="79" t="n"/>
       <c r="AD2" s="79" t="n"/>
-      <c r="AK2" s="1" t="inlineStr">
+      <c r="AE2" s="79" t="n"/>
+      <c r="AL2" s="1" t="inlineStr">
         <is>
           <t>COMSEE_SC3_14092020203358</t>
         </is>
       </c>
-      <c r="AL2" s="40" t="inlineStr">
+      <c r="AM2" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AM2" s="1" t="inlineStr">
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>COMSEEFACBG_14092020204147</t>
         </is>
       </c>
-      <c r="AN2" s="40" t="inlineStr">
+      <c r="AO2" s="40" t="inlineStr">
         <is>
           <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
         </is>
       </c>
-      <c r="AO2" s="40" t="n">
+      <c r="AP2" s="40" t="n">
         <v>1000</v>
       </c>
-      <c r="AP2" s="40" t="inlineStr">
+      <c r="AQ2" s="40" t="inlineStr">
         <is>
           <t>Outstandings  X Rate (4%)</t>
         </is>
       </c>
-      <c r="AQ2" s="40" t="inlineStr">
+      <c r="AR2" s="40" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
       </c>
-      <c r="AR2" s="40" t="inlineStr">
+      <c r="AS2" s="40" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="AS2" s="1" t="inlineStr">
+      <c r="AT2" s="1" t="inlineStr">
         <is>
           <t>16-Oct-2021</t>
         </is>
       </c>
-      <c r="AT2" s="30" t="inlineStr">
+      <c r="AU2" s="30" t="inlineStr">
         <is>
           <t>ESPS11112500003</t>
         </is>
       </c>
-      <c r="AU2" s="30" t="inlineStr">
+      <c r="AV2" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AV2" s="40" t="inlineStr">
+      <c r="AW2" s="40" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AW2" s="40" t="inlineStr">
+      <c r="AX2" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee Issuance</t>
         </is>
       </c>
-      <c r="AX2" s="40" t="inlineStr">
+      <c r="AY2" s="40" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AY2" s="40" t="inlineStr">
+      <c r="AZ2" s="40" t="inlineStr">
         <is>
           <t>Awaiting Release</t>
         </is>
       </c>
-      <c r="AZ2" s="40" t="inlineStr">
+      <c r="BA2" s="40" t="inlineStr">
         <is>
           <t>Pay In Advance</t>
         </is>
@@ -4743,150 +4753,155 @@
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
+          <t>2020-11-13</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>2020-11-19</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>2020-11-13</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="inlineStr">
+        <is>
+          <t>3.52</t>
+        </is>
+      </c>
+      <c r="R3" s="1" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>Financial Letter of Credit</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="V3" s="1" t="inlineStr">
+        <is>
           <t>2020-10-16</t>
         </is>
       </c>
-      <c r="O3" s="1" t="inlineStr">
-        <is>
-          <t>2020-10-22</t>
-        </is>
-      </c>
-      <c r="P3" s="1" t="inlineStr">
-        <is>
-          <t>2020-10-16</t>
-        </is>
-      </c>
-      <c r="Q3" s="1" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S3" s="1" t="inlineStr">
-        <is>
-          <t>Financial Letter of Credit</t>
-        </is>
-      </c>
-      <c r="T3" s="1" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
-      <c r="U3" s="1" t="inlineStr">
-        <is>
-          <t>2020-10-16</t>
-        </is>
-      </c>
-      <c r="V3" s="1" t="inlineStr">
+      <c r="W3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="W3" s="1" t="inlineStr">
+      <c r="X3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="X3" s="1" t="inlineStr">
+      <c r="Y3" s="1" t="inlineStr">
         <is>
           <t>2021-10-18</t>
         </is>
       </c>
-      <c r="Y3" s="38" t="inlineStr">
+      <c r="Z3" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="Z3" s="1" t="inlineStr">
+      <c r="AA3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AA3" s="1" t="inlineStr">
+      <c r="AB3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AB3" s="1" t="inlineStr">
+      <c r="AC3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AC3" s="79" t="n"/>
       <c r="AD3" s="79" t="n"/>
-      <c r="AK3" s="1" t="inlineStr">
+      <c r="AE3" s="79" t="n"/>
+      <c r="AL3" s="1" t="inlineStr">
         <is>
           <t>COMSEE_SC3_14092020211728</t>
         </is>
       </c>
-      <c r="AL3" s="40" t="inlineStr">
+      <c r="AM3" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AM3" s="1" t="inlineStr">
+      <c r="AN3" s="1" t="inlineStr">
         <is>
           <t>COMSEEFACBG_14092020212610</t>
         </is>
       </c>
-      <c r="AN3" s="40" t="inlineStr">
+      <c r="AO3" s="40" t="inlineStr">
         <is>
           <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
         </is>
       </c>
-      <c r="AO3" s="40" t="n">
+      <c r="AP3" s="40" t="n">
         <v>1000</v>
       </c>
-      <c r="AP3" s="40" t="inlineStr">
+      <c r="AQ3" s="40" t="inlineStr">
         <is>
           <t>Outstandings  X Rate (4%)</t>
         </is>
       </c>
-      <c r="AQ3" s="40" t="inlineStr">
+      <c r="AR3" s="40" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
       </c>
-      <c r="AR3" s="40" t="inlineStr">
+      <c r="AS3" s="40" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="AS3" s="1" t="inlineStr">
+      <c r="AT3" s="1" t="inlineStr">
         <is>
           <t>16-Oct-2021</t>
         </is>
       </c>
-      <c r="AT3" s="30" t="inlineStr">
+      <c r="AU3" s="30" t="inlineStr">
         <is>
           <t>ESPS11112500003</t>
         </is>
       </c>
-      <c r="AU3" s="30" t="inlineStr">
+      <c r="AV3" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AV3" s="40" t="inlineStr">
+      <c r="AW3" s="40" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AW3" s="40" t="inlineStr">
+      <c r="AX3" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee Issuance</t>
         </is>
       </c>
-      <c r="AX3" s="40" t="inlineStr">
+      <c r="AY3" s="40" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AY3" s="40" t="inlineStr">
+      <c r="AZ3" s="40" t="inlineStr">
         <is>
           <t>Awaiting Release</t>
         </is>
       </c>
-      <c r="AZ3" s="40" t="inlineStr">
+      <c r="BA3" s="40" t="inlineStr">
         <is>
           <t>Pay In Advance</t>
         </is>
@@ -4894,7 +4909,7 @@
     </row>
     <row r="4"/>
     <row r="5">
-      <c r="AR5" s="49" t="n"/>
+      <c r="AS5" s="49" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
GDE-7336 Script for CommSee handling ongoing fees for V2 Endpoint
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="29" activeTab="33" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="16" activeTab="17" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -3546,7 +3546,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3880,7 +3880,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4161,11 +4161,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA5"/>
+  <dimension ref="A1:BC5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q1" sqref="Q1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4181,39 +4181,39 @@
     <col width="28.7109375" customWidth="1" style="30" min="13" max="13"/>
     <col width="27.85546875" customWidth="1" style="30" min="14" max="14"/>
     <col width="36.140625" customWidth="1" style="30" min="15" max="15"/>
-    <col width="31.42578125" customWidth="1" style="30" min="16" max="19"/>
-    <col width="21.42578125" customWidth="1" style="30" min="20" max="21"/>
-    <col width="25.140625" customWidth="1" style="30" min="22" max="22"/>
-    <col width="26" customWidth="1" style="30" min="23" max="23"/>
-    <col width="33.140625" customWidth="1" style="30" min="24" max="24"/>
-    <col width="30.7109375" customWidth="1" style="30" min="25" max="25"/>
-    <col width="36.28515625" bestFit="1" customWidth="1" style="30" min="26" max="26"/>
-    <col width="28" customWidth="1" style="30" min="27" max="27"/>
-    <col width="34" customWidth="1" style="30" min="28" max="28"/>
-    <col width="33.28515625" customWidth="1" style="30" min="29" max="29"/>
-    <col width="31.85546875" customWidth="1" style="30" min="30" max="30"/>
-    <col width="26.28515625" customWidth="1" style="30" min="31" max="31"/>
-    <col width="26.42578125" customWidth="1" style="30" min="32" max="32"/>
-    <col width="30.42578125" customWidth="1" style="30" min="33" max="33"/>
-    <col width="25.85546875" customWidth="1" style="30" min="34" max="34"/>
-    <col width="19.42578125" customWidth="1" style="30" min="35" max="35"/>
-    <col width="21.5703125" customWidth="1" style="30" min="36" max="36"/>
-    <col width="27.5703125" customWidth="1" style="30" min="37" max="37"/>
-    <col width="11.42578125" customWidth="1" style="30" min="38" max="38"/>
-    <col width="36" customWidth="1" style="30" min="39" max="39"/>
-    <col width="20.85546875" customWidth="1" style="30" min="40" max="40"/>
-    <col width="18.85546875" customWidth="1" style="30" min="41" max="41"/>
-    <col width="23.42578125" customWidth="1" style="30" min="42" max="42"/>
-    <col width="22.42578125" customWidth="1" style="30" min="43" max="43"/>
-    <col width="16.7109375" customWidth="1" style="30" min="44" max="44"/>
-    <col width="17" customWidth="1" style="30" min="45" max="45"/>
-    <col width="18.85546875" customWidth="1" style="30" min="46" max="46"/>
-    <col width="17.5703125" customWidth="1" style="30" min="47" max="47"/>
-    <col width="17.28515625" customWidth="1" style="30" min="48" max="48"/>
-    <col width="23.42578125" customWidth="1" style="30" min="49" max="49"/>
-    <col width="36.7109375" customWidth="1" style="30" min="50" max="50"/>
-    <col width="35.85546875" customWidth="1" style="30" min="51" max="51"/>
-    <col width="26.5703125" customWidth="1" style="30" min="52" max="53"/>
+    <col width="31.42578125" customWidth="1" style="30" min="16" max="21"/>
+    <col width="21.42578125" customWidth="1" style="30" min="22" max="23"/>
+    <col width="25.140625" customWidth="1" style="30" min="24" max="24"/>
+    <col width="26" customWidth="1" style="30" min="25" max="25"/>
+    <col width="33.140625" customWidth="1" style="30" min="26" max="26"/>
+    <col width="30.7109375" customWidth="1" style="30" min="27" max="27"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="30" min="28" max="28"/>
+    <col width="28" customWidth="1" style="30" min="29" max="29"/>
+    <col width="34" customWidth="1" style="30" min="30" max="30"/>
+    <col width="33.28515625" customWidth="1" style="30" min="31" max="31"/>
+    <col width="31.85546875" customWidth="1" style="30" min="32" max="32"/>
+    <col width="26.28515625" customWidth="1" style="30" min="33" max="33"/>
+    <col width="26.42578125" customWidth="1" style="30" min="34" max="34"/>
+    <col width="30.42578125" customWidth="1" style="30" min="35" max="35"/>
+    <col width="25.85546875" customWidth="1" style="30" min="36" max="36"/>
+    <col width="19.42578125" customWidth="1" style="30" min="37" max="37"/>
+    <col width="21.5703125" customWidth="1" style="30" min="38" max="38"/>
+    <col width="27.5703125" customWidth="1" style="30" min="39" max="39"/>
+    <col width="11.42578125" customWidth="1" style="30" min="40" max="40"/>
+    <col width="36" customWidth="1" style="30" min="41" max="41"/>
+    <col width="20.85546875" customWidth="1" style="30" min="42" max="42"/>
+    <col width="18.85546875" customWidth="1" style="30" min="43" max="43"/>
+    <col width="23.42578125" customWidth="1" style="30" min="44" max="44"/>
+    <col width="22.42578125" customWidth="1" style="30" min="45" max="45"/>
+    <col width="16.7109375" customWidth="1" style="30" min="46" max="46"/>
+    <col width="17" customWidth="1" style="30" min="47" max="47"/>
+    <col width="18.85546875" customWidth="1" style="30" min="48" max="48"/>
+    <col width="17.5703125" customWidth="1" style="30" min="49" max="49"/>
+    <col width="17.28515625" customWidth="1" style="30" min="50" max="50"/>
+    <col width="23.42578125" customWidth="1" style="30" min="51" max="51"/>
+    <col width="36.7109375" customWidth="1" style="30" min="52" max="52"/>
+    <col width="35.85546875" customWidth="1" style="30" min="53" max="53"/>
+    <col width="26.5703125" customWidth="1" style="30" min="54" max="55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="150">
@@ -4299,185 +4299,195 @@
       </c>
       <c r="Q1" s="56" t="inlineStr">
         <is>
+          <t>Fee_CycleStartDate</t>
+        </is>
+      </c>
+      <c r="R1" s="56" t="inlineStr">
+        <is>
+          <t>Fee_AccrualEndDate</t>
+        </is>
+      </c>
+      <c r="S1" s="56" t="inlineStr">
+        <is>
           <t>Fee_AccruedToDate</t>
         </is>
       </c>
-      <c r="R1" s="56" t="inlineStr">
+      <c r="T1" s="56" t="inlineStr">
         <is>
           <t>Fee_PaidToDate</t>
         </is>
       </c>
-      <c r="S1" s="56" t="inlineStr">
+      <c r="U1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Alias</t>
         </is>
       </c>
-      <c r="T1" s="56" t="inlineStr">
+      <c r="V1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RiskType</t>
         </is>
       </c>
-      <c r="U1" s="56" t="inlineStr">
+      <c r="W1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="V1" s="56" t="inlineStr">
+      <c r="X1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_EffectiveDate</t>
         </is>
       </c>
-      <c r="W1" s="56" t="inlineStr">
+      <c r="Y1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetAmount</t>
         </is>
       </c>
-      <c r="X1" s="56" t="inlineStr">
+      <c r="Z1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetFacCCYAmount</t>
         </is>
       </c>
-      <c r="Y1" s="56" t="inlineStr">
+      <c r="AA1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_MaturityExpiryDate</t>
         </is>
       </c>
-      <c r="Z1" s="77" t="inlineStr">
+      <c r="AB1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Favouree</t>
         </is>
       </c>
-      <c r="AA1" s="56" t="inlineStr">
+      <c r="AC1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBGrossAmount</t>
         </is>
       </c>
-      <c r="AB1" s="56" t="inlineStr">
+      <c r="AD1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalOriginalAmount</t>
         </is>
       </c>
-      <c r="AC1" s="56" t="inlineStr">
+      <c r="AE1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalCurrentAmount</t>
         </is>
       </c>
-      <c r="AD1" s="56" t="inlineStr">
+      <c r="AF1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingFrequency</t>
         </is>
       </c>
-      <c r="AE1" s="56" t="inlineStr">
+      <c r="AG1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingDate</t>
         </is>
       </c>
-      <c r="AF1" s="56" t="inlineStr">
+      <c r="AH1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PaymentMode</t>
         </is>
       </c>
-      <c r="AG1" s="56" t="inlineStr">
+      <c r="AI1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="AH1" s="56" t="inlineStr">
+      <c r="AJ1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PricingOption</t>
         </is>
       </c>
-      <c r="AI1" s="56" t="inlineStr">
+      <c r="AK1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Margin</t>
         </is>
       </c>
-      <c r="AJ1" s="56" t="inlineStr">
+      <c r="AL1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AllInRate</t>
         </is>
       </c>
-      <c r="AK1" s="56" t="inlineStr">
+      <c r="AM1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AccruedInterest</t>
         </is>
       </c>
-      <c r="AL1" s="78" t="inlineStr">
+      <c r="AN1" s="78" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="AM1" s="77" t="inlineStr">
+      <c r="AO1" s="77" t="inlineStr">
         <is>
           <t>OutstandingSelect_Type</t>
         </is>
       </c>
-      <c r="AN1" s="78" t="inlineStr">
+      <c r="AP1" s="78" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="AO1" s="77" t="inlineStr">
+      <c r="AQ1" s="77" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
       </c>
-      <c r="AP1" s="77" t="inlineStr">
+      <c r="AR1" s="77" t="inlineStr">
         <is>
           <t>Amount_Requested</t>
         </is>
       </c>
-      <c r="AQ1" s="77" t="inlineStr">
+      <c r="AS1" s="77" t="inlineStr">
         <is>
           <t>Issuance_Fee</t>
         </is>
       </c>
-      <c r="AR1" s="77" t="inlineStr">
+      <c r="AT1" s="77" t="inlineStr">
         <is>
           <t>SBLC_Status</t>
         </is>
       </c>
-      <c r="AS1" s="77" t="inlineStr">
+      <c r="AU1" s="77" t="inlineStr">
         <is>
           <t>Cycle_Frequency</t>
         </is>
       </c>
-      <c r="AT1" s="77" t="inlineStr">
+      <c r="AV1" s="77" t="inlineStr">
         <is>
           <t>SBLC_ExpiryDate</t>
         </is>
       </c>
-      <c r="AU1" s="77" t="inlineStr">
+      <c r="AW1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Alias</t>
         </is>
       </c>
-      <c r="AV1" s="77" t="inlineStr">
+      <c r="AX1" s="77" t="inlineStr">
         <is>
           <t>Cycle_Number</t>
         </is>
       </c>
-      <c r="AW1" s="77" t="inlineStr">
+      <c r="AY1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Type</t>
         </is>
       </c>
-      <c r="AX1" s="77" t="inlineStr">
+      <c r="AZ1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Type</t>
         </is>
       </c>
-      <c r="AY1" s="77" t="inlineStr">
+      <c r="BA1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Status_Awaiting_Approval</t>
         </is>
       </c>
-      <c r="AZ1" s="77" t="inlineStr">
+      <c r="BB1" s="77" t="inlineStr">
         <is>
           <t>Transaction_Status_Awaiting_Release</t>
         </is>
       </c>
-      <c r="BA1" s="150" t="inlineStr">
+      <c r="BC1" s="150" t="inlineStr">
         <is>
           <t>AccrualRule_PayInAdvance</t>
         </is>
@@ -4554,142 +4564,144 @@
           <t>2020-11-13</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="n"/>
+      <c r="R2" s="1" t="n"/>
+      <c r="S2" s="1" t="inlineStr">
         <is>
           <t>3.52</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>Financial Letter of Credit</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>2020-10-16</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>2021-10-18</t>
         </is>
       </c>
-      <c r="Z2" s="38" t="inlineStr">
+      <c r="AB2" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="AA2" s="1" t="inlineStr">
+      <c r="AC2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AB2" s="1" t="inlineStr">
+      <c r="AD2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
+      <c r="AE2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AD2" s="79" t="n"/>
-      <c r="AE2" s="79" t="n"/>
-      <c r="AL2" s="1" t="inlineStr">
+      <c r="AF2" s="79" t="n"/>
+      <c r="AG2" s="79" t="n"/>
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>COMSEE_SC3_14092020203358</t>
         </is>
       </c>
-      <c r="AM2" s="40" t="inlineStr">
+      <c r="AO2" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AN2" s="1" t="inlineStr">
+      <c r="AP2" s="1" t="inlineStr">
         <is>
           <t>COMSEEFACBG_14092020204147</t>
         </is>
       </c>
-      <c r="AO2" s="40" t="inlineStr">
+      <c r="AQ2" s="40" t="inlineStr">
         <is>
           <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
         </is>
       </c>
-      <c r="AP2" s="40" t="n">
+      <c r="AR2" s="40" t="n">
         <v>1000</v>
       </c>
-      <c r="AQ2" s="40" t="inlineStr">
+      <c r="AS2" s="40" t="inlineStr">
         <is>
           <t>Outstandings  X Rate (4%)</t>
         </is>
       </c>
-      <c r="AR2" s="40" t="inlineStr">
+      <c r="AT2" s="40" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
       </c>
-      <c r="AS2" s="40" t="inlineStr">
+      <c r="AU2" s="40" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="AT2" s="1" t="inlineStr">
+      <c r="AV2" s="1" t="inlineStr">
         <is>
           <t>16-Oct-2021</t>
         </is>
       </c>
-      <c r="AU2" s="30" t="inlineStr">
+      <c r="AW2" s="30" t="inlineStr">
         <is>
           <t>ESPS11112500003</t>
         </is>
       </c>
-      <c r="AV2" s="30" t="inlineStr">
+      <c r="AX2" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AW2" s="40" t="inlineStr">
+      <c r="AY2" s="40" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AX2" s="40" t="inlineStr">
+      <c r="AZ2" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee Issuance</t>
         </is>
       </c>
-      <c r="AY2" s="40" t="inlineStr">
+      <c r="BA2" s="40" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AZ2" s="40" t="inlineStr">
+      <c r="BB2" s="40" t="inlineStr">
         <is>
           <t>Awaiting Release</t>
         </is>
       </c>
-      <c r="BA2" s="40" t="inlineStr">
+      <c r="BC2" s="40" t="inlineStr">
         <is>
           <t>Pay In Advance</t>
         </is>
@@ -4753,155 +4765,157 @@
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-13</t>
+          <t>2020-11-20</t>
         </is>
       </c>
       <c r="O3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-19</t>
+          <t>2020-11-26</t>
         </is>
       </c>
       <c r="P3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-13</t>
-        </is>
-      </c>
-      <c r="Q3" s="1" t="inlineStr">
-        <is>
-          <t>3.63</t>
-        </is>
-      </c>
-      <c r="R3" s="1" t="inlineStr">
+          <t>2020-11-20</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="n"/>
+      <c r="R3" s="1" t="n"/>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>4.51</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="T3" s="1" t="inlineStr">
+      <c r="V3" s="1" t="inlineStr">
         <is>
           <t>Financial Letter of Credit</t>
         </is>
       </c>
-      <c r="U3" s="1" t="inlineStr">
+      <c r="W3" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="V3" s="1" t="inlineStr">
+      <c r="X3" s="1" t="inlineStr">
         <is>
           <t>2020-10-16</t>
         </is>
       </c>
-      <c r="W3" s="1" t="inlineStr">
+      <c r="Y3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="X3" s="1" t="inlineStr">
+      <c r="Z3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="Y3" s="1" t="inlineStr">
+      <c r="AA3" s="1" t="inlineStr">
         <is>
           <t>2021-10-18</t>
         </is>
       </c>
-      <c r="Z3" s="38" t="inlineStr">
+      <c r="AB3" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="AA3" s="1" t="inlineStr">
+      <c r="AC3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AB3" s="1" t="inlineStr">
+      <c r="AD3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AC3" s="1" t="inlineStr">
+      <c r="AE3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AD3" s="79" t="n"/>
-      <c r="AE3" s="79" t="n"/>
-      <c r="AL3" s="1" t="inlineStr">
+      <c r="AF3" s="79" t="n"/>
+      <c r="AG3" s="79" t="n"/>
+      <c r="AN3" s="1" t="inlineStr">
         <is>
           <t>COMSEE_SC3_14092020211728</t>
         </is>
       </c>
-      <c r="AM3" s="40" t="inlineStr">
+      <c r="AO3" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AN3" s="1" t="inlineStr">
+      <c r="AP3" s="1" t="inlineStr">
         <is>
           <t>COMSEEFACBG_14092020212610</t>
         </is>
       </c>
-      <c r="AO3" s="40" t="inlineStr">
+      <c r="AQ3" s="40" t="inlineStr">
         <is>
           <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
         </is>
       </c>
-      <c r="AP3" s="40" t="n">
+      <c r="AR3" s="40" t="n">
         <v>1000</v>
       </c>
-      <c r="AQ3" s="40" t="inlineStr">
+      <c r="AS3" s="40" t="inlineStr">
         <is>
           <t>Outstandings  X Rate (4%)</t>
         </is>
       </c>
-      <c r="AR3" s="40" t="inlineStr">
+      <c r="AT3" s="40" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
       </c>
-      <c r="AS3" s="40" t="inlineStr">
+      <c r="AU3" s="40" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="AT3" s="1" t="inlineStr">
+      <c r="AV3" s="1" t="inlineStr">
         <is>
           <t>16-Oct-2021</t>
         </is>
       </c>
-      <c r="AU3" s="30" t="inlineStr">
+      <c r="AW3" s="30" t="inlineStr">
         <is>
           <t>ESPS11112500003</t>
         </is>
       </c>
-      <c r="AV3" s="30" t="inlineStr">
+      <c r="AX3" s="30" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AW3" s="40" t="inlineStr">
+      <c r="AY3" s="40" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AX3" s="40" t="inlineStr">
+      <c r="AZ3" s="40" t="inlineStr">
         <is>
           <t>SBLC/Guarantee Issuance</t>
         </is>
       </c>
-      <c r="AY3" s="40" t="inlineStr">
+      <c r="BA3" s="40" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AZ3" s="40" t="inlineStr">
+      <c r="BB3" s="40" t="inlineStr">
         <is>
           <t>Awaiting Release</t>
         </is>
       </c>
-      <c r="BA3" s="40" t="inlineStr">
+      <c r="BC3" s="40" t="inlineStr">
         <is>
           <t>Pay In Advance</t>
         </is>
@@ -4909,7 +4923,7 @@
     </row>
     <row r="4"/>
     <row r="5">
-      <c r="AS5" s="49" t="n"/>
+      <c r="AU5" s="49" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -4924,11 +4938,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EQ3"/>
+  <dimension ref="A1:ES3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q1" sqref="Q1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4945,128 +4959,128 @@
     <col width="18" customWidth="1" style="30" min="13" max="13"/>
     <col width="17.5703125" customWidth="1" style="30" min="14" max="14"/>
     <col width="15.42578125" customWidth="1" style="30" min="15" max="15"/>
-    <col width="13.28515625" customWidth="1" style="30" min="16" max="16"/>
-    <col width="19.5703125" customWidth="1" style="30" min="17" max="19"/>
-    <col width="21.42578125" customWidth="1" style="30" min="20" max="21"/>
-    <col width="25.140625" customWidth="1" style="30" min="22" max="22"/>
-    <col width="26" customWidth="1" style="30" min="23" max="23"/>
-    <col width="33.140625" customWidth="1" style="30" min="24" max="24"/>
-    <col width="30.7109375" customWidth="1" style="30" min="25" max="25"/>
-    <col width="21.85546875" customWidth="1" style="30" min="26" max="26"/>
-    <col width="28" customWidth="1" style="30" min="27" max="27"/>
-    <col width="34" customWidth="1" style="30" min="28" max="28"/>
-    <col width="33.28515625" customWidth="1" style="30" min="29" max="29"/>
-    <col width="31.85546875" customWidth="1" style="30" min="30" max="30"/>
-    <col width="26.28515625" customWidth="1" style="30" min="31" max="31"/>
-    <col width="26.42578125" customWidth="1" style="30" min="32" max="32"/>
-    <col width="30.42578125" customWidth="1" style="30" min="33" max="33"/>
-    <col width="25.85546875" customWidth="1" style="30" min="34" max="34"/>
-    <col width="19.42578125" customWidth="1" style="30" min="35" max="35"/>
-    <col width="21.5703125" customWidth="1" style="30" min="36" max="36"/>
-    <col width="27.5703125" customWidth="1" style="30" min="37" max="37"/>
-    <col width="34.7109375" customWidth="1" style="30" min="38" max="38"/>
-    <col width="33.85546875" customWidth="1" style="30" min="39" max="40"/>
-    <col width="21.42578125" customWidth="1" style="30" min="41" max="41"/>
-    <col width="29.140625" customWidth="1" style="30" min="42" max="42"/>
-    <col width="34" customWidth="1" style="30" min="43" max="43"/>
-    <col width="31.5703125" customWidth="1" style="30" min="44" max="44"/>
-    <col width="15.140625" customWidth="1" style="30" min="45" max="45"/>
-    <col width="11.28515625" customWidth="1" style="30" min="46" max="46"/>
-    <col width="18" customWidth="1" style="30" min="47" max="47"/>
-    <col width="15.5703125" customWidth="1" style="30" min="48" max="48"/>
-    <col width="15.7109375" customWidth="1" style="30" min="49" max="49"/>
-    <col width="16.5703125" customWidth="1" style="30" min="50" max="50"/>
-    <col width="41.85546875" customWidth="1" style="30" min="51" max="51"/>
-    <col width="22.140625" customWidth="1" style="30" min="52" max="52"/>
-    <col width="21.85546875" customWidth="1" style="30" min="53" max="53"/>
-    <col width="25.140625" customWidth="1" style="30" min="54" max="54"/>
-    <col width="22.42578125" customWidth="1" style="30" min="55" max="55"/>
-    <col width="27.5703125" customWidth="1" style="30" min="56" max="56"/>
-    <col width="23.42578125" customWidth="1" style="30" min="57" max="57"/>
-    <col width="29.140625" customWidth="1" style="30" min="58" max="58"/>
-    <col width="39.7109375" customWidth="1" style="30" min="59" max="59"/>
-    <col width="19" customWidth="1" style="30" min="60" max="60"/>
-    <col width="32.42578125" customWidth="1" style="30" min="61" max="61"/>
-    <col width="17.28515625" customWidth="1" style="30" min="62" max="62"/>
-    <col width="28.7109375" customWidth="1" style="30" min="63" max="63"/>
-    <col width="23.5703125" customWidth="1" style="30" min="64" max="64"/>
-    <col width="45.28515625" customWidth="1" style="30" min="65" max="65"/>
-    <col width="29.85546875" customWidth="1" style="30" min="66" max="66"/>
-    <col width="14.28515625" customWidth="1" style="30" min="67" max="67"/>
-    <col width="23" customWidth="1" style="30" min="68" max="68"/>
-    <col width="19.85546875" customWidth="1" style="30" min="69" max="72"/>
-    <col width="24.7109375" customWidth="1" style="30" min="73" max="74"/>
-    <col width="25" customWidth="1" style="30" min="75" max="75"/>
-    <col width="24.42578125" customWidth="1" style="30" min="76" max="76"/>
-    <col width="30.42578125" customWidth="1" style="30" min="77" max="77"/>
-    <col width="36" customWidth="1" style="30" min="78" max="78"/>
-    <col width="34.42578125" customWidth="1" style="30" min="79" max="79"/>
-    <col width="26.7109375" customWidth="1" style="30" min="80" max="80"/>
-    <col width="17.28515625" customWidth="1" style="30" min="81" max="82"/>
-    <col width="34.140625" customWidth="1" style="30" min="83" max="83"/>
-    <col width="28.42578125" customWidth="1" style="30" min="84" max="84"/>
-    <col width="24.7109375" customWidth="1" style="30" min="85" max="85"/>
-    <col width="30.28515625" customWidth="1" style="30" min="86" max="86"/>
-    <col width="17.5703125" customWidth="1" style="30" min="87" max="87"/>
-    <col width="20.28515625" customWidth="1" style="30" min="88" max="88"/>
-    <col width="12.140625" customWidth="1" style="30" min="89" max="89"/>
-    <col width="21.42578125" customWidth="1" style="30" min="90" max="90"/>
-    <col width="24.140625" customWidth="1" style="30" min="91" max="91"/>
-    <col width="16" customWidth="1" style="30" min="92" max="92"/>
-    <col width="14" customWidth="1" style="30" min="93" max="93"/>
-    <col width="16.7109375" customWidth="1" style="30" min="94" max="94"/>
-    <col width="10" customWidth="1" style="30" min="95" max="95"/>
-    <col width="8.5703125" customWidth="1" style="30" min="96" max="96"/>
-    <col width="19.140625" customWidth="1" style="30" min="97" max="97"/>
-    <col width="37.7109375" customWidth="1" style="30" min="98" max="98"/>
-    <col width="15.85546875" customWidth="1" style="30" min="99" max="99"/>
-    <col width="9.28515625" customWidth="1" style="30" min="100" max="100"/>
-    <col width="16.7109375" customWidth="1" style="30" min="101" max="102"/>
-    <col width="12.85546875" customWidth="1" style="30" min="103" max="103"/>
-    <col width="32.42578125" customWidth="1" style="30" min="104" max="104"/>
-    <col width="11.7109375" customWidth="1" style="30" min="105" max="105"/>
-    <col width="35" customWidth="1" style="30" min="106" max="106"/>
-    <col width="18.140625" customWidth="1" style="30" min="107" max="107"/>
-    <col width="15.7109375" customWidth="1" style="30" min="108" max="108"/>
-    <col width="24" customWidth="1" style="30" min="109" max="109"/>
-    <col width="11.5703125" customWidth="1" style="30" min="110" max="110"/>
-    <col width="8.28515625" customWidth="1" style="30" min="111" max="111"/>
-    <col width="16.5703125" customWidth="1" style="30" min="112" max="112"/>
-    <col width="32.85546875" customWidth="1" style="30" min="113" max="113"/>
-    <col width="18.7109375" customWidth="1" style="30" min="114" max="114"/>
-    <col width="18.28515625" customWidth="1" style="30" min="115" max="115"/>
-    <col width="10.42578125" customWidth="1" style="30" min="116" max="116"/>
-    <col width="9.7109375" customWidth="1" style="30" min="117" max="117"/>
-    <col width="12.7109375" customWidth="1" style="30" min="118" max="118"/>
-    <col width="11.7109375" customWidth="1" style="30" min="119" max="119"/>
-    <col width="24" customWidth="1" style="30" min="120" max="120"/>
-    <col width="43.7109375" customWidth="1" style="30" min="121" max="121"/>
-    <col width="44.85546875" customWidth="1" style="30" min="122" max="122"/>
-    <col width="30.140625" customWidth="1" style="30" min="123" max="123"/>
-    <col width="29.42578125" customWidth="1" style="30" min="124" max="124"/>
-    <col width="25.28515625" customWidth="1" style="30" min="125" max="125"/>
-    <col width="9.5703125" customWidth="1" style="30" min="126" max="126"/>
-    <col width="25.7109375" customWidth="1" style="30" min="127" max="127"/>
-    <col width="19.7109375" customWidth="1" style="30" min="128" max="128"/>
-    <col width="28.5703125" customWidth="1" style="30" min="129" max="129"/>
-    <col width="21.140625" customWidth="1" style="30" min="130" max="130"/>
-    <col width="14.5703125" customWidth="1" style="30" min="131" max="131"/>
-    <col width="20.5703125" customWidth="1" style="30" min="132" max="132"/>
-    <col width="18.28515625" customWidth="1" style="30" min="133" max="133"/>
-    <col width="18.85546875" customWidth="1" style="30" min="134" max="134"/>
-    <col width="35" customWidth="1" style="30" min="135" max="135"/>
-    <col width="20" customWidth="1" style="30" min="136" max="136"/>
-    <col width="32.42578125" customWidth="1" style="30" min="137" max="137"/>
-    <col width="21.5703125" customWidth="1" style="30" min="138" max="138"/>
-    <col width="13.5703125" customWidth="1" style="30" min="139" max="139"/>
-    <col width="26.28515625" customWidth="1" style="30" min="140" max="140"/>
-    <col width="19.140625" customWidth="1" style="30" min="141" max="141"/>
-    <col width="44" customWidth="1" style="30" min="142" max="142"/>
-    <col width="23.5703125" customWidth="1" style="30" min="143" max="143"/>
-    <col width="26.28515625" customWidth="1" style="30" min="144" max="144"/>
-    <col width="34.85546875" customWidth="1" style="30" min="145" max="145"/>
-    <col width="9.140625" customWidth="1" style="30" min="146" max="146"/>
-    <col width="15.85546875" customWidth="1" style="30" min="147" max="147"/>
+    <col width="13.28515625" customWidth="1" style="30" min="16" max="18"/>
+    <col width="19.5703125" customWidth="1" style="30" min="19" max="21"/>
+    <col width="21.42578125" customWidth="1" style="30" min="22" max="23"/>
+    <col width="25.140625" customWidth="1" style="30" min="24" max="24"/>
+    <col width="26" customWidth="1" style="30" min="25" max="25"/>
+    <col width="33.140625" customWidth="1" style="30" min="26" max="26"/>
+    <col width="30.7109375" customWidth="1" style="30" min="27" max="27"/>
+    <col width="21.85546875" customWidth="1" style="30" min="28" max="28"/>
+    <col width="28" customWidth="1" style="30" min="29" max="29"/>
+    <col width="34" customWidth="1" style="30" min="30" max="30"/>
+    <col width="33.28515625" customWidth="1" style="30" min="31" max="31"/>
+    <col width="31.85546875" customWidth="1" style="30" min="32" max="32"/>
+    <col width="26.28515625" customWidth="1" style="30" min="33" max="33"/>
+    <col width="26.42578125" customWidth="1" style="30" min="34" max="34"/>
+    <col width="30.42578125" customWidth="1" style="30" min="35" max="35"/>
+    <col width="25.85546875" customWidth="1" style="30" min="36" max="36"/>
+    <col width="19.42578125" customWidth="1" style="30" min="37" max="37"/>
+    <col width="21.5703125" customWidth="1" style="30" min="38" max="38"/>
+    <col width="27.5703125" customWidth="1" style="30" min="39" max="39"/>
+    <col width="34.7109375" customWidth="1" style="30" min="40" max="40"/>
+    <col width="33.85546875" customWidth="1" style="30" min="41" max="42"/>
+    <col width="21.42578125" customWidth="1" style="30" min="43" max="43"/>
+    <col width="29.140625" customWidth="1" style="30" min="44" max="44"/>
+    <col width="34" customWidth="1" style="30" min="45" max="45"/>
+    <col width="31.5703125" customWidth="1" style="30" min="46" max="46"/>
+    <col width="15.140625" customWidth="1" style="30" min="47" max="47"/>
+    <col width="11.28515625" customWidth="1" style="30" min="48" max="48"/>
+    <col width="18" customWidth="1" style="30" min="49" max="49"/>
+    <col width="15.5703125" customWidth="1" style="30" min="50" max="50"/>
+    <col width="15.7109375" customWidth="1" style="30" min="51" max="51"/>
+    <col width="16.5703125" customWidth="1" style="30" min="52" max="52"/>
+    <col width="41.85546875" customWidth="1" style="30" min="53" max="53"/>
+    <col width="22.140625" customWidth="1" style="30" min="54" max="54"/>
+    <col width="21.85546875" customWidth="1" style="30" min="55" max="55"/>
+    <col width="25.140625" customWidth="1" style="30" min="56" max="56"/>
+    <col width="22.42578125" customWidth="1" style="30" min="57" max="57"/>
+    <col width="27.5703125" customWidth="1" style="30" min="58" max="58"/>
+    <col width="23.42578125" customWidth="1" style="30" min="59" max="59"/>
+    <col width="29.140625" customWidth="1" style="30" min="60" max="60"/>
+    <col width="39.7109375" customWidth="1" style="30" min="61" max="61"/>
+    <col width="19" customWidth="1" style="30" min="62" max="62"/>
+    <col width="32.42578125" customWidth="1" style="30" min="63" max="63"/>
+    <col width="17.28515625" customWidth="1" style="30" min="64" max="64"/>
+    <col width="28.7109375" customWidth="1" style="30" min="65" max="65"/>
+    <col width="23.5703125" customWidth="1" style="30" min="66" max="66"/>
+    <col width="45.28515625" customWidth="1" style="30" min="67" max="67"/>
+    <col width="29.85546875" customWidth="1" style="30" min="68" max="68"/>
+    <col width="14.28515625" customWidth="1" style="30" min="69" max="69"/>
+    <col width="23" customWidth="1" style="30" min="70" max="70"/>
+    <col width="19.85546875" customWidth="1" style="30" min="71" max="74"/>
+    <col width="24.7109375" customWidth="1" style="30" min="75" max="76"/>
+    <col width="25" customWidth="1" style="30" min="77" max="77"/>
+    <col width="24.42578125" customWidth="1" style="30" min="78" max="78"/>
+    <col width="30.42578125" customWidth="1" style="30" min="79" max="79"/>
+    <col width="36" customWidth="1" style="30" min="80" max="80"/>
+    <col width="34.42578125" customWidth="1" style="30" min="81" max="81"/>
+    <col width="26.7109375" customWidth="1" style="30" min="82" max="82"/>
+    <col width="17.28515625" customWidth="1" style="30" min="83" max="84"/>
+    <col width="34.140625" customWidth="1" style="30" min="85" max="85"/>
+    <col width="28.42578125" customWidth="1" style="30" min="86" max="86"/>
+    <col width="24.7109375" customWidth="1" style="30" min="87" max="87"/>
+    <col width="30.28515625" customWidth="1" style="30" min="88" max="88"/>
+    <col width="17.5703125" customWidth="1" style="30" min="89" max="89"/>
+    <col width="20.28515625" customWidth="1" style="30" min="90" max="90"/>
+    <col width="12.140625" customWidth="1" style="30" min="91" max="91"/>
+    <col width="21.42578125" customWidth="1" style="30" min="92" max="92"/>
+    <col width="24.140625" customWidth="1" style="30" min="93" max="93"/>
+    <col width="16" customWidth="1" style="30" min="94" max="94"/>
+    <col width="14" customWidth="1" style="30" min="95" max="95"/>
+    <col width="16.7109375" customWidth="1" style="30" min="96" max="96"/>
+    <col width="10" customWidth="1" style="30" min="97" max="97"/>
+    <col width="8.5703125" customWidth="1" style="30" min="98" max="98"/>
+    <col width="19.140625" customWidth="1" style="30" min="99" max="99"/>
+    <col width="37.7109375" customWidth="1" style="30" min="100" max="100"/>
+    <col width="15.85546875" customWidth="1" style="30" min="101" max="101"/>
+    <col width="9.28515625" customWidth="1" style="30" min="102" max="102"/>
+    <col width="16.7109375" customWidth="1" style="30" min="103" max="104"/>
+    <col width="12.85546875" customWidth="1" style="30" min="105" max="105"/>
+    <col width="32.42578125" customWidth="1" style="30" min="106" max="106"/>
+    <col width="11.7109375" customWidth="1" style="30" min="107" max="107"/>
+    <col width="35" customWidth="1" style="30" min="108" max="108"/>
+    <col width="18.140625" customWidth="1" style="30" min="109" max="109"/>
+    <col width="15.7109375" customWidth="1" style="30" min="110" max="110"/>
+    <col width="24" customWidth="1" style="30" min="111" max="111"/>
+    <col width="11.5703125" customWidth="1" style="30" min="112" max="112"/>
+    <col width="8.28515625" customWidth="1" style="30" min="113" max="113"/>
+    <col width="16.5703125" customWidth="1" style="30" min="114" max="114"/>
+    <col width="32.85546875" customWidth="1" style="30" min="115" max="115"/>
+    <col width="18.7109375" customWidth="1" style="30" min="116" max="116"/>
+    <col width="18.28515625" customWidth="1" style="30" min="117" max="117"/>
+    <col width="10.42578125" customWidth="1" style="30" min="118" max="118"/>
+    <col width="9.7109375" customWidth="1" style="30" min="119" max="119"/>
+    <col width="12.7109375" customWidth="1" style="30" min="120" max="120"/>
+    <col width="11.7109375" customWidth="1" style="30" min="121" max="121"/>
+    <col width="24" customWidth="1" style="30" min="122" max="122"/>
+    <col width="43.7109375" customWidth="1" style="30" min="123" max="123"/>
+    <col width="44.85546875" customWidth="1" style="30" min="124" max="124"/>
+    <col width="30.140625" customWidth="1" style="30" min="125" max="125"/>
+    <col width="29.42578125" customWidth="1" style="30" min="126" max="126"/>
+    <col width="25.28515625" customWidth="1" style="30" min="127" max="127"/>
+    <col width="9.5703125" customWidth="1" style="30" min="128" max="128"/>
+    <col width="25.7109375" customWidth="1" style="30" min="129" max="129"/>
+    <col width="19.7109375" customWidth="1" style="30" min="130" max="130"/>
+    <col width="28.5703125" customWidth="1" style="30" min="131" max="131"/>
+    <col width="21.140625" customWidth="1" style="30" min="132" max="132"/>
+    <col width="14.5703125" customWidth="1" style="30" min="133" max="133"/>
+    <col width="20.5703125" customWidth="1" style="30" min="134" max="134"/>
+    <col width="18.28515625" customWidth="1" style="30" min="135" max="135"/>
+    <col width="18.85546875" customWidth="1" style="30" min="136" max="136"/>
+    <col width="35" customWidth="1" style="30" min="137" max="137"/>
+    <col width="20" customWidth="1" style="30" min="138" max="138"/>
+    <col width="32.42578125" customWidth="1" style="30" min="139" max="139"/>
+    <col width="21.5703125" customWidth="1" style="30" min="140" max="140"/>
+    <col width="13.5703125" customWidth="1" style="30" min="141" max="141"/>
+    <col width="26.28515625" customWidth="1" style="30" min="142" max="142"/>
+    <col width="19.140625" customWidth="1" style="30" min="143" max="143"/>
+    <col width="44" customWidth="1" style="30" min="144" max="144"/>
+    <col width="23.5703125" customWidth="1" style="30" min="145" max="145"/>
+    <col width="26.28515625" customWidth="1" style="30" min="146" max="146"/>
+    <col width="34.85546875" customWidth="1" style="30" min="147" max="147"/>
+    <col width="9.140625" customWidth="1" style="30" min="148" max="148"/>
+    <col width="15.85546875" customWidth="1" style="30" min="149" max="149"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="50" thickBot="1">
@@ -5152,227 +5166,235 @@
       </c>
       <c r="Q1" s="56" t="inlineStr">
         <is>
+          <t>Fee_CycleStartDate</t>
+        </is>
+      </c>
+      <c r="R1" s="56" t="inlineStr">
+        <is>
+          <t>Fee_AccrualEndDate</t>
+        </is>
+      </c>
+      <c r="S1" s="56" t="inlineStr">
+        <is>
           <t>Fee_AccruedToDate</t>
         </is>
       </c>
-      <c r="R1" s="56" t="inlineStr">
+      <c r="T1" s="56" t="inlineStr">
         <is>
           <t>Fee_PaidToDate</t>
         </is>
       </c>
-      <c r="S1" s="56" t="inlineStr">
+      <c r="U1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Alias</t>
         </is>
       </c>
-      <c r="T1" s="56" t="inlineStr">
+      <c r="V1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RiskType</t>
         </is>
       </c>
-      <c r="U1" s="56" t="inlineStr">
+      <c r="W1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="V1" s="56" t="inlineStr">
+      <c r="X1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_EffectiveDate</t>
         </is>
       </c>
-      <c r="W1" s="56" t="inlineStr">
+      <c r="Y1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetAmount</t>
         </is>
       </c>
-      <c r="X1" s="56" t="inlineStr">
+      <c r="Z1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBNetFacCCYAmount</t>
         </is>
       </c>
-      <c r="Y1" s="56" t="inlineStr">
+      <c r="AA1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_MaturityExpiryDate</t>
         </is>
       </c>
-      <c r="Z1" s="77" t="inlineStr">
+      <c r="AB1" s="77" t="inlineStr">
         <is>
           <t>Outstanding_Favouree</t>
         </is>
       </c>
-      <c r="AA1" s="56" t="inlineStr">
+      <c r="AC1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_HBGrossAmount</t>
         </is>
       </c>
-      <c r="AB1" s="56" t="inlineStr">
+      <c r="AD1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalOriginalAmount</t>
         </is>
       </c>
-      <c r="AC1" s="56" t="inlineStr">
+      <c r="AE1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_GlobalCurrentAmount</t>
         </is>
       </c>
-      <c r="AD1" s="56" t="inlineStr">
+      <c r="AF1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingFrequency</t>
         </is>
       </c>
-      <c r="AE1" s="56" t="inlineStr">
+      <c r="AG1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_RepricingDate</t>
         </is>
       </c>
-      <c r="AF1" s="56" t="inlineStr">
+      <c r="AH1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PaymentMode</t>
         </is>
       </c>
-      <c r="AG1" s="56" t="inlineStr">
+      <c r="AI1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="AH1" s="56" t="inlineStr">
+      <c r="AJ1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_PricingOption</t>
         </is>
       </c>
-      <c r="AI1" s="56" t="inlineStr">
+      <c r="AK1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_Margin</t>
         </is>
       </c>
-      <c r="AJ1" s="56" t="inlineStr">
+      <c r="AL1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AllInRate</t>
         </is>
       </c>
-      <c r="AK1" s="56" t="inlineStr">
+      <c r="AM1" s="56" t="inlineStr">
         <is>
           <t>Outstanding_AccruedInterest</t>
         </is>
       </c>
-      <c r="AL1" s="77" t="inlineStr">
+      <c r="AN1" s="77" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="AM1" s="77" t="inlineStr">
+      <c r="AO1" s="77" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="AN1" s="77" t="inlineStr">
+      <c r="AP1" s="77" t="inlineStr">
         <is>
           <t>OutstandingSelect_Type</t>
         </is>
       </c>
-      <c r="AO1" s="77" t="inlineStr">
+      <c r="AQ1" s="77" t="inlineStr">
         <is>
           <t>Borrower1_ShortName</t>
         </is>
       </c>
-      <c r="AP1" s="77" t="inlineStr">
+      <c r="AR1" s="77" t="inlineStr">
         <is>
           <t>Computed_ProjectedCycleDue</t>
         </is>
       </c>
-      <c r="AQ1" s="77" t="inlineStr">
+      <c r="AS1" s="77" t="inlineStr">
         <is>
           <t>IssuanceFeePayment_EffectiveDate</t>
         </is>
       </c>
-      <c r="AR1" s="77" t="inlineStr">
+      <c r="AT1" s="77" t="inlineStr">
         <is>
           <t>SBLCFeePayment_NoticeMethod</t>
         </is>
       </c>
-      <c r="AS1" s="81" t="inlineStr">
+      <c r="AU1" s="81" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="AT1" s="81" t="inlineStr">
+      <c r="AV1" s="81" t="inlineStr">
         <is>
           <t>Search_By</t>
         </is>
       </c>
-      <c r="AU1" s="77" t="inlineStr">
+      <c r="AW1" s="77" t="inlineStr">
         <is>
           <t>CycleNumber</t>
         </is>
       </c>
-      <c r="AV1" s="44" t="inlineStr">
+      <c r="AX1" s="44" t="inlineStr">
         <is>
           <t>Workflow_Item</t>
         </is>
       </c>
-      <c r="AW1" s="44" t="inlineStr">
+      <c r="AY1" s="44" t="inlineStr">
         <is>
           <t>LIQCustomer_ID</t>
         </is>
       </c>
-      <c r="AX1" s="44" t="inlineStr">
+      <c r="AZ1" s="44" t="inlineStr">
         <is>
           <t>Borrower_Profile</t>
         </is>
       </c>
-      <c r="AY1" s="71" t="inlineStr">
+      <c r="BA1" s="71" t="inlineStr">
         <is>
           <t>RemittanceInstruction_RTGSDescriptionAUD</t>
         </is>
       </c>
-      <c r="AZ1" s="71" t="inlineStr">
+      <c r="BB1" s="71" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
       </c>
-      <c r="BA1" s="44" t="inlineStr">
+      <c r="BC1" s="44" t="inlineStr">
         <is>
           <t>HostBankSharePct</t>
         </is>
       </c>
-      <c r="BB1" s="44" t="inlineStr">
+      <c r="BD1" s="44" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="BC1" s="44" t="inlineStr">
+      <c r="BE1" s="44" t="inlineStr">
         <is>
           <t>Servicing_Alias</t>
         </is>
       </c>
-      <c r="BD1" s="44" t="inlineStr">
+      <c r="BF1" s="44" t="inlineStr">
         <is>
           <t>Servicing_Name</t>
         </is>
       </c>
-      <c r="BE1" s="44" t="inlineStr">
+      <c r="BG1" s="44" t="inlineStr">
         <is>
           <t>Servicing_Location</t>
         </is>
       </c>
-      <c r="BF1" s="71" t="inlineStr">
+      <c r="BH1" s="71" t="inlineStr">
         <is>
           <t>Computed_ProjectedCycleDue</t>
         </is>
       </c>
-      <c r="BG1" s="71" t="inlineStr">
+      <c r="BI1" s="71" t="inlineStr">
         <is>
           <t>Host_Bank</t>
         </is>
       </c>
-      <c r="BH1" s="150" t="inlineStr">
+      <c r="BJ1" s="150" t="inlineStr">
         <is>
           <t>AccrualRule_PayInAdvance</t>
         </is>
       </c>
-      <c r="BJ1" s="150" t="n"/>
-      <c r="CR1" s="80" t="n"/>
-      <c r="CS1" s="80" t="n"/>
+      <c r="BL1" s="150" t="n"/>
       <c r="CT1" s="80" t="n"/>
       <c r="CU1" s="80" t="n"/>
       <c r="CV1" s="80" t="n"/>
@@ -5423,6 +5445,8 @@
       <c r="EO1" s="80" t="n"/>
       <c r="EP1" s="80" t="n"/>
       <c r="EQ1" s="80" t="n"/>
+      <c r="ER1" s="80" t="n"/>
+      <c r="ES1" s="80" t="n"/>
     </row>
     <row r="2" ht="15" customFormat="1" customHeight="1" s="82">
       <c r="A2" s="30" t="inlineStr">
@@ -5497,205 +5521,205 @@
           <t>2020-10-15</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
+      <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="n"/>
       <c r="S2" s="1" t="inlineStr">
         <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="n"/>
+      <c r="U2" s="1" t="inlineStr">
+        <is>
           <t>60000786</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>Financial Letter of Credit</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>2020-10-15</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>2021-10-15</t>
         </is>
       </c>
-      <c r="Z2" s="38" t="inlineStr">
+      <c r="AB2" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="AA2" s="1" t="inlineStr">
+      <c r="AC2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AB2" s="1" t="inlineStr">
+      <c r="AD2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
+      <c r="AE2" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AD2" s="30" t="n"/>
-      <c r="AE2" s="30" t="n"/>
       <c r="AF2" s="30" t="n"/>
       <c r="AG2" s="30" t="n"/>
       <c r="AH2" s="30" t="n"/>
       <c r="AI2" s="30" t="n"/>
       <c r="AJ2" s="30" t="n"/>
       <c r="AK2" s="30" t="n"/>
-      <c r="AL2" s="1" t="inlineStr">
+      <c r="AL2" s="30" t="n"/>
+      <c r="AM2" s="30" t="n"/>
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>COMSEE_SC3_14092020203358</t>
         </is>
       </c>
-      <c r="AM2" s="1" t="inlineStr">
+      <c r="AO2" s="1" t="inlineStr">
         <is>
           <t>COMSEEFACBG_14092020204147</t>
         </is>
       </c>
-      <c r="AN2" s="1" t="inlineStr">
+      <c r="AP2" s="1" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AO2" s="1" t="inlineStr">
+      <c r="AQ2" s="1" t="inlineStr">
         <is>
           <t>BORROWER1111</t>
         </is>
       </c>
-      <c r="AP2" s="1" t="n">
+      <c r="AR2" s="1" t="n">
         <v>0.11</v>
       </c>
-      <c r="AQ2" s="30" t="inlineStr">
+      <c r="AS2" s="30" t="inlineStr">
         <is>
           <t>17-Sep-2018</t>
         </is>
       </c>
-      <c r="AR2" s="82" t="inlineStr">
+      <c r="AT2" s="82" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="AS2" s="82" t="inlineStr">
+      <c r="AU2" s="82" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AT2" s="82" t="inlineStr">
+      <c r="AV2" s="82" t="inlineStr">
         <is>
           <t>Deal/Facility</t>
         </is>
       </c>
-      <c r="AU2" s="83" t="inlineStr">
+      <c r="AW2" s="83" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AV2" s="30" t="inlineStr">
+      <c r="AX2" s="30" t="inlineStr">
         <is>
           <t>Create Cashflows</t>
         </is>
       </c>
-      <c r="AW2" s="30" t="inlineStr">
+      <c r="AY2" s="30" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="AX2" s="30" t="inlineStr">
+      <c r="AZ2" s="30" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="AY2" s="1" t="inlineStr">
+      <c r="BA2" s="1" t="inlineStr">
         <is>
           <t>RTGS1</t>
         </is>
       </c>
-      <c r="AZ2" s="1" t="inlineStr">
+      <c r="BB2" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="BA2" s="30" t="inlineStr">
+      <c r="BC2" s="30" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="BB2" s="30" t="inlineStr">
+      <c r="BD2" s="30" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="BC2" s="30" t="inlineStr">
+      <c r="BE2" s="30" t="inlineStr">
         <is>
           <t>JB</t>
         </is>
       </c>
-      <c r="BD2" s="30" t="inlineStr">
+      <c r="BF2" s="30" t="inlineStr">
         <is>
           <t>BLOGGS</t>
         </is>
       </c>
-      <c r="BE2" s="30" t="inlineStr">
+      <c r="BG2" s="30" t="inlineStr">
         <is>
           <t>Melbourne, VIC,Australia</t>
         </is>
       </c>
-      <c r="BF2" s="30" t="n">
+      <c r="BH2" s="30" t="n">
         <v>0.33</v>
       </c>
-      <c r="BG2" s="30" t="inlineStr">
+      <c r="BI2" s="30" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/IT_AKD</t>
         </is>
       </c>
-      <c r="BH2" s="83" t="n"/>
-      <c r="BI2" s="83" t="n"/>
       <c r="BJ2" s="83" t="n"/>
       <c r="BK2" s="83" t="n"/>
       <c r="BL2" s="83" t="n"/>
       <c r="BM2" s="83" t="n"/>
       <c r="BN2" s="83" t="n"/>
       <c r="BO2" s="83" t="n"/>
+      <c r="BP2" s="83" t="n"/>
       <c r="BQ2" s="83" t="n"/>
-      <c r="BR2" s="83" t="n"/>
       <c r="BS2" s="83" t="n"/>
+      <c r="BT2" s="83" t="n"/>
       <c r="BU2" s="83" t="n"/>
-      <c r="BV2" s="83" t="n"/>
       <c r="BW2" s="83" t="n"/>
       <c r="BX2" s="83" t="n"/>
       <c r="BY2" s="83" t="n"/>
       <c r="BZ2" s="83" t="n"/>
-      <c r="CC2" s="83" t="n"/>
+      <c r="CA2" s="83" t="n"/>
+      <c r="CB2" s="83" t="n"/>
       <c r="CE2" s="83" t="n"/>
-      <c r="CF2" s="83" t="n"/>
-      <c r="CK2" s="83" t="n"/>
-      <c r="CN2" s="83" t="n"/>
-      <c r="CQ2" s="83" t="n"/>
-      <c r="CR2" s="83" t="n"/>
+      <c r="CG2" s="83" t="n"/>
+      <c r="CH2" s="83" t="n"/>
+      <c r="CM2" s="83" t="n"/>
+      <c r="CP2" s="83" t="n"/>
       <c r="CS2" s="83" t="n"/>
       <c r="CT2" s="83" t="n"/>
       <c r="CU2" s="83" t="n"/>
@@ -5704,8 +5728,8 @@
       <c r="CX2" s="83" t="n"/>
       <c r="CY2" s="83" t="n"/>
       <c r="CZ2" s="83" t="n"/>
+      <c r="DA2" s="83" t="n"/>
       <c r="DB2" s="83" t="n"/>
-      <c r="DC2" s="83" t="n"/>
       <c r="DD2" s="83" t="n"/>
       <c r="DE2" s="83" t="n"/>
       <c r="DF2" s="83" t="n"/>
@@ -5716,8 +5740,8 @@
       <c r="DK2" s="83" t="n"/>
       <c r="DL2" s="83" t="n"/>
       <c r="DM2" s="83" t="n"/>
-      <c r="DP2" s="83" t="n"/>
-      <c r="DQ2" s="83" t="n"/>
+      <c r="DN2" s="83" t="n"/>
+      <c r="DO2" s="83" t="n"/>
       <c r="DR2" s="83" t="n"/>
       <c r="DS2" s="83" t="n"/>
       <c r="DT2" s="83" t="n"/>
@@ -5727,9 +5751,9 @@
       <c r="DX2" s="83" t="n"/>
       <c r="DY2" s="83" t="n"/>
       <c r="DZ2" s="83" t="n"/>
-      <c r="ED2" s="83" t="n"/>
+      <c r="EA2" s="83" t="n"/>
+      <c r="EB2" s="83" t="n"/>
       <c r="EF2" s="83" t="n"/>
-      <c r="EG2" s="83" t="n"/>
       <c r="EH2" s="83" t="n"/>
       <c r="EI2" s="83" t="n"/>
       <c r="EJ2" s="83" t="n"/>
@@ -5740,6 +5764,8 @@
       <c r="EO2" s="83" t="n"/>
       <c r="EP2" s="83" t="n"/>
       <c r="EQ2" s="83" t="n"/>
+      <c r="ER2" s="83" t="n"/>
+      <c r="ES2" s="83" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="151" t="inlineStr">
@@ -5812,178 +5838,180 @@
           <t>2020-11-20</t>
         </is>
       </c>
-      <c r="Q3" s="1" t="inlineStr">
+      <c r="Q3" s="1" t="n"/>
+      <c r="R3" s="1" t="n"/>
+      <c r="S3" s="1" t="inlineStr">
         <is>
           <t>4.29</t>
         </is>
       </c>
-      <c r="R3" s="1" t="inlineStr">
+      <c r="T3" s="1" t="inlineStr">
         <is>
           <t>4.29</t>
         </is>
       </c>
-      <c r="S3" s="1" t="inlineStr">
+      <c r="U3" s="1" t="inlineStr">
         <is>
           <t>60000787</t>
         </is>
       </c>
-      <c r="T3" s="1" t="inlineStr">
+      <c r="V3" s="1" t="inlineStr">
         <is>
           <t>Financial Letter of Credit</t>
         </is>
       </c>
-      <c r="U3" s="1" t="inlineStr">
+      <c r="W3" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="V3" s="1" t="inlineStr">
+      <c r="X3" s="1" t="inlineStr">
         <is>
           <t>2020-10-16</t>
         </is>
       </c>
-      <c r="W3" s="1" t="inlineStr">
+      <c r="Y3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="X3" s="1" t="inlineStr">
+      <c r="Z3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="Y3" s="1" t="inlineStr">
+      <c r="AA3" s="1" t="inlineStr">
         <is>
           <t>2021-10-18</t>
         </is>
       </c>
-      <c r="Z3" s="38" t="inlineStr">
+      <c r="AB3" s="38" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="AA3" s="1" t="inlineStr">
+      <c r="AC3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AB3" s="1" t="inlineStr">
+      <c r="AD3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AC3" s="1" t="inlineStr">
+      <c r="AE3" s="1" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AL3" s="1" t="inlineStr">
+      <c r="AN3" s="1" t="inlineStr">
         <is>
           <t>COMSEE_SC3_14092020211728</t>
         </is>
       </c>
-      <c r="AM3" s="1" t="inlineStr">
+      <c r="AO3" s="1" t="inlineStr">
         <is>
           <t>COMSEEFACBG_14092020212610</t>
         </is>
       </c>
-      <c r="AN3" s="1" t="inlineStr">
+      <c r="AP3" s="1" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AO3" s="1" t="inlineStr">
+      <c r="AQ3" s="1" t="inlineStr">
         <is>
           <t>BORROWER1111</t>
         </is>
       </c>
-      <c r="AP3" s="1" t="n">
+      <c r="AR3" s="1" t="n">
         <v>0.11</v>
       </c>
-      <c r="AQ3" s="30" t="inlineStr">
+      <c r="AS3" s="30" t="inlineStr">
         <is>
           <t>17-Sep-2018</t>
         </is>
       </c>
-      <c r="AR3" s="82" t="inlineStr">
+      <c r="AT3" s="82" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="AS3" s="82" t="inlineStr">
+      <c r="AU3" s="82" t="inlineStr">
         <is>
           <t>SBLC/Guarantee</t>
         </is>
       </c>
-      <c r="AT3" s="82" t="inlineStr">
+      <c r="AV3" s="82" t="inlineStr">
         <is>
           <t>Deal/Facility</t>
         </is>
       </c>
-      <c r="AU3" s="83" t="inlineStr">
+      <c r="AW3" s="83" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AV3" s="30" t="inlineStr">
+      <c r="AX3" s="30" t="inlineStr">
         <is>
           <t>Create Cashflows</t>
         </is>
       </c>
-      <c r="AW3" s="30" t="inlineStr">
+      <c r="AY3" s="30" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="AX3" s="30" t="inlineStr">
+      <c r="AZ3" s="30" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="AY3" s="1" t="inlineStr">
+      <c r="BA3" s="1" t="inlineStr">
         <is>
           <t>RTGS1</t>
         </is>
       </c>
-      <c r="AZ3" s="1" t="inlineStr">
+      <c r="BB3" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="BA3" s="30" t="inlineStr">
+      <c r="BC3" s="30" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="BB3" s="30" t="inlineStr">
+      <c r="BD3" s="30" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="BC3" s="30" t="inlineStr">
+      <c r="BE3" s="30" t="inlineStr">
         <is>
           <t>JB</t>
         </is>
       </c>
-      <c r="BD3" s="30" t="inlineStr">
+      <c r="BF3" s="30" t="inlineStr">
         <is>
           <t>BLOGGS</t>
         </is>
       </c>
-      <c r="BE3" s="30" t="inlineStr">
+      <c r="BG3" s="30" t="inlineStr">
         <is>
           <t>Melbourne, VIC,Australia</t>
         </is>
       </c>
-      <c r="BF3" s="30" t="n">
+      <c r="BH3" s="30" t="n">
         <v>0.33</v>
       </c>
-      <c r="BG3" s="30" t="inlineStr">
+      <c r="BI3" s="30" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/IT_AKD</t>
         </is>
       </c>
-      <c r="BH3" s="40" t="inlineStr">
+      <c r="BJ3" s="40" t="inlineStr">
         <is>
           <t>Pay In Advance</t>
         </is>
@@ -20946,11 +20974,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DC2"/>
+  <dimension ref="A1:DC3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AY2" sqref="AY2"/>
+      <pane xSplit="2" topLeftCell="AO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -21607,7 +21635,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>3000730</t>
+          <t>3000733</t>
         </is>
       </c>
       <c r="D2" s="45" t="inlineStr">
@@ -21632,17 +21660,17 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_18092020164920</t>
+          <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>1000861</t>
+          <t>1000865</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>2020-11-25</t>
+          <t>2020-11-26</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -21726,7 +21754,7 @@
       </c>
       <c r="AB2" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM18092020165749</t>
+          <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
       <c r="AC2" s="38" t="inlineStr">
@@ -21923,7 +21951,7 @@
       </c>
       <c r="BQ2" s="1" t="inlineStr">
         <is>
-          <t>25-Nov-2021</t>
+          <t>26-Nov-2021</t>
         </is>
       </c>
       <c r="BR2" s="30" t="inlineStr">
@@ -22103,6 +22131,515 @@
         </is>
       </c>
       <c r="DC2" s="30" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>3000734</t>
+        </is>
+      </c>
+      <c r="D3" s="45" t="inlineStr">
+        <is>
+          <t>rodel</t>
+        </is>
+      </c>
+      <c r="E3" s="37" t="inlineStr">
+        <is>
+          <t>\DataSet\API_DataSet\Input\ComSee\</t>
+        </is>
+      </c>
+      <c r="F3" s="37" t="inlineStr">
+        <is>
+          <t>COM_RES_07</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>2019-10-12</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_20092020200120</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>1000866</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>2020-11-26</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="L3" s="45" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>AUSNA</t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>Non-Agency Australia</t>
+        </is>
+      </c>
+      <c r="O3" s="38" t="inlineStr">
+        <is>
+          <t>BP_CML</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>Commercial Lending</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="V3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="W3" s="1" t="inlineStr">
+        <is>
+          <t>GLB</t>
+        </is>
+      </c>
+      <c r="X3" s="38" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="Y3" s="3" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_</t>
+        </is>
+      </c>
+      <c r="Z3" s="3" t="inlineStr">
+        <is>
+          <t>CS7</t>
+        </is>
+      </c>
+      <c r="AA3" s="30" t="inlineStr">
+        <is>
+          <t>S724062019190029CNO</t>
+        </is>
+      </c>
+      <c r="AB3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020200906</t>
+        </is>
+      </c>
+      <c r="AC3" s="38" t="inlineStr">
+        <is>
+          <t>Sales Group 1</t>
+        </is>
+      </c>
+      <c r="AD3" s="1" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="AE3" s="30" t="inlineStr">
+        <is>
+          <t>Melbourne, VIC,Australia</t>
+        </is>
+      </c>
+      <c r="AF3" s="38" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="AG3" s="38" t="inlineStr">
+        <is>
+          <t>GCP</t>
+        </is>
+      </c>
+      <c r="AH3" s="38" t="inlineStr">
+        <is>
+          <t>General Corp Purpose</t>
+        </is>
+      </c>
+      <c r="AI3" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="AJ3" s="38" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="AK3" s="38" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AL3" s="38" t="inlineStr">
+        <is>
+          <t>Lending,${SPACE}${SPACE}Operations</t>
+        </is>
+      </c>
+      <c r="AM3" s="38" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AN3" s="38" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="AO3" s="38" t="inlineStr">
+        <is>
+          <t>10,000,000.00</t>
+        </is>
+      </c>
+      <c r="AP3" s="38" t="inlineStr">
+        <is>
+          <t>Sydney, Australia</t>
+        </is>
+      </c>
+      <c r="AQ3" s="40" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AR3" s="38" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AS3" s="38" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AT3" s="38" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AU3" s="38" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AV3" s="38" t="inlineStr">
+        <is>
+          <t>Start of current cycle</t>
+        </is>
+      </c>
+      <c r="AW3" s="30" t="inlineStr">
+        <is>
+          <t>Start of next interest cycle</t>
+        </is>
+      </c>
+      <c r="AX3" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY3" s="38" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="AZ3" s="38" t="inlineStr">
+        <is>
+          <t>Effective date of change</t>
+        </is>
+      </c>
+      <c r="BA3" s="38" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="BB3" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC3" s="30" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="BD3" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="BE3" s="38" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="BF3" s="38" t="inlineStr">
+        <is>
+          <t>IT_COL</t>
+        </is>
+      </c>
+      <c r="BG3" s="30" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="BH3" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="BI3" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="BJ3" s="30" t="inlineStr">
+        <is>
+          <t>Add Comment</t>
+        </is>
+      </c>
+      <c r="BK3" s="38" t="inlineStr">
+        <is>
+          <t>Business Verification,${SPACE}${SPACE}BVT</t>
+        </is>
+      </c>
+      <c r="BL3" s="30" t="inlineStr">
+        <is>
+          <t>LENDING</t>
+        </is>
+      </c>
+      <c r="BM3" s="38" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="BN3" s="38" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="BO3" s="38" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="BP3" s="38" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="BQ3" s="1" t="inlineStr">
+        <is>
+          <t>26-Nov-2021</t>
+        </is>
+      </c>
+      <c r="BR3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="BT3" s="41" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia -DBU</t>
+        </is>
+      </c>
+      <c r="BU3" s="41" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="BV3" s="41" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BW3" s="41" t="inlineStr">
+        <is>
+          <t>ZOE</t>
+        </is>
+      </c>
+      <c r="BX3" s="41" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="BY3" s="41" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="BZ3" s="41" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+      <c r="CA3" s="41" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank Australia - DBU</t>
+        </is>
+      </c>
+      <c r="CB3" s="104" t="inlineStr">
+        <is>
+          <t>FJAPR01</t>
+        </is>
+      </c>
+      <c r="CC3" s="2" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CD3" s="104" t="inlineStr">
+        <is>
+          <t>FJUSR01</t>
+        </is>
+      </c>
+      <c r="CE3" s="2" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CF3" s="104" t="inlineStr">
+        <is>
+          <t>FJMGR01</t>
+        </is>
+      </c>
+      <c r="CG3" s="104" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CH3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CI3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CJ3" s="41" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH% DBU</t>
+        </is>
+      </c>
+      <c r="CK3" s="41" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK OF AUSTRALIA - DBU</t>
+        </is>
+      </c>
+      <c r="CL3" s="41" t="inlineStr">
+        <is>
+          <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
+        </is>
+      </c>
+      <c r="CM3" s="41" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="CN3" s="41" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="CO3" s="41" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="CP3" s="41" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="CQ3" s="41" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="CR3" s="41" t="inlineStr">
+        <is>
+          <t>BLOGGS</t>
+        </is>
+      </c>
+      <c r="CS3" s="41" t="inlineStr">
+        <is>
+          <t>Bloggs,  John</t>
+        </is>
+      </c>
+      <c r="CT3" s="41" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="CU3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CV3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CW3" s="3" t="n"/>
+      <c r="CX3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CY3" s="41" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="CZ3" s="41" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="DA3" s="41" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="DB3" s="41" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK AUST -DBU</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -22117,13 +22654,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY2"/>
+  <dimension ref="A1:AY3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="AN2" sqref="AN2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -22423,22 +22960,22 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM18092020165749</t>
+          <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>3000730</t>
+          <t>3000733</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>2020-11-25</t>
+          <t>2020-11-26</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>2021-12-25</t>
+          <t>2021-12-26</t>
         </is>
       </c>
       <c r="G2" s="30" t="inlineStr">
@@ -22550,7 +23087,7 @@
       </c>
       <c r="AD2" s="1" t="inlineStr">
         <is>
-          <t>2021-11-25</t>
+          <t>2021-11-26</t>
         </is>
       </c>
       <c r="AE2" s="3" t="inlineStr">
@@ -22560,7 +23097,7 @@
       </c>
       <c r="AF2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_18092020164920</t>
+          <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
       <c r="AG2" s="30" t="inlineStr">
@@ -22649,6 +23186,250 @@
         </is>
       </c>
       <c r="AY2" s="48" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020200906</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>3000734</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>2020-11-26</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>2021-12-26</t>
+        </is>
+      </c>
+      <c r="G3" s="30" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>IT_COL|Corporate Lending</t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>AUSNA</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>Non-Agency Australia</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="V3" s="1" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="W3" s="1" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="X3" s="1" t="inlineStr">
+        <is>
+          <t>HFIAU</t>
+        </is>
+      </c>
+      <c r="Y3" s="1" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="Z3" s="1" t="inlineStr">
+        <is>
+          <t>CB001</t>
+        </is>
+      </c>
+      <c r="AA3" s="1" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="AB3" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AC3" s="1" t="inlineStr">
+        <is>
+          <t>Australian (Sydney)</t>
+        </is>
+      </c>
+      <c r="AD3" s="1" t="inlineStr">
+        <is>
+          <t>2021-11-26</t>
+        </is>
+      </c>
+      <c r="AE3" s="3" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM</t>
+        </is>
+      </c>
+      <c r="AF3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_20092020200120</t>
+        </is>
+      </c>
+      <c r="AG3" s="30" t="inlineStr">
+        <is>
+          <t>S124062019191047FMB</t>
+        </is>
+      </c>
+      <c r="AH3" s="47" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AI3" s="47" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="AK3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="AL3" s="30" t="inlineStr">
+        <is>
+          <t>16-Aug-2019</t>
+        </is>
+      </c>
+      <c r="AM3" s="30" t="inlineStr">
+        <is>
+          <t>15-Sep-2019</t>
+        </is>
+      </c>
+      <c r="AN3" s="38" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AO3" s="38" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="AP3" s="47" t="inlineStr">
+        <is>
+          <t>Fixed Rate Loan</t>
+        </is>
+      </c>
+      <c r="AQ3" s="47" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AR3" s="47" t="inlineStr">
+        <is>
+          <t>Acquisitions</t>
+        </is>
+      </c>
+      <c r="AS3" s="30" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AT3" s="30" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia</t>
+        </is>
+      </c>
+      <c r="AU3" s="30" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="AV3" s="1" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="AW3" s="30" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AX3" s="30" t="inlineStr">
+        <is>
+          <t>BLOGGS</t>
+        </is>
+      </c>
+      <c r="AY3" s="48" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
@@ -22667,13 +23448,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="U3" sqref="U3"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -22681,24 +23462,24 @@
     <col width="6.140625" customWidth="1" style="30" min="1" max="1"/>
     <col width="21.7109375" customWidth="1" style="30" min="2" max="7"/>
     <col width="27.85546875" customWidth="1" style="30" min="8" max="8"/>
-    <col width="21.7109375" customWidth="1" style="30" min="9" max="18"/>
-    <col width="22.85546875" customWidth="1" style="30" min="19" max="19"/>
-    <col width="22.7109375" customWidth="1" style="30" min="20" max="20"/>
-    <col width="27.140625" customWidth="1" style="30" min="21" max="21"/>
-    <col width="23.42578125" customWidth="1" style="30" min="22" max="22"/>
-    <col width="21.85546875" customWidth="1" style="30" min="23" max="23"/>
-    <col width="26.42578125" customWidth="1" style="30" min="24" max="24"/>
-    <col width="23.5703125" customWidth="1" style="30" min="25" max="26"/>
-    <col width="21.85546875" customWidth="1" style="30" min="27" max="27"/>
-    <col width="15.7109375" customWidth="1" style="30" min="28" max="28"/>
-    <col width="24.7109375" customWidth="1" style="30" min="29" max="30"/>
-    <col width="16.42578125" customWidth="1" style="30" min="31" max="31"/>
-    <col width="21.42578125" customWidth="1" style="30" min="32" max="32"/>
-    <col width="17.85546875" customWidth="1" style="30" min="33" max="33"/>
-    <col width="21" customWidth="1" style="30" min="34" max="35"/>
-    <col width="22" customWidth="1" style="30" min="36" max="36"/>
-    <col width="25.42578125" customWidth="1" style="30" min="37" max="37"/>
-    <col width="26.5703125" bestFit="1" customWidth="1" min="38" max="38"/>
+    <col width="21.7109375" customWidth="1" style="30" min="9" max="20"/>
+    <col width="22.85546875" customWidth="1" style="30" min="21" max="21"/>
+    <col width="22.7109375" customWidth="1" style="30" min="22" max="22"/>
+    <col width="27.140625" customWidth="1" style="30" min="23" max="23"/>
+    <col width="23.42578125" customWidth="1" style="30" min="24" max="24"/>
+    <col width="21.85546875" customWidth="1" style="30" min="25" max="25"/>
+    <col width="26.42578125" customWidth="1" style="30" min="26" max="26"/>
+    <col width="23.5703125" customWidth="1" style="30" min="27" max="28"/>
+    <col width="21.85546875" customWidth="1" style="30" min="29" max="29"/>
+    <col width="15.7109375" customWidth="1" style="30" min="30" max="30"/>
+    <col width="24.7109375" customWidth="1" style="30" min="31" max="32"/>
+    <col width="16.42578125" customWidth="1" style="30" min="33" max="33"/>
+    <col width="21.42578125" customWidth="1" style="30" min="34" max="34"/>
+    <col width="17.85546875" customWidth="1" style="30" min="35" max="35"/>
+    <col width="21" customWidth="1" style="30" min="36" max="37"/>
+    <col width="22" customWidth="1" style="30" min="38" max="38"/>
+    <col width="25.42578125" customWidth="1" style="30" min="39" max="39"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" min="40" max="40"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="50">
@@ -22784,110 +23565,120 @@
       </c>
       <c r="Q1" s="56" t="inlineStr">
         <is>
+          <t>Fee_CycleStartDate</t>
+        </is>
+      </c>
+      <c r="R1" s="56" t="inlineStr">
+        <is>
+          <t>Fee_AccrualEndDate</t>
+        </is>
+      </c>
+      <c r="S1" s="56" t="inlineStr">
+        <is>
           <t>Fee_AccruedToDate</t>
         </is>
       </c>
-      <c r="R1" s="56" t="inlineStr">
+      <c r="T1" s="56" t="inlineStr">
         <is>
           <t>Fee_PaidToDate</t>
         </is>
       </c>
-      <c r="S1" s="50" t="inlineStr">
+      <c r="U1" s="50" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="T1" s="50" t="inlineStr">
+      <c r="V1" s="50" t="inlineStr">
         <is>
           <t>OngoingFee_Category1</t>
         </is>
       </c>
-      <c r="U1" s="50" t="inlineStr">
+      <c r="W1" s="50" t="inlineStr">
         <is>
           <t>OngoingFee_Type1</t>
         </is>
       </c>
-      <c r="V1" s="50" t="inlineStr">
+      <c r="X1" s="50" t="inlineStr">
         <is>
           <t>OngoingFee_RateBasis1</t>
         </is>
       </c>
-      <c r="W1" s="50" t="inlineStr">
+      <c r="Y1" s="50" t="inlineStr">
         <is>
           <t>OngoingFee_AfterItem</t>
         </is>
       </c>
-      <c r="X1" s="50" t="inlineStr">
+      <c r="Z1" s="50" t="inlineStr">
         <is>
           <t>OngoingFee_AfterItemType</t>
         </is>
       </c>
-      <c r="Y1" s="50" t="inlineStr">
+      <c r="AA1" s="50" t="inlineStr">
         <is>
           <t>Facility_PercentWhole</t>
         </is>
       </c>
-      <c r="Z1" s="50" t="inlineStr">
+      <c r="AB1" s="50" t="inlineStr">
         <is>
           <t>Facility_Percent</t>
         </is>
       </c>
-      <c r="AA1" s="50" t="inlineStr">
+      <c r="AC1" s="50" t="inlineStr">
         <is>
           <t>OngoingFee_SpreadType1</t>
         </is>
       </c>
-      <c r="AB1" s="50" t="inlineStr">
+      <c r="AD1" s="50" t="inlineStr">
         <is>
           <t>OngoingFee_SpreadType2</t>
         </is>
       </c>
-      <c r="AC1" s="50" t="inlineStr">
+      <c r="AE1" s="50" t="inlineStr">
         <is>
           <t>Interest_AddItem</t>
         </is>
       </c>
-      <c r="AD1" s="50" t="inlineStr">
+      <c r="AF1" s="50" t="inlineStr">
         <is>
           <t>Interest_OptionName1</t>
         </is>
       </c>
-      <c r="AE1" s="50" t="inlineStr">
+      <c r="AG1" s="50" t="inlineStr">
         <is>
           <t>Interest_RateBasis</t>
         </is>
       </c>
-      <c r="AF1" s="50" t="inlineStr">
+      <c r="AH1" s="50" t="inlineStr">
         <is>
           <t>Interest_SpreadType1</t>
         </is>
       </c>
-      <c r="AG1" s="50" t="inlineStr">
+      <c r="AI1" s="50" t="inlineStr">
         <is>
           <t>Interest_SpreadType2</t>
         </is>
       </c>
-      <c r="AH1" s="50" t="inlineStr">
+      <c r="AJ1" s="50" t="inlineStr">
         <is>
           <t>Interest_SpreadValue1</t>
         </is>
       </c>
-      <c r="AI1" s="50" t="inlineStr">
+      <c r="AK1" s="50" t="inlineStr">
         <is>
           <t>Interest_SpreadAmt1</t>
         </is>
       </c>
-      <c r="AJ1" s="50" t="inlineStr">
+      <c r="AL1" s="50" t="inlineStr">
         <is>
           <t>Interest_BaseRateCode1</t>
         </is>
       </c>
-      <c r="AK1" s="50" t="inlineStr">
+      <c r="AM1" s="50" t="inlineStr">
         <is>
           <t>Facility_PricingRuleOption1</t>
         </is>
       </c>
-      <c r="AL1" s="150" t="inlineStr">
+      <c r="AN1" s="150" t="inlineStr">
         <is>
           <t>AccrualRule_PayInAdvance</t>
         </is>
@@ -22916,7 +23707,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>3000730</t>
+          <t>3000733</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -22931,12 +23722,12 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM18092020165749</t>
+          <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000437</t>
+          <t>ONG000000000443</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
@@ -22961,127 +23752,339 @@
       </c>
       <c r="N2" s="1" t="inlineStr">
         <is>
-          <t>2020-11-25</t>
+          <t>2020-11-26</t>
         </is>
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>2021-12-25</t>
+          <t>2021-12-26</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
+          <t>2021-02-26</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>2020-11-26</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
           <t>2021-02-25</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="S2" s="1" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
-        <is>
-          <t>CSSC7_TERM18092020165749</t>
-        </is>
-      </c>
-      <c r="T2" s="47" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020193010</t>
+        </is>
+      </c>
+      <c r="V2" s="47" t="inlineStr">
         <is>
           <t>Facility Ongoing Fee</t>
         </is>
       </c>
-      <c r="U2" s="47" t="inlineStr">
+      <c r="W2" s="47" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="V2" s="52" t="inlineStr">
+      <c r="X2" s="52" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="W2" s="47" t="inlineStr">
+      <c r="Y2" s="47" t="inlineStr">
         <is>
           <t>FormulaCategory</t>
         </is>
       </c>
-      <c r="X2" s="47" t="inlineStr">
+      <c r="Z2" s="47" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="Y2" s="47" t="inlineStr">
+      <c r="AA2" s="47" t="inlineStr">
         <is>
           <t>4%</t>
         </is>
       </c>
-      <c r="Z2" s="47" t="inlineStr">
+      <c r="AB2" s="47" t="inlineStr">
         <is>
           <t>4.000000</t>
         </is>
       </c>
-      <c r="AA2" s="38" t="inlineStr">
+      <c r="AC2" s="38" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AB2" s="40" t="inlineStr">
+      <c r="AD2" s="40" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AC2" s="30" t="inlineStr">
+      <c r="AE2" s="30" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
       </c>
-      <c r="AD2" s="47" t="inlineStr">
+      <c r="AF2" s="47" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AE2" s="53" t="inlineStr">
+      <c r="AG2" s="53" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AF2" s="38" t="inlineStr">
+      <c r="AH2" s="38" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AG2" s="40" t="inlineStr">
+      <c r="AI2" s="40" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AH2" s="30" t="inlineStr">
+      <c r="AJ2" s="30" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AI2" s="30" t="inlineStr">
+      <c r="AK2" s="30" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AJ2" s="30" t="inlineStr">
+      <c r="AL2" s="30" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="AK2" s="30" t="inlineStr">
+      <c r="AM2" s="30" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AL2" s="40" t="inlineStr">
-        <is>
-          <t>Pay In Advance</t>
+      <c r="AN2" s="40" t="inlineStr">
+        <is>
+          <t>Pay In Arrears</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C3" s="10" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V2</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>3000734</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020200906</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>ONG000000000444</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>Released</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>2020-11-26</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>2021-12-26</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-26</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="inlineStr">
+        <is>
+          <t>2020-11-26</t>
+        </is>
+      </c>
+      <c r="R3" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-25</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020200906</t>
+        </is>
+      </c>
+      <c r="V3" s="47" t="inlineStr">
+        <is>
+          <t>Facility Ongoing Fee</t>
+        </is>
+      </c>
+      <c r="W3" s="47" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="X3" s="52" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="Y3" s="47" t="inlineStr">
+        <is>
+          <t>FormulaCategory</t>
+        </is>
+      </c>
+      <c r="Z3" s="47" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="AA3" s="47" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="AB3" s="47" t="inlineStr">
+        <is>
+          <t>4.000000</t>
+        </is>
+      </c>
+      <c r="AC3" s="38" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+      <c r="AD3" s="40" t="inlineStr">
+        <is>
+          <t>Basis Points</t>
+        </is>
+      </c>
+      <c r="AE3" s="30" t="inlineStr">
+        <is>
+          <t>Option</t>
+        </is>
+      </c>
+      <c r="AF3" s="47" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AG3" s="53" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="AH3" s="38" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+      <c r="AI3" s="40" t="inlineStr">
+        <is>
+          <t>Basis Points</t>
+        </is>
+      </c>
+      <c r="AJ3" s="30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AK3" s="30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AL3" s="30" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="AM3" s="30" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AN3" s="40" t="inlineStr">
+        <is>
+          <t>Pay In Arrears</t>
         </is>
       </c>
     </row>
@@ -23098,10 +24101,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -23352,7 +24355,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_18092020164920</t>
+          <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -23362,7 +24365,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM18092020165749</t>
+          <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -23427,7 +24430,7 @@
       </c>
       <c r="R2" s="1" t="inlineStr">
         <is>
-          <t>25-Dec-2021</t>
+          <t>26-Dec-2021</t>
         </is>
       </c>
       <c r="S2" s="2" t="inlineStr">
@@ -23536,6 +24539,208 @@
         </is>
       </c>
       <c r="AN2" s="30" t="inlineStr">
+        <is>
+          <t>Awaiting release</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_20092020200120</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020200906</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I3" s="30" t="inlineStr">
+        <is>
+          <t>ESPS11810226</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM17092020214046</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>60000242</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="O3" s="2" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="Q3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="R3" s="1" t="inlineStr">
+        <is>
+          <t>26-Dec-2021</t>
+        </is>
+      </c>
+      <c r="S3" s="2" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>Weeks</t>
+        </is>
+      </c>
+      <c r="W3" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="X3" s="30" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="Y3" s="2" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="Z3" s="30" t="inlineStr">
+        <is>
+          <t>Outstandings</t>
+        </is>
+      </c>
+      <c r="AA3" s="30" t="inlineStr">
+        <is>
+          <t>Awaiting Approval</t>
+        </is>
+      </c>
+      <c r="AB3" s="30" t="inlineStr">
+        <is>
+          <t>Loan Initial Drawdown</t>
+        </is>
+      </c>
+      <c r="AC3" s="2" t="inlineStr">
+        <is>
+          <t>Awaiting Rate Approval</t>
+        </is>
+      </c>
+      <c r="AD3" s="2" t="inlineStr">
+        <is>
+          <t>Awaiting Release Cashflows</t>
+        </is>
+      </c>
+      <c r="AE3" s="2" t="inlineStr">
+        <is>
+          <t>Borrower</t>
+        </is>
+      </c>
+      <c r="AF3" s="30" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="AG3" s="2" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="AH3" s="30" t="inlineStr">
+        <is>
+          <t>DOIT</t>
+        </is>
+      </c>
+      <c r="AI3" s="30" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AJ3" s="30" t="inlineStr">
+        <is>
+          <t>RTGSAUD1-0736</t>
+        </is>
+      </c>
+      <c r="AK3" s="108" t="inlineStr">
+        <is>
+          <t>12001001836</t>
+        </is>
+      </c>
+      <c r="AL3" s="108" t="inlineStr">
+        <is>
+          <t>18567000000</t>
+        </is>
+      </c>
+      <c r="AM3" s="30" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+      <c r="AN3" s="30" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
@@ -23554,11 +24759,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI2"/>
+  <dimension ref="A1:CI3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -23792,12 +24997,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_18092020164920</t>
+          <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM18092020165749</t>
+          <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
       <c r="E2" s="30" t="inlineStr">
@@ -23849,6 +25054,81 @@
         <v>100</v>
       </c>
       <c r="O2" s="30" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_20092020200120</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020200906</t>
+        </is>
+      </c>
+      <c r="E3" s="30" t="inlineStr">
+        <is>
+          <t>ESPS11810226</t>
+        </is>
+      </c>
+      <c r="F3" s="30" t="inlineStr">
+        <is>
+          <t>Deal/Facility</t>
+        </is>
+      </c>
+      <c r="G3" s="30" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>60000242</t>
+        </is>
+      </c>
+      <c r="I3" s="30" t="inlineStr">
+        <is>
+          <t>RTGSAUD1-0736</t>
+        </is>
+      </c>
+      <c r="J3" s="30" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="L3" s="30" t="inlineStr">
+        <is>
+          <t>Principal Payment</t>
+        </is>
+      </c>
+      <c r="M3" s="117" t="inlineStr">
+        <is>
+          <t>10,000.00</t>
+        </is>
+      </c>
+      <c r="N3" s="108" t="n">
+        <v>100</v>
+      </c>
+      <c r="O3" s="30" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/BP_CML</t>
         </is>
@@ -23869,8 +25149,8 @@
   </sheetPr>
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -24006,12 +25286,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_18092020164920</t>
+          <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM18092020165749</t>
+          <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -24088,6 +25368,106 @@
         </is>
       </c>
       <c r="T2" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM12102019171714</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_20092020200120</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020200906</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>60000242</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>08-Feb-2019</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>FIXED Interest Due</t>
+        </is>
+      </c>
+      <c r="H3" s="30" t="inlineStr">
+        <is>
+          <t>ESPS11810226</t>
+        </is>
+      </c>
+      <c r="I3" s="30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J3" s="30" t="inlineStr">
+        <is>
+          <t>Projected Due</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>8.77</t>
+        </is>
+      </c>
+      <c r="L3" s="30" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="M3" s="30" t="inlineStr">
+        <is>
+          <t>Payments</t>
+        </is>
+      </c>
+      <c r="N3" s="30" t="inlineStr">
+        <is>
+          <t>Awaiting Approval</t>
+        </is>
+      </c>
+      <c r="O3" s="30" t="inlineStr">
+        <is>
+          <t>Interest Payment</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="Q3" s="30" t="inlineStr">
+        <is>
+          <t>RTGSAUD1-0736</t>
+        </is>
+      </c>
+      <c r="R3" s="108" t="n">
+        <v>100</v>
+      </c>
+      <c r="S3" s="30" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
         <is>
           <t>CSSC7_TERM12102019171714</t>
         </is>
@@ -24116,7 +25496,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -24336,7 +25716,7 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_18092020164920</t>
+          <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
       <c r="H2" s="30" t="inlineStr">
@@ -24376,12 +25756,12 @@
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM18092020165749</t>
+          <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_18092020164920</t>
+          <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
       <c r="Q2" s="30" t="inlineStr">
@@ -24448,12 +25828,150 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" s="49" t="n"/>
-      <c r="E3" s="40" t="n"/>
-      <c r="F3" s="40" t="n"/>
-      <c r="Z3" s="74" t="n"/>
-      <c r="AA3" s="74" t="n"/>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="151" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="45" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>09-Jan-2019</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>10-Mar-2019</t>
+        </is>
+      </c>
+      <c r="E3" s="40" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="F3" s="40" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_20092020200120</t>
+        </is>
+      </c>
+      <c r="H3" s="30" t="inlineStr">
+        <is>
+          <t>RTGSAUD1-0736</t>
+        </is>
+      </c>
+      <c r="I3" s="30" t="inlineStr">
+        <is>
+          <t>06000505</t>
+        </is>
+      </c>
+      <c r="J3" s="30" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="K3" s="30" t="inlineStr">
+        <is>
+          <t>DOIT</t>
+        </is>
+      </c>
+      <c r="L3" s="30" t="inlineStr">
+        <is>
+          <t>ESPS11810226</t>
+        </is>
+      </c>
+      <c r="M3" s="30" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+      <c r="N3" s="30" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM20092020200906</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_20092020200120</t>
+        </is>
+      </c>
+      <c r="Q3" s="30" t="inlineStr">
+        <is>
+          <t>ONG000000000213</t>
+        </is>
+      </c>
+      <c r="R3" s="30" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="S3" s="30" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="T3" s="30" t="inlineStr">
+        <is>
+          <t>UNUT Fee Due</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>01-Feb-2019</t>
+        </is>
+      </c>
+      <c r="V3" s="30" t="inlineStr">
+        <is>
+          <t>04-Jun-2018</t>
+        </is>
+      </c>
+      <c r="W3" s="30" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="X3" s="30" t="n">
+        <v>9.859999999999999</v>
+      </c>
+      <c r="Z3" s="74" t="inlineStr">
+        <is>
+          <t>90,000.00</t>
+        </is>
+      </c>
+      <c r="AA3" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="AB3" s="30" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="AC3" s="30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD3" s="1" t="inlineStr">
+        <is>
+          <t>08-Feb-2019</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="U4" s="48" t="n"/>

</xml_diff>

<commit_message>
GDE-7340 Test Case for SBLC V2 Fees Cycle Dates Single Accrual
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3196,7 +3196,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC3_14092020211728</t>
+          <t>COMSEE_SC3_22092020152332</t>
         </is>
       </c>
       <c r="F3" s="38" t="inlineStr">
@@ -3464,7 +3464,7 @@
       </c>
       <c r="BI3" s="1" t="inlineStr">
         <is>
-          <t>16-Oct-2021</t>
+          <t>27-Nov-2021</t>
         </is>
       </c>
       <c r="BJ3" s="41" t="inlineStr">
@@ -3777,12 +3777,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC3_14092020211728</t>
+          <t>COMSEE_SC3_22092020152332</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>COMSEEFACBG_14092020212610</t>
+          <t>COMSEEFACBG_22092020153120</t>
         </is>
       </c>
       <c r="E3" s="30" t="inlineStr">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>3000671</t>
+          <t>3000735</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>60000787</t>
+          <t>60000956</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
@@ -4765,24 +4765,32 @@
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-20</t>
+          <t>2020-11-27</t>
         </is>
       </c>
       <c r="O3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-26</t>
+          <t>2020-12-03</t>
         </is>
       </c>
       <c r="P3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-20</t>
-        </is>
-      </c>
-      <c r="Q3" s="1" t="n"/>
-      <c r="R3" s="1" t="n"/>
+          <t>2020-11-27</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="inlineStr">
+        <is>
+          <t>2020-11-27</t>
+        </is>
+      </c>
+      <c r="R3" s="1" t="inlineStr">
+        <is>
+          <t>2020-12-03</t>
+        </is>
+      </c>
       <c r="S3" s="1" t="inlineStr">
         <is>
-          <t>4.51</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="T3" s="1" t="inlineStr">
@@ -4802,7 +4810,7 @@
       </c>
       <c r="X3" s="1" t="inlineStr">
         <is>
-          <t>2020-10-16</t>
+          <t>2020-11-27</t>
         </is>
       </c>
       <c r="Y3" s="1" t="inlineStr">
@@ -4817,7 +4825,7 @@
       </c>
       <c r="AA3" s="1" t="inlineStr">
         <is>
-          <t>2021-10-18</t>
+          <t>2021-11-29</t>
         </is>
       </c>
       <c r="AB3" s="38" t="inlineStr">
@@ -4844,7 +4852,7 @@
       <c r="AG3" s="79" t="n"/>
       <c r="AN3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC3_14092020211728</t>
+          <t>COMSEE_SC3_22092020152332</t>
         </is>
       </c>
       <c r="AO3" s="40" t="inlineStr">
@@ -4854,7 +4862,7 @@
       </c>
       <c r="AP3" s="1" t="inlineStr">
         <is>
-          <t>COMSEEFACBG_14092020212610</t>
+          <t>COMSEEFACBG_22092020153120</t>
         </is>
       </c>
       <c r="AQ3" s="40" t="inlineStr">
@@ -4882,7 +4890,7 @@
       </c>
       <c r="AV3" s="1" t="inlineStr">
         <is>
-          <t>16-Oct-2021</t>
+          <t>27-Nov-2021</t>
         </is>
       </c>
       <c r="AW3" s="30" t="inlineStr">
@@ -5790,7 +5798,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>3000671</t>
+          <t>3000735</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -5805,7 +5813,7 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>60000787</t>
+          <t>60000956</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
@@ -5852,7 +5860,7 @@
       </c>
       <c r="U3" s="1" t="inlineStr">
         <is>
-          <t>60000787</t>
+          <t>60000956</t>
         </is>
       </c>
       <c r="V3" s="1" t="inlineStr">
@@ -5907,12 +5915,12 @@
       </c>
       <c r="AN3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC3_14092020211728</t>
+          <t>COMSEE_SC3_22092020152332</t>
         </is>
       </c>
       <c r="AO3" s="1" t="inlineStr">
         <is>
-          <t>COMSEEFACBG_14092020212610</t>
+          <t>COMSEEFACBG_22092020153120</t>
         </is>
       </c>
       <c r="AP3" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-7344 Script Updates for Zero Cycle Due with Single Line Accrual due to Paid Cycle Due
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="16" activeTab="17" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="35" activeTab="37" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -4795,7 +4795,7 @@
       </c>
       <c r="T3" s="1" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>10.96</t>
         </is>
       </c>
       <c r="V3" s="1" t="inlineStr">
@@ -4929,7 +4929,6 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
     <row r="5">
       <c r="AU5" s="49" t="n"/>
     </row>
@@ -4948,7 +4947,7 @@
   </sheetPr>
   <dimension ref="A1:ES3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q1" sqref="Q1:R1"/>
     </sheetView>
@@ -20985,8 +20984,8 @@
   <dimension ref="A1:DC3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+      <pane xSplit="2" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -22153,7 +22152,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>3000734</t>
+          <t>3000745</t>
         </is>
       </c>
       <c r="D3" s="45" t="inlineStr">
@@ -22178,17 +22177,17 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_20092020200120</t>
+          <t>COMSEE_SC7_24092020204527</t>
         </is>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>1000866</t>
+          <t>1000884</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-26</t>
+          <t>2020-12-31</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
@@ -22272,7 +22271,7 @@
       </c>
       <c r="AB3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM20092020200906</t>
+          <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
       <c r="AC3" s="38" t="inlineStr">
@@ -22469,7 +22468,7 @@
       </c>
       <c r="BQ3" s="1" t="inlineStr">
         <is>
-          <t>26-Nov-2021</t>
+          <t>31-Dec-2021</t>
         </is>
       </c>
       <c r="BR3" s="30" t="inlineStr">
@@ -23212,22 +23211,22 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM20092020200906</t>
+          <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>3000734</t>
+          <t>3000745</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-26</t>
+          <t>2020-12-31</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>2021-12-26</t>
+          <t>2022-01-30</t>
         </is>
       </c>
       <c r="G3" s="30" t="inlineStr">
@@ -23339,7 +23338,7 @@
       </c>
       <c r="AD3" s="1" t="inlineStr">
         <is>
-          <t>2021-11-26</t>
+          <t>2021-12-31</t>
         </is>
       </c>
       <c r="AE3" s="3" t="inlineStr">
@@ -23349,7 +23348,7 @@
       </c>
       <c r="AF3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_20092020200120</t>
+          <t>COMSEE_SC7_24092020204527</t>
         </is>
       </c>
       <c r="AG3" s="30" t="inlineStr">
@@ -23462,7 +23461,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:R1"/>
+      <selection pane="bottomRight" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -23917,7 +23916,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>3000734</t>
+          <t>3000745</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -23932,12 +23931,12 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM20092020200906</t>
+          <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000444</t>
+          <t>ONG000000000468</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
@@ -23962,27 +23961,27 @@
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-26</t>
+          <t>2020-12-31</t>
         </is>
       </c>
       <c r="O3" s="1" t="inlineStr">
         <is>
-          <t>2021-12-26</t>
+          <t>2022-01-30</t>
         </is>
       </c>
       <c r="P3" s="1" t="inlineStr">
         <is>
-          <t>2021-02-26</t>
+          <t>2021-01-07</t>
         </is>
       </c>
       <c r="Q3" s="1" t="inlineStr">
         <is>
-          <t>2020-11-26</t>
+          <t>2020-12-31</t>
         </is>
       </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
-          <t>2021-02-25</t>
+          <t>2021-01-06</t>
         </is>
       </c>
       <c r="S3" s="1" t="inlineStr">
@@ -23992,12 +23991,12 @@
       </c>
       <c r="T3" s="1" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>10.96</t>
         </is>
       </c>
       <c r="U3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM20092020200906</t>
+          <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
       <c r="V3" s="47" t="inlineStr">
@@ -24112,7 +24111,7 @@
   <dimension ref="A1:AN3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -24565,7 +24564,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_20092020200120</t>
+          <t>COMSEE_SC7_24092020204527</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -24575,7 +24574,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM20092020200906</t>
+          <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -24640,7 +24639,7 @@
       </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
-          <t>26-Dec-2021</t>
+          <t>30-Jan-2022</t>
         </is>
       </c>
       <c r="S3" s="2" t="inlineStr">
@@ -25080,12 +25079,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_20092020200120</t>
+          <t>COMSEE_SC7_24092020204527</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM20092020200906</t>
+          <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
       <c r="E3" s="30" t="inlineStr">
@@ -25394,12 +25393,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_20092020200120</t>
+          <t>COMSEE_SC7_24092020204527</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM20092020200906</t>
+          <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -25502,9 +25501,9 @@
   </sheetPr>
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:AD3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -25849,12 +25848,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>09-Jan-2019</t>
+          <t>08-Dec-2020</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>10-Mar-2019</t>
+          <t>06-Feb-2021</t>
         </is>
       </c>
       <c r="E3" s="40" t="inlineStr">
@@ -25869,12 +25868,12 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_20092020200120</t>
-        </is>
-      </c>
-      <c r="H3" s="30" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-0736</t>
+          <t>COMSEE_SC7_24092020204527</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>RTGS1</t>
         </is>
       </c>
       <c r="I3" s="30" t="inlineStr">
@@ -25892,14 +25891,14 @@
           <t>DOIT</t>
         </is>
       </c>
-      <c r="L3" s="30" t="inlineStr">
-        <is>
-          <t>ESPS11810226</t>
-        </is>
-      </c>
-      <c r="M3" s="30" t="inlineStr">
-        <is>
-          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_COL</t>
         </is>
       </c>
       <c r="N3" s="30" t="inlineStr">
@@ -25909,12 +25908,12 @@
       </c>
       <c r="O3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM20092020200906</t>
+          <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
       <c r="P3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_20092020200120</t>
+          <t>COMSEE_SC7_24092020204527</t>
         </is>
       </c>
       <c r="Q3" s="30" t="inlineStr">
@@ -25922,24 +25921,24 @@
           <t>ONG000000000213</t>
         </is>
       </c>
-      <c r="R3" s="30" t="inlineStr">
-        <is>
-          <t>Commitment Fee</t>
-        </is>
-      </c>
-      <c r="S3" s="30" t="inlineStr">
-        <is>
-          <t>Commitment Fee</t>
-        </is>
-      </c>
-      <c r="T3" s="30" t="inlineStr">
-        <is>
-          <t>UNUT Fee Due</t>
+      <c r="R3" s="1" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>FACI Fee Due</t>
         </is>
       </c>
       <c r="U3" s="1" t="inlineStr">
         <is>
-          <t>01-Feb-2019</t>
+          <t>01-Jan-2021</t>
         </is>
       </c>
       <c r="V3" s="30" t="inlineStr">
@@ -25977,7 +25976,7 @@
       </c>
       <c r="AD3" s="1" t="inlineStr">
         <is>
-          <t>08-Feb-2019</t>
+          <t>07-Jan-2021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-7341 Test Case for Cycle Dates for V2 Fees with Multiple Accrual
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="35" activeTab="37" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="30" activeTab="33" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -366,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -623,6 +623,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20984,8 +20987,8 @@
   <dimension ref="A1:DC3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD3" sqref="AD3"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:DB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -22152,7 +22155,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>3000745</t>
+          <t>3000734</t>
         </is>
       </c>
       <c r="D3" s="45" t="inlineStr">
@@ -22177,17 +22180,17 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_24092020204527</t>
+          <t>COMSEE_SC7_20092020200120</t>
         </is>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>1000884</t>
+          <t>1000866</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-11-26</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
@@ -22254,24 +22257,24 @@
           <t>Global</t>
         </is>
       </c>
-      <c r="Y3" s="3" t="inlineStr">
+      <c r="Y3" s="152" t="inlineStr">
         <is>
           <t>COMSEE_SC7_</t>
         </is>
       </c>
-      <c r="Z3" s="3" t="inlineStr">
+      <c r="Z3" s="152" t="inlineStr">
         <is>
           <t>CS7</t>
         </is>
       </c>
-      <c r="AA3" s="30" t="inlineStr">
+      <c r="AA3" s="1" t="inlineStr">
         <is>
           <t>S724062019190029CNO</t>
         </is>
       </c>
       <c r="AB3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM24092020205243</t>
+          <t>CSSC7_TERM20092020200906</t>
         </is>
       </c>
       <c r="AC3" s="38" t="inlineStr">
@@ -22284,7 +22287,7 @@
           <t>BORROWER1111</t>
         </is>
       </c>
-      <c r="AE3" s="30" t="inlineStr">
+      <c r="AE3" s="1" t="inlineStr">
         <is>
           <t>Melbourne, VIC,Australia</t>
         </is>
@@ -22374,12 +22377,12 @@
           <t>Start of current cycle</t>
         </is>
       </c>
-      <c r="AW3" s="30" t="inlineStr">
+      <c r="AW3" s="1" t="inlineStr">
         <is>
           <t>Start of next interest cycle</t>
         </is>
       </c>
-      <c r="AX3" s="30" t="n">
+      <c r="AX3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AY3" s="38" t="inlineStr">
@@ -22397,10 +22400,10 @@
           <t>Next Business Day</t>
         </is>
       </c>
-      <c r="BB3" s="30" t="n">
+      <c r="BB3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="BC3" s="30" t="inlineStr">
+      <c r="BC3" s="1" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
@@ -22420,18 +22423,18 @@
           <t>IT_COL</t>
         </is>
       </c>
-      <c r="BG3" s="30" t="inlineStr">
+      <c r="BG3" s="1" t="inlineStr">
         <is>
           <t>Origination</t>
         </is>
       </c>
-      <c r="BH3" s="30" t="n">
+      <c r="BH3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="BI3" s="30" t="n">
+      <c r="BI3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="BJ3" s="30" t="inlineStr">
+      <c r="BJ3" s="1" t="inlineStr">
         <is>
           <t>Add Comment</t>
         </is>
@@ -22441,7 +22444,7 @@
           <t>Business Verification,${SPACE}${SPACE}BVT</t>
         </is>
       </c>
-      <c r="BL3" s="30" t="inlineStr">
+      <c r="BL3" s="1" t="inlineStr">
         <is>
           <t>LENDING</t>
         </is>
@@ -22468,14 +22471,15 @@
       </c>
       <c r="BQ3" s="1" t="inlineStr">
         <is>
-          <t>31-Dec-2021</t>
-        </is>
-      </c>
-      <c r="BR3" s="30" t="inlineStr">
+          <t>26-Nov-2021</t>
+        </is>
+      </c>
+      <c r="BR3" s="1" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
+      <c r="BS3" s="1" t="n"/>
       <c r="BT3" s="41" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia -DBU</t>
@@ -22546,12 +22550,12 @@
           <t>password1</t>
         </is>
       </c>
-      <c r="CH3" s="30" t="inlineStr">
+      <c r="CH3" s="1" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="CI3" s="30" t="inlineStr">
+      <c r="CI3" s="1" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
@@ -22611,18 +22615,18 @@
           <t>IMT</t>
         </is>
       </c>
-      <c r="CU3" s="30" t="inlineStr">
+      <c r="CU3" s="1" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="CV3" s="30" t="inlineStr">
+      <c r="CV3" s="1" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="CW3" s="3" t="n"/>
-      <c r="CX3" s="30" t="inlineStr">
+      <c r="CW3" s="152" t="n"/>
+      <c r="CX3" s="1" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
@@ -22664,10 +22668,10 @@
   <dimension ref="A1:AY3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -23211,25 +23215,25 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM24092020205243</t>
+          <t>CSSC7_TERM20092020200906</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>3000745</t>
+          <t>3000734</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-11-26</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>2022-01-30</t>
-        </is>
-      </c>
-      <c r="G3" s="30" t="inlineStr">
+          <t>2021-12-26</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
@@ -23237,7 +23241,7 @@
       <c r="H3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="30" t="inlineStr">
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>Term</t>
         </is>
@@ -23338,20 +23342,20 @@
       </c>
       <c r="AD3" s="1" t="inlineStr">
         <is>
-          <t>2021-12-31</t>
-        </is>
-      </c>
-      <c r="AE3" s="3" t="inlineStr">
+          <t>2021-11-26</t>
+        </is>
+      </c>
+      <c r="AE3" s="152" t="inlineStr">
         <is>
           <t>CSSC7_TERM</t>
         </is>
       </c>
       <c r="AF3" s="1" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_24092020204527</t>
-        </is>
-      </c>
-      <c r="AG3" s="30" t="inlineStr">
+          <t>COMSEE_SC7_20092020200120</t>
+        </is>
+      </c>
+      <c r="AG3" s="1" t="inlineStr">
         <is>
           <t>S124062019191047FMB</t>
         </is>
@@ -23366,17 +23370,18 @@
           <t>100,000.00</t>
         </is>
       </c>
-      <c r="AK3" s="30" t="inlineStr">
+      <c r="AJ3" s="1" t="n"/>
+      <c r="AK3" s="1" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="AL3" s="30" t="inlineStr">
+      <c r="AL3" s="1" t="inlineStr">
         <is>
           <t>16-Aug-2019</t>
         </is>
       </c>
-      <c r="AM3" s="30" t="inlineStr">
+      <c r="AM3" s="1" t="inlineStr">
         <is>
           <t>15-Sep-2019</t>
         </is>
@@ -23406,17 +23411,17 @@
           <t>Acquisitions</t>
         </is>
       </c>
-      <c r="AS3" s="30" t="inlineStr">
+      <c r="AS3" s="1" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AT3" s="30" t="inlineStr">
+      <c r="AT3" s="1" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia</t>
         </is>
       </c>
-      <c r="AU3" s="30" t="inlineStr">
+      <c r="AU3" s="1" t="inlineStr">
         <is>
           <t>Sydney, NSW,Australia</t>
         </is>
@@ -23426,17 +23431,17 @@
           <t>BORROWER1111</t>
         </is>
       </c>
-      <c r="AW3" s="30" t="inlineStr">
+      <c r="AW3" s="1" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AX3" s="30" t="inlineStr">
+      <c r="AX3" s="1" t="inlineStr">
         <is>
           <t>BLOGGS</t>
         </is>
       </c>
-      <c r="AY3" s="48" t="inlineStr">
+      <c r="AY3" s="153" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
@@ -23457,11 +23462,11 @@
   </sheetPr>
   <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="Q3" sqref="Q3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3:AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -23916,7 +23921,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>3000745</t>
+          <t>3000734</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -23931,12 +23936,12 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM24092020205243</t>
+          <t>CSSC7_TERM20092020200906</t>
         </is>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000468</t>
+          <t>ONG000000000444</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
@@ -23961,24 +23966,24 @@
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
+          <t>2020-11-26</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>2021-12-26</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>2021-01-07</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="inlineStr">
+        <is>
           <t>2020-12-31</t>
         </is>
       </c>
-      <c r="O3" s="1" t="inlineStr">
-        <is>
-          <t>2022-01-30</t>
-        </is>
-      </c>
-      <c r="P3" s="1" t="inlineStr">
-        <is>
-          <t>2021-01-07</t>
-        </is>
-      </c>
-      <c r="Q3" s="1" t="inlineStr">
-        <is>
-          <t>2020-12-31</t>
-        </is>
-      </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
           <t>2021-01-06</t>
@@ -23986,17 +23991,17 @@
       </c>
       <c r="S3" s="1" t="inlineStr">
         <is>
-          <t>10.96</t>
+          <t>438.34</t>
         </is>
       </c>
       <c r="T3" s="1" t="inlineStr">
         <is>
-          <t>10.96</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="U3" s="1" t="inlineStr">
         <is>
-          <t>CSSC7_TERM24092020205243</t>
+          <t>CSSC7_TERM20092020200906</t>
         </is>
       </c>
       <c r="V3" s="47" t="inlineStr">
@@ -24044,7 +24049,7 @@
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AE3" s="30" t="inlineStr">
+      <c r="AE3" s="1" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
@@ -24054,7 +24059,7 @@
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AG3" s="53" t="inlineStr">
+      <c r="AG3" s="154" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
@@ -24069,22 +24074,22 @@
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AJ3" s="30" t="inlineStr">
+      <c r="AJ3" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AK3" s="30" t="inlineStr">
+      <c r="AK3" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AL3" s="30" t="inlineStr">
+      <c r="AL3" s="1" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="AM3" s="30" t="inlineStr">
+      <c r="AM3" s="1" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
@@ -25501,7 +25506,7 @@
   </sheetPr>
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>

</xml_diff>

<commit_message>
GDE-7403 CommSee V1 Outstanding for Fixed Rate Loans
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="35" activeTab="37" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="29" activeTab="34" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -186,11 +186,6 @@
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <sz val="8"/>
     </font>
   </fonts>
   <fills count="14">
@@ -389,7 +384,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -670,6 +665,10 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1987,8 +1986,8 @@
   </sheetPr>
   <dimension ref="A1:BF15"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:BE4"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -7618,8 +7617,8 @@
   <dimension ref="A1:DB5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CC2" sqref="CC2"/>
+      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -22559,11 +22558,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DC5"/>
+  <dimension ref="A1:DC6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN18" sqref="AN18"/>
+      <pane xSplit="2" topLeftCell="AW1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BC6" sqref="BC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -25247,6 +25246,515 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C6" s="159" t="inlineStr">
+        <is>
+          <t>3000848</t>
+        </is>
+      </c>
+      <c r="D6" s="165" t="inlineStr">
+        <is>
+          <t>rodel</t>
+        </is>
+      </c>
+      <c r="E6" s="141" t="inlineStr">
+        <is>
+          <t>\DataSet\API_DataSet\Input\ComSee\</t>
+        </is>
+      </c>
+      <c r="F6" s="141" t="inlineStr">
+        <is>
+          <t>COM_RES_07</t>
+        </is>
+      </c>
+      <c r="G6" s="159" t="inlineStr">
+        <is>
+          <t>2019-10-12</t>
+        </is>
+      </c>
+      <c r="H6" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="I6" s="159" t="inlineStr">
+        <is>
+          <t>1001040</t>
+        </is>
+      </c>
+      <c r="J6" s="159" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="K6" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="L6" s="165" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="M6" s="159" t="inlineStr">
+        <is>
+          <t>AUSNA</t>
+        </is>
+      </c>
+      <c r="N6" s="159" t="inlineStr">
+        <is>
+          <t>Non-Agency Australia</t>
+        </is>
+      </c>
+      <c r="O6" s="149" t="inlineStr">
+        <is>
+          <t>BP_CML</t>
+        </is>
+      </c>
+      <c r="P6" s="159" t="inlineStr">
+        <is>
+          <t>Commercial Lending</t>
+        </is>
+      </c>
+      <c r="Q6" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="U6" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="V6" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="W6" s="159" t="inlineStr">
+        <is>
+          <t>GLB</t>
+        </is>
+      </c>
+      <c r="X6" s="149" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="Y6" s="109" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_</t>
+        </is>
+      </c>
+      <c r="Z6" s="109" t="inlineStr">
+        <is>
+          <t>CS7</t>
+        </is>
+      </c>
+      <c r="AA6" s="26" t="inlineStr">
+        <is>
+          <t>S724062019190029CNO</t>
+        </is>
+      </c>
+      <c r="AB6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="AC6" s="149" t="inlineStr">
+        <is>
+          <t>Sales Group 1</t>
+        </is>
+      </c>
+      <c r="AD6" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="AE6" s="26" t="inlineStr">
+        <is>
+          <t>Melbourne, VIC,Australia</t>
+        </is>
+      </c>
+      <c r="AF6" s="149" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="AG6" s="149" t="inlineStr">
+        <is>
+          <t>GCP</t>
+        </is>
+      </c>
+      <c r="AH6" s="149" t="inlineStr">
+        <is>
+          <t>General Corp Purpose</t>
+        </is>
+      </c>
+      <c r="AI6" s="149" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="AJ6" s="149" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="AK6" s="149" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AL6" s="149" t="inlineStr">
+        <is>
+          <t>Lending,${SPACE}${SPACE}Operations</t>
+        </is>
+      </c>
+      <c r="AM6" s="149" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AN6" s="149" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="AO6" s="149" t="inlineStr">
+        <is>
+          <t>10,000,000.00</t>
+        </is>
+      </c>
+      <c r="AP6" s="149" t="inlineStr">
+        <is>
+          <t>Sydney, Australia</t>
+        </is>
+      </c>
+      <c r="AQ6" s="148" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AR6" s="149" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AS6" s="149" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AT6" s="149" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AU6" s="149" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AV6" s="149" t="inlineStr">
+        <is>
+          <t>Start of current cycle</t>
+        </is>
+      </c>
+      <c r="AW6" s="26" t="inlineStr">
+        <is>
+          <t>Start of next interest cycle</t>
+        </is>
+      </c>
+      <c r="AX6" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY6" s="149" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="AZ6" s="149" t="inlineStr">
+        <is>
+          <t>Effective date of change</t>
+        </is>
+      </c>
+      <c r="BA6" s="149" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="BB6" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC6" s="26" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="BD6" s="149" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="BE6" s="149" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="BF6" s="149" t="inlineStr">
+        <is>
+          <t>IT_COL</t>
+        </is>
+      </c>
+      <c r="BG6" s="26" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="BH6" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="BI6" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="BJ6" s="26" t="inlineStr">
+        <is>
+          <t>Add Comment</t>
+        </is>
+      </c>
+      <c r="BK6" s="149" t="inlineStr">
+        <is>
+          <t>Business Verification,${SPACE}${SPACE}BVT</t>
+        </is>
+      </c>
+      <c r="BL6" s="26" t="inlineStr">
+        <is>
+          <t>LENDING</t>
+        </is>
+      </c>
+      <c r="BM6" s="149" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="BN6" s="149" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="BO6" s="149" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="BP6" s="149" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="BQ6" s="159" t="inlineStr">
+        <is>
+          <t>28-Jan-2022</t>
+        </is>
+      </c>
+      <c r="BR6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="BT6" s="143" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia -DBU</t>
+        </is>
+      </c>
+      <c r="BU6" s="143" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="BV6" s="143" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BW6" s="143" t="inlineStr">
+        <is>
+          <t>ZOE</t>
+        </is>
+      </c>
+      <c r="BX6" s="143" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="BY6" s="143" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="BZ6" s="143" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+      <c r="CA6" s="143" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank Australia - DBU</t>
+        </is>
+      </c>
+      <c r="CB6" s="69" t="inlineStr">
+        <is>
+          <t>FJAPR01</t>
+        </is>
+      </c>
+      <c r="CC6" s="1" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CD6" s="69" t="inlineStr">
+        <is>
+          <t>FJUSR01</t>
+        </is>
+      </c>
+      <c r="CE6" s="1" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CF6" s="69" t="inlineStr">
+        <is>
+          <t>FJMGR01</t>
+        </is>
+      </c>
+      <c r="CG6" s="69" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CH6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CI6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CJ6" s="143" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH% DBU</t>
+        </is>
+      </c>
+      <c r="CK6" s="143" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK OF AUSTRALIA - DBU</t>
+        </is>
+      </c>
+      <c r="CL6" s="143" t="inlineStr">
+        <is>
+          <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
+        </is>
+      </c>
+      <c r="CM6" s="143" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="CN6" s="143" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="CO6" s="143" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="CP6" s="143" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="CQ6" s="143" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="CR6" s="143" t="inlineStr">
+        <is>
+          <t>BLOGGS</t>
+        </is>
+      </c>
+      <c r="CS6" s="143" t="inlineStr">
+        <is>
+          <t>Bloggs,  John</t>
+        </is>
+      </c>
+      <c r="CT6" s="143" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="CU6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CV6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CW6" s="109" t="n"/>
+      <c r="CX6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CY6" s="143" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="CZ6" s="143" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="DA6" s="143" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="DB6" s="143" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK AUST -DBU</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -25260,13 +25768,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY5"/>
+  <dimension ref="A1:AY6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -26532,6 +27040,250 @@
         </is>
       </c>
     </row>
+    <row r="6" ht="15" customHeight="1" s="157">
+      <c r="A6" s="108" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="D6" s="159" t="inlineStr">
+        <is>
+          <t>3000848</t>
+        </is>
+      </c>
+      <c r="E6" s="159" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="F6" s="159" t="inlineStr">
+        <is>
+          <t>2022-02-27</t>
+        </is>
+      </c>
+      <c r="G6" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="H6" s="159" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="26" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="J6" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="K6" s="159" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="L6" s="159" t="inlineStr">
+        <is>
+          <t>90000.00</t>
+        </is>
+      </c>
+      <c r="M6" s="159" t="inlineStr">
+        <is>
+          <t>IT_COL|Corporate Lending</t>
+        </is>
+      </c>
+      <c r="N6" s="159" t="inlineStr">
+        <is>
+          <t>AUSNA</t>
+        </is>
+      </c>
+      <c r="O6" s="159" t="inlineStr">
+        <is>
+          <t>Non-Agency Australia</t>
+        </is>
+      </c>
+      <c r="P6" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="T6" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="U6" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="V6" s="159" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="W6" s="159" t="inlineStr">
+        <is>
+          <t>90000.00</t>
+        </is>
+      </c>
+      <c r="X6" s="159" t="inlineStr">
+        <is>
+          <t>HFIAU</t>
+        </is>
+      </c>
+      <c r="Y6" s="159" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="Z6" s="159" t="inlineStr">
+        <is>
+          <t>CB001</t>
+        </is>
+      </c>
+      <c r="AA6" s="159" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="AB6" s="159" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AC6" s="159" t="inlineStr">
+        <is>
+          <t>Australian (Sydney)</t>
+        </is>
+      </c>
+      <c r="AD6" s="159" t="inlineStr">
+        <is>
+          <t>2022-01-28</t>
+        </is>
+      </c>
+      <c r="AE6" s="109" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM</t>
+        </is>
+      </c>
+      <c r="AF6" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="AG6" s="26" t="inlineStr">
+        <is>
+          <t>S124062019191047FMB</t>
+        </is>
+      </c>
+      <c r="AH6" s="150" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AI6" s="150" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="AK6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="AL6" s="26" t="inlineStr">
+        <is>
+          <t>16-Aug-2019</t>
+        </is>
+      </c>
+      <c r="AM6" s="26" t="inlineStr">
+        <is>
+          <t>15-Sep-2019</t>
+        </is>
+      </c>
+      <c r="AN6" s="149" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AO6" s="149" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="AP6" s="150" t="inlineStr">
+        <is>
+          <t>Fixed Rate Loan</t>
+        </is>
+      </c>
+      <c r="AQ6" s="150" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AR6" s="150" t="inlineStr">
+        <is>
+          <t>Acquisitions</t>
+        </is>
+      </c>
+      <c r="AS6" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AT6" s="26" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia</t>
+        </is>
+      </c>
+      <c r="AU6" s="26" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="AV6" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="AW6" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AX6" s="26" t="inlineStr">
+        <is>
+          <t>BLOGGS</t>
+        </is>
+      </c>
+      <c r="AY6" s="35" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -26545,13 +27297,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN5"/>
+  <dimension ref="A1:AN6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -27589,6 +28341,208 @@
         </is>
       </c>
     </row>
+    <row r="6" ht="15" customHeight="1" s="157">
+      <c r="A6" s="108" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C6" s="140" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D6" s="140" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V1</t>
+        </is>
+      </c>
+      <c r="E6" s="159" t="inlineStr">
+        <is>
+          <t>3000848</t>
+        </is>
+      </c>
+      <c r="F6" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G6" s="159" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="H6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="I6" s="159" t="inlineStr">
+        <is>
+          <t>ONG000000000604</t>
+        </is>
+      </c>
+      <c r="J6" s="159" t="inlineStr">
+        <is>
+          <t>Released</t>
+        </is>
+      </c>
+      <c r="K6" s="159" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="L6" s="159" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="M6" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="N6" s="159" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="O6" s="159" t="inlineStr">
+        <is>
+          <t>2022-02-27</t>
+        </is>
+      </c>
+      <c r="P6" s="159" t="inlineStr">
+        <is>
+          <t>2021-04-28</t>
+        </is>
+      </c>
+      <c r="Q6" s="159" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="R6" s="159" t="inlineStr">
+        <is>
+          <t>2021-04-27</t>
+        </is>
+      </c>
+      <c r="S6" s="159" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="T6" s="159" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="U6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="V6" s="150" t="inlineStr">
+        <is>
+          <t>Facility Ongoing Fee</t>
+        </is>
+      </c>
+      <c r="W6" s="150" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="X6" s="37" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="Y6" s="150" t="inlineStr">
+        <is>
+          <t>FormulaCategory</t>
+        </is>
+      </c>
+      <c r="Z6" s="150" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="AA6" s="150" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="AB6" s="150" t="inlineStr">
+        <is>
+          <t>4.000000</t>
+        </is>
+      </c>
+      <c r="AC6" s="149" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+      <c r="AD6" s="148" t="inlineStr">
+        <is>
+          <t>Basis Points</t>
+        </is>
+      </c>
+      <c r="AE6" s="26" t="inlineStr">
+        <is>
+          <t>Option</t>
+        </is>
+      </c>
+      <c r="AF6" s="150" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AG6" s="38" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="AH6" s="149" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+      <c r="AI6" s="148" t="inlineStr">
+        <is>
+          <t>Basis Points</t>
+        </is>
+      </c>
+      <c r="AJ6" s="26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AK6" s="26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AL6" s="26" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="AM6" s="26" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AN6" s="148" t="inlineStr">
+        <is>
+          <t>Pay In Arrears</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -27602,244 +28556,379 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN5"/>
+  <dimension ref="A1:BN6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="5.7109375" customWidth="1" style="1" min="1" max="1"/>
-    <col width="21.7109375" customWidth="1" style="1" min="2" max="2"/>
-    <col width="29.28515625" customWidth="1" style="1" min="3" max="3"/>
-    <col width="24" customWidth="1" style="1" min="4" max="4"/>
-    <col width="27.85546875" customWidth="1" style="1" min="5" max="5"/>
-    <col width="24" customWidth="1" style="1" min="6" max="6"/>
-    <col width="34.28515625" customWidth="1" style="1" min="7" max="8"/>
-    <col width="24" customWidth="1" style="1" min="9" max="10"/>
-    <col width="27.85546875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.28515625" customWidth="1" style="1" min="12" max="12"/>
-    <col width="18.42578125" customWidth="1" style="1" min="13" max="13"/>
-    <col width="18.5703125" customWidth="1" style="1" min="14" max="14"/>
-    <col width="22.5703125" customWidth="1" style="1" min="15" max="16"/>
-    <col width="16.7109375" customWidth="1" style="1" min="17" max="17"/>
-    <col width="18.140625" customWidth="1" style="1" min="18" max="18"/>
-    <col width="23" customWidth="1" style="1" min="19" max="20"/>
-    <col width="18.7109375" customWidth="1" style="1" min="21" max="21"/>
-    <col width="30.28515625" customWidth="1" style="1" min="22" max="22"/>
-    <col width="27.7109375" customWidth="1" style="1" min="23" max="23"/>
-    <col width="22.85546875" customWidth="1" style="1" min="24" max="24"/>
-    <col width="26.85546875" customWidth="1" style="1" min="25" max="25"/>
-    <col width="37.140625" customWidth="1" style="1" min="26" max="26"/>
-    <col width="25" customWidth="1" style="1" min="27" max="27"/>
-    <col width="19.85546875" customWidth="1" style="1" min="28" max="28"/>
-    <col width="32.7109375" customWidth="1" style="1" min="29" max="29"/>
-    <col width="34" customWidth="1" style="1" min="30" max="32"/>
-    <col width="31.85546875" customWidth="1" style="1" min="33" max="38"/>
-    <col width="40" customWidth="1" style="26" min="39" max="39"/>
-    <col width="14.7109375" customWidth="1" style="26" min="40" max="40"/>
+    <col width="21.7109375" customWidth="1" style="1" min="2" max="6"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
+    <col width="29.28515625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="24" customWidth="1" style="1" min="9" max="9"/>
+    <col width="27.85546875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="24" customWidth="1" style="1" min="11" max="11"/>
+    <col width="34.28515625" customWidth="1" style="1" min="12" max="13"/>
+    <col width="24" customWidth="1" style="1" min="14" max="16"/>
+    <col width="27.85546875" customWidth="1" style="1" min="17" max="17"/>
+    <col width="19.28515625" customWidth="1" style="1" min="18" max="19"/>
+    <col width="18.42578125" customWidth="1" style="1" min="20" max="21"/>
+    <col width="18.5703125" customWidth="1" style="1" min="22" max="23"/>
+    <col width="22.5703125" customWidth="1" style="1" min="24" max="24"/>
+    <col width="27.85546875" bestFit="1" customWidth="1" style="1" min="25" max="25"/>
+    <col width="27.85546875" customWidth="1" style="1" min="26" max="29"/>
+    <col width="22.5703125" customWidth="1" style="1" min="30" max="30"/>
+    <col width="16.7109375" customWidth="1" style="1" min="31" max="32"/>
+    <col width="18.140625" customWidth="1" style="1" min="33" max="36"/>
+    <col width="23" customWidth="1" style="1" min="37" max="38"/>
+    <col width="18.7109375" customWidth="1" style="1" min="39" max="39"/>
+    <col width="30.28515625" customWidth="1" style="1" min="40" max="40"/>
+    <col width="27.7109375" customWidth="1" style="1" min="41" max="41"/>
+    <col width="22.85546875" customWidth="1" style="1" min="42" max="42"/>
+    <col width="26.85546875" customWidth="1" style="1" min="43" max="43"/>
+    <col width="37.140625" customWidth="1" style="1" min="44" max="44"/>
+    <col width="25" customWidth="1" style="1" min="45" max="45"/>
+    <col width="19.85546875" customWidth="1" style="1" min="46" max="46"/>
+    <col width="32.7109375" customWidth="1" style="1" min="47" max="47"/>
+    <col width="34" customWidth="1" style="1" min="48" max="50"/>
+    <col width="31.85546875" customWidth="1" style="1" min="51" max="56"/>
+    <col width="40" customWidth="1" style="26" min="57" max="57"/>
+    <col width="14.7109375" customWidth="1" style="26" min="58" max="58"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="157" min="59" max="59"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="70" thickBot="1">
-      <c r="A1" s="71" t="inlineStr">
+      <c r="A1" s="167" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="72" t="inlineStr">
+      <c r="B1" s="166" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="71" t="inlineStr">
+      <c r="C1" s="168" t="inlineStr">
+        <is>
+          <t>OutputFilePath</t>
+        </is>
+      </c>
+      <c r="D1" s="169" t="inlineStr">
+        <is>
+          <t>ResponseJson</t>
+        </is>
+      </c>
+      <c r="E1" s="169" t="inlineStr">
+        <is>
+          <t>COM_ID</t>
+        </is>
+      </c>
+      <c r="F1" s="169" t="inlineStr">
+        <is>
+          <t>Customer_ExternalID</t>
+        </is>
+      </c>
+      <c r="G1" s="169" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="H1" s="71" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="71" t="inlineStr">
+      <c r="I1" s="71" t="inlineStr">
         <is>
           <t>Facility_Currency</t>
         </is>
       </c>
-      <c r="E1" s="71" t="inlineStr">
+      <c r="J1" s="71" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="F1" s="71" t="inlineStr">
+      <c r="K1" s="71" t="inlineStr">
         <is>
           <t>Facility_Spread</t>
         </is>
       </c>
-      <c r="G1" s="71" t="inlineStr">
+      <c r="L1" s="71" t="inlineStr">
         <is>
           <t>Facility_CurrentAvailToDraw</t>
         </is>
       </c>
-      <c r="H1" s="71" t="inlineStr">
+      <c r="M1" s="71" t="inlineStr">
         <is>
           <t>Facility_CurrentGlobalOutstandings</t>
         </is>
       </c>
-      <c r="I1" s="71" t="inlineStr">
+      <c r="N1" s="71" t="inlineStr">
         <is>
           <t>Borrower1_ShortName</t>
         </is>
       </c>
-      <c r="J1" s="71" t="inlineStr">
+      <c r="O1" s="71" t="inlineStr">
         <is>
           <t>Outstanding_Type</t>
         </is>
       </c>
-      <c r="K1" s="71" t="inlineStr">
+      <c r="P1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_RiskType</t>
+        </is>
+      </c>
+      <c r="Q1" s="71" t="inlineStr">
         <is>
           <t>Loan_FacilityName</t>
         </is>
       </c>
-      <c r="L1" s="71" t="inlineStr">
+      <c r="R1" s="71" t="inlineStr">
         <is>
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="M1" s="71" t="inlineStr">
+      <c r="S1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_Alias</t>
+        </is>
+      </c>
+      <c r="T1" s="71" t="inlineStr">
         <is>
           <t>Loan_PricingOption</t>
         </is>
       </c>
-      <c r="N1" s="71" t="inlineStr">
+      <c r="U1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_PricingOption</t>
+        </is>
+      </c>
+      <c r="V1" s="71" t="inlineStr">
         <is>
           <t>Loan_Currency</t>
         </is>
       </c>
-      <c r="O1" s="71" t="inlineStr">
+      <c r="W1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_Currency</t>
+        </is>
+      </c>
+      <c r="X1" s="71" t="inlineStr">
         <is>
           <t>Loan_RequestedAmount</t>
         </is>
       </c>
-      <c r="P1" s="71" t="inlineStr">
+      <c r="Y1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_HBGrossAmount</t>
+        </is>
+      </c>
+      <c r="Z1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_HBNetAmount</t>
+        </is>
+      </c>
+      <c r="AA1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_HBNetFacCCYAmount</t>
+        </is>
+      </c>
+      <c r="AB1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_GlobalOriginalAmount</t>
+        </is>
+      </c>
+      <c r="AC1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_GlobalCurrentAmount</t>
+        </is>
+      </c>
+      <c r="AD1" s="71" t="inlineStr">
         <is>
           <t>HostBankSharePct</t>
         </is>
       </c>
-      <c r="Q1" s="71" t="inlineStr">
+      <c r="AE1" s="71" t="inlineStr">
         <is>
           <t>Loan_EffectiveDate</t>
         </is>
       </c>
-      <c r="R1" s="71" t="inlineStr">
+      <c r="AF1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_EffectiveDate</t>
+        </is>
+      </c>
+      <c r="AG1" s="71" t="inlineStr">
         <is>
           <t>Loan_MaturityDate</t>
         </is>
       </c>
-      <c r="S1" s="71" t="inlineStr">
+      <c r="AH1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_MaturityExpiryDate</t>
+        </is>
+      </c>
+      <c r="AI1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_PaymentMode</t>
+        </is>
+      </c>
+      <c r="AJ1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_IntCycleFrequency</t>
+        </is>
+      </c>
+      <c r="AK1" s="71" t="inlineStr">
         <is>
           <t>Loan_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="T1" s="71" t="inlineStr">
+      <c r="AL1" s="71" t="inlineStr">
         <is>
           <t>Loan_Accrue</t>
         </is>
       </c>
-      <c r="U1" s="71" t="inlineStr">
+      <c r="AM1" s="71" t="inlineStr">
         <is>
           <t>Borrower_BaseRate</t>
         </is>
       </c>
-      <c r="V1" s="71" t="inlineStr">
+      <c r="AN1" s="71" t="inlineStr">
         <is>
           <t>Repayment_ScheduleFrequency</t>
         </is>
       </c>
-      <c r="W1" s="71" t="inlineStr">
+      <c r="AO1" s="71" t="inlineStr">
         <is>
           <t>Repayment_NumberOfCycles</t>
         </is>
       </c>
-      <c r="X1" s="71" t="inlineStr">
+      <c r="AP1" s="71" t="inlineStr">
         <is>
           <t>Repayment_TriggerDate</t>
         </is>
       </c>
-      <c r="Y1" s="71" t="inlineStr">
+      <c r="AQ1" s="71" t="inlineStr">
         <is>
           <t>Repayment_NonBusDayRule</t>
         </is>
       </c>
-      <c r="Z1" s="70" t="inlineStr">
+      <c r="AR1" s="70" t="inlineStr">
         <is>
           <t>WIP_TransactionType</t>
         </is>
       </c>
-      <c r="AA1" s="70" t="inlineStr">
+      <c r="AS1" s="70" t="inlineStr">
         <is>
           <t>WIP_AwaitingApprovalStatus</t>
         </is>
       </c>
-      <c r="AB1" s="70" t="inlineStr">
+      <c r="AT1" s="70" t="inlineStr">
         <is>
           <t>WIP_OutstandingType</t>
         </is>
       </c>
-      <c r="AC1" s="70" t="inlineStr">
+      <c r="AU1" s="70" t="inlineStr">
         <is>
           <t>WIP_AwaitingRateApprovalStatus</t>
         </is>
       </c>
-      <c r="AD1" s="70" t="inlineStr">
+      <c r="AV1" s="70" t="inlineStr">
         <is>
           <t>WIP_AwaitingReleaseCashflowsStatus</t>
         </is>
       </c>
-      <c r="AE1" s="70" t="inlineStr">
+      <c r="AW1" s="70" t="inlineStr">
         <is>
           <t>Borrower_Profile</t>
         </is>
       </c>
-      <c r="AF1" s="70" t="inlineStr">
+      <c r="AX1" s="70" t="inlineStr">
         <is>
           <t>LIQCustomer_ID</t>
         </is>
       </c>
-      <c r="AG1" s="70" t="inlineStr">
+      <c r="AY1" s="70" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
       </c>
-      <c r="AH1" s="70" t="inlineStr">
+      <c r="AZ1" s="70" t="inlineStr">
         <is>
           <t>Remittance_Status</t>
         </is>
       </c>
-      <c r="AI1" s="70" t="inlineStr">
+      <c r="BA1" s="70" t="inlineStr">
         <is>
           <t>Loan_Currency</t>
         </is>
       </c>
-      <c r="AJ1" s="70" t="inlineStr">
+      <c r="BB1" s="70" t="inlineStr">
         <is>
           <t>Remittance_Description</t>
         </is>
       </c>
-      <c r="AK1" s="70" t="inlineStr">
+      <c r="BC1" s="70" t="inlineStr">
         <is>
           <t>HostBank_GLAccount</t>
         </is>
       </c>
-      <c r="AL1" s="70" t="inlineStr">
+      <c r="BD1" s="70" t="inlineStr">
         <is>
           <t>Borrower_GLAccount</t>
         </is>
       </c>
-      <c r="AM1" s="118" t="inlineStr">
+      <c r="BE1" s="118" t="inlineStr">
         <is>
           <t>Host_Bank</t>
         </is>
       </c>
-      <c r="AN1" s="118" t="inlineStr">
+      <c r="BF1" s="118" t="inlineStr">
         <is>
           <t>NoticeStatus</t>
+        </is>
+      </c>
+      <c r="BG1" s="118" t="inlineStr">
+        <is>
+          <t>Outstanding_Margin</t>
+        </is>
+      </c>
+      <c r="BH1" s="118" t="inlineStr">
+        <is>
+          <t>Outstanding_AllInRate</t>
+        </is>
+      </c>
+      <c r="BI1" s="118" t="inlineStr">
+        <is>
+          <t>Outstanding_AccruedInterest</t>
+        </is>
+      </c>
+      <c r="BJ1" s="118" t="inlineStr">
+        <is>
+          <t>Outstanding_Favouree</t>
+        </is>
+      </c>
+      <c r="BK1" s="118" t="inlineStr">
+        <is>
+          <t>Outstanding_RepricingFrequency</t>
+        </is>
+      </c>
+      <c r="BL1" s="118" t="inlineStr">
+        <is>
+          <t>Outstanding_RepricingDate</t>
+        </is>
+      </c>
+      <c r="BM1" s="118" t="inlineStr">
+        <is>
+          <t>Outstanding_cycleDue</t>
+        </is>
+      </c>
+      <c r="BN1" s="118" t="inlineStr">
+        <is>
+          <t>Outstanding_paidToDate</t>
         </is>
       </c>
     </row>
@@ -27854,192 +28943,241 @@
           <t>COMSEE_SCENARIO_07</t>
         </is>
       </c>
-      <c r="C2" s="159" t="inlineStr">
+      <c r="C2" s="165" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D2" s="140" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V1</t>
+        </is>
+      </c>
+      <c r="E2" s="159" t="inlineStr">
+        <is>
+          <t>3000733</t>
+        </is>
+      </c>
+      <c r="F2" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G2" s="159" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="H2" s="159" t="inlineStr">
         <is>
           <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="E2" s="159" t="inlineStr">
+      <c r="J2" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G2" s="159" t="inlineStr">
+      <c r="L2" s="159" t="inlineStr">
         <is>
           <t>100,000.00</t>
         </is>
       </c>
-      <c r="H2" s="159" t="inlineStr">
+      <c r="M2" s="159" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="I2" s="26" t="inlineStr">
+      <c r="N2" s="26" t="inlineStr">
         <is>
           <t>ESPS11810226</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="K2" s="159" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="Q2" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM17092020214046</t>
         </is>
       </c>
-      <c r="L2" s="159" t="inlineStr">
+      <c r="R2" s="159" t="inlineStr">
         <is>
           <t>60000242</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="S2" s="159" t="inlineStr">
+        <is>
+          <t>60000242</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="n"/>
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>10000.00</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="n"/>
+      <c r="Z2" s="1" t="n"/>
+      <c r="AA2" s="1" t="n"/>
+      <c r="AB2" s="1" t="n"/>
+      <c r="AC2" s="1" t="n"/>
+      <c r="AD2" s="1" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="Q2" s="26" t="inlineStr">
+      <c r="AE2" s="26" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="R2" s="159" t="inlineStr">
+      <c r="AG2" s="159" t="inlineStr">
         <is>
           <t>26-Dec-2021</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
+      <c r="AH2" s="159" t="n"/>
+      <c r="AI2" s="159" t="n"/>
+      <c r="AJ2" s="159" t="n"/>
+      <c r="AK2" s="1" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="AL2" s="1" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="AM2" s="1" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>Weeks</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="AO2" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="X2" s="26" t="inlineStr">
+      <c r="AP2" s="26" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="AQ2" s="1" t="inlineStr">
         <is>
           <t>Next Business Day</t>
         </is>
       </c>
-      <c r="Z2" s="26" t="inlineStr">
+      <c r="AR2" s="26" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AA2" s="26" t="inlineStr">
+      <c r="AS2" s="26" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AB2" s="26" t="inlineStr">
+      <c r="AT2" s="26" t="inlineStr">
         <is>
           <t>Loan Initial Drawdown</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
+      <c r="AU2" s="1" t="inlineStr">
         <is>
           <t>Awaiting Rate Approval</t>
         </is>
       </c>
-      <c r="AD2" s="1" t="inlineStr">
+      <c r="AV2" s="1" t="inlineStr">
         <is>
           <t>Awaiting Release Cashflows</t>
         </is>
       </c>
-      <c r="AE2" s="1" t="inlineStr">
+      <c r="AW2" s="1" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="AF2" s="26" t="inlineStr">
+      <c r="AX2" s="26" t="inlineStr">
         <is>
           <t>195</t>
         </is>
       </c>
-      <c r="AG2" s="1" t="inlineStr">
+      <c r="AY2" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AH2" s="26" t="inlineStr">
+      <c r="AZ2" s="26" t="inlineStr">
         <is>
           <t>DOIT</t>
         </is>
       </c>
-      <c r="AI2" s="26" t="inlineStr">
+      <c r="BA2" s="26" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AJ2" s="26" t="inlineStr">
+      <c r="BB2" s="26" t="inlineStr">
         <is>
           <t>RTGSAUD1-0736</t>
         </is>
       </c>
-      <c r="AK2" s="73" t="inlineStr">
+      <c r="BC2" s="73" t="inlineStr">
         <is>
           <t>12001001836</t>
         </is>
       </c>
-      <c r="AL2" s="73" t="inlineStr">
+      <c r="BD2" s="73" t="inlineStr">
         <is>
           <t>18567000000</t>
         </is>
       </c>
-      <c r="AM2" s="26" t="inlineStr">
-        <is>
-          <t>CB001/Hold for Investment - Australia/BP_CML</t>
-        </is>
-      </c>
-      <c r="AN2" s="26" t="inlineStr">
+      <c r="BE2" s="159" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_COL</t>
+        </is>
+      </c>
+      <c r="BF2" s="26" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
@@ -28056,192 +29194,236 @@
           <t>COMSEE_SCENARIO_07</t>
         </is>
       </c>
-      <c r="C3" s="159" t="inlineStr">
+      <c r="C3" s="165" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D3" s="140" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V2</t>
+        </is>
+      </c>
+      <c r="E3" s="159" t="inlineStr">
+        <is>
+          <t>3000734</t>
+        </is>
+      </c>
+      <c r="F3" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G3" s="159" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="H3" s="159" t="inlineStr">
         <is>
           <t>COMSEE_SC7_24092020204527</t>
         </is>
       </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="E3" s="159" t="inlineStr">
+      <c r="J3" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM24092020205243</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="K3" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G3" s="159" t="inlineStr">
+      <c r="L3" s="159" t="inlineStr">
         <is>
           <t>100,000.00</t>
         </is>
       </c>
-      <c r="H3" s="159" t="inlineStr">
+      <c r="M3" s="159" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="I3" s="26" t="inlineStr">
+      <c r="N3" s="26" t="inlineStr">
         <is>
           <t>ESPS11810226</t>
         </is>
       </c>
-      <c r="J3" s="1" t="inlineStr">
+      <c r="O3" s="1" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="K3" s="159" t="inlineStr">
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="Q3" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM17092020214046</t>
         </is>
       </c>
-      <c r="L3" s="159" t="inlineStr">
+      <c r="R3" s="159" t="inlineStr">
         <is>
           <t>60000242</t>
         </is>
       </c>
-      <c r="M3" s="1" t="inlineStr">
+      <c r="S3" s="159" t="inlineStr">
+        <is>
+          <t>60000242</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="N3" s="1" t="inlineStr">
+      <c r="V3" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="O3" s="1" t="inlineStr">
+      <c r="W3" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="X3" s="1" t="inlineStr">
         <is>
           <t>10000.00</t>
         </is>
       </c>
-      <c r="P3" s="1" t="inlineStr">
+      <c r="AD3" s="1" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="Q3" s="26" t="inlineStr">
+      <c r="AE3" s="26" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="R3" s="159" t="inlineStr">
+      <c r="AF3" s="26" t="n"/>
+      <c r="AG3" s="159" t="inlineStr">
         <is>
           <t>30-Jan-2022</t>
         </is>
       </c>
-      <c r="S3" s="1" t="inlineStr">
+      <c r="AH3" s="159" t="n"/>
+      <c r="AI3" s="159" t="n"/>
+      <c r="AJ3" s="159" t="n"/>
+      <c r="AK3" s="1" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="T3" s="1" t="inlineStr">
+      <c r="AL3" s="1" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="U3" s="1" t="inlineStr">
+      <c r="AM3" s="1" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="V3" s="1" t="inlineStr">
+      <c r="AN3" s="1" t="inlineStr">
         <is>
           <t>Weeks</t>
         </is>
       </c>
-      <c r="W3" s="1" t="inlineStr">
+      <c r="AO3" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="X3" s="26" t="inlineStr">
+      <c r="AP3" s="26" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="Y3" s="1" t="inlineStr">
+      <c r="AQ3" s="1" t="inlineStr">
         <is>
           <t>Next Business Day</t>
         </is>
       </c>
-      <c r="Z3" s="26" t="inlineStr">
+      <c r="AR3" s="26" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AA3" s="26" t="inlineStr">
+      <c r="AS3" s="26" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AB3" s="26" t="inlineStr">
+      <c r="AT3" s="26" t="inlineStr">
         <is>
           <t>Loan Initial Drawdown</t>
         </is>
       </c>
-      <c r="AC3" s="1" t="inlineStr">
+      <c r="AU3" s="1" t="inlineStr">
         <is>
           <t>Awaiting Rate Approval</t>
         </is>
       </c>
-      <c r="AD3" s="1" t="inlineStr">
+      <c r="AV3" s="1" t="inlineStr">
         <is>
           <t>Awaiting Release Cashflows</t>
         </is>
       </c>
-      <c r="AE3" s="1" t="inlineStr">
+      <c r="AW3" s="1" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="AF3" s="26" t="inlineStr">
+      <c r="AX3" s="26" t="inlineStr">
         <is>
           <t>195</t>
         </is>
       </c>
-      <c r="AG3" s="1" t="inlineStr">
+      <c r="AY3" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AH3" s="26" t="inlineStr">
+      <c r="AZ3" s="26" t="inlineStr">
         <is>
           <t>DOIT</t>
         </is>
       </c>
-      <c r="AI3" s="26" t="inlineStr">
+      <c r="BA3" s="26" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AJ3" s="26" t="inlineStr">
+      <c r="BB3" s="26" t="inlineStr">
         <is>
           <t>RTGSAUD1-0736</t>
         </is>
       </c>
-      <c r="AK3" s="73" t="inlineStr">
+      <c r="BC3" s="73" t="inlineStr">
         <is>
           <t>12001001836</t>
         </is>
       </c>
-      <c r="AL3" s="73" t="inlineStr">
+      <c r="BD3" s="73" t="inlineStr">
         <is>
           <t>18567000000</t>
         </is>
       </c>
-      <c r="AM3" s="26" t="inlineStr">
-        <is>
-          <t>CB001/Hold for Investment - Australia/BP_CML</t>
-        </is>
-      </c>
-      <c r="AN3" s="26" t="inlineStr">
+      <c r="BE3" s="159" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_COL</t>
+        </is>
+      </c>
+      <c r="BF3" s="26" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
@@ -28258,192 +29440,236 @@
           <t>COMSEE_SCENARIO_07</t>
         </is>
       </c>
-      <c r="C4" s="159" t="inlineStr">
+      <c r="C4" s="165" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D4" s="140" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V2</t>
+        </is>
+      </c>
+      <c r="E4" s="159" t="inlineStr">
+        <is>
+          <t>3000790</t>
+        </is>
+      </c>
+      <c r="F4" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G4" s="159" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="H4" s="159" t="inlineStr">
         <is>
           <t>COMSEE_SC7_02102020203942</t>
         </is>
       </c>
-      <c r="D4" s="1" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="E4" s="159" t="inlineStr">
+      <c r="J4" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM02102020204739</t>
         </is>
       </c>
-      <c r="F4" s="1" t="inlineStr">
+      <c r="K4" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G4" s="159" t="inlineStr">
+      <c r="L4" s="159" t="inlineStr">
         <is>
           <t>100,000.00</t>
         </is>
       </c>
-      <c r="H4" s="159" t="inlineStr">
+      <c r="M4" s="159" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="I4" s="26" t="inlineStr">
+      <c r="N4" s="26" t="inlineStr">
         <is>
           <t>ESPS11810226</t>
         </is>
       </c>
-      <c r="J4" s="1" t="inlineStr">
+      <c r="O4" s="1" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="K4" s="159" t="inlineStr">
+      <c r="P4" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="Q4" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM17092020214046</t>
         </is>
       </c>
-      <c r="L4" s="159" t="inlineStr">
+      <c r="R4" s="159" t="inlineStr">
         <is>
           <t>60000242</t>
         </is>
       </c>
-      <c r="M4" s="1" t="inlineStr">
+      <c r="S4" s="159" t="inlineStr">
+        <is>
+          <t>60000242</t>
+        </is>
+      </c>
+      <c r="T4" s="1" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="N4" s="1" t="inlineStr">
+      <c r="V4" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="O4" s="1" t="inlineStr">
+      <c r="W4" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="X4" s="1" t="inlineStr">
         <is>
           <t>10000.00</t>
         </is>
       </c>
-      <c r="P4" s="1" t="inlineStr">
+      <c r="AD4" s="1" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="Q4" s="26" t="inlineStr">
+      <c r="AE4" s="26" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="R4" s="159" t="inlineStr">
+      <c r="AF4" s="26" t="n"/>
+      <c r="AG4" s="159" t="inlineStr">
         <is>
           <t>17-Feb-2022</t>
         </is>
       </c>
-      <c r="S4" s="1" t="inlineStr">
+      <c r="AH4" s="159" t="n"/>
+      <c r="AI4" s="159" t="n"/>
+      <c r="AJ4" s="159" t="n"/>
+      <c r="AK4" s="1" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="T4" s="1" t="inlineStr">
+      <c r="AL4" s="1" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="U4" s="1" t="inlineStr">
+      <c r="AM4" s="1" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="V4" s="1" t="inlineStr">
+      <c r="AN4" s="1" t="inlineStr">
         <is>
           <t>Weeks</t>
         </is>
       </c>
-      <c r="W4" s="1" t="inlineStr">
+      <c r="AO4" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="X4" s="26" t="inlineStr">
+      <c r="AP4" s="26" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="Y4" s="1" t="inlineStr">
+      <c r="AQ4" s="1" t="inlineStr">
         <is>
           <t>Next Business Day</t>
         </is>
       </c>
-      <c r="Z4" s="26" t="inlineStr">
+      <c r="AR4" s="26" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AA4" s="26" t="inlineStr">
+      <c r="AS4" s="26" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AB4" s="26" t="inlineStr">
+      <c r="AT4" s="26" t="inlineStr">
         <is>
           <t>Loan Initial Drawdown</t>
         </is>
       </c>
-      <c r="AC4" s="1" t="inlineStr">
+      <c r="AU4" s="1" t="inlineStr">
         <is>
           <t>Awaiting Rate Approval</t>
         </is>
       </c>
-      <c r="AD4" s="1" t="inlineStr">
+      <c r="AV4" s="1" t="inlineStr">
         <is>
           <t>Awaiting Release Cashflows</t>
         </is>
       </c>
-      <c r="AE4" s="1" t="inlineStr">
+      <c r="AW4" s="1" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="AF4" s="26" t="inlineStr">
+      <c r="AX4" s="26" t="inlineStr">
         <is>
           <t>195</t>
         </is>
       </c>
-      <c r="AG4" s="1" t="inlineStr">
+      <c r="AY4" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AH4" s="26" t="inlineStr">
+      <c r="AZ4" s="26" t="inlineStr">
         <is>
           <t>DOIT</t>
         </is>
       </c>
-      <c r="AI4" s="26" t="inlineStr">
+      <c r="BA4" s="26" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AJ4" s="26" t="inlineStr">
+      <c r="BB4" s="26" t="inlineStr">
         <is>
           <t>RTGSAUD1-0736</t>
         </is>
       </c>
-      <c r="AK4" s="73" t="inlineStr">
+      <c r="BC4" s="73" t="inlineStr">
         <is>
           <t>12001001836</t>
         </is>
       </c>
-      <c r="AL4" s="73" t="inlineStr">
+      <c r="BD4" s="73" t="inlineStr">
         <is>
           <t>18567000000</t>
         </is>
       </c>
-      <c r="AM4" s="26" t="inlineStr">
-        <is>
-          <t>CB001/Hold for Investment - Australia/BP_CML</t>
-        </is>
-      </c>
-      <c r="AN4" s="26" t="inlineStr">
+      <c r="BE4" s="159" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_COL</t>
+        </is>
+      </c>
+      <c r="BF4" s="26" t="inlineStr">
         <is>
           <t>Awaiting release</t>
         </is>
@@ -28460,194 +29686,545 @@
           <t>COMSEE_SCENARIO_07</t>
         </is>
       </c>
-      <c r="C5" s="159" t="inlineStr">
+      <c r="C5" s="165" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D5" s="140" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V2</t>
+        </is>
+      </c>
+      <c r="E5" s="159" t="inlineStr">
+        <is>
+          <t>3000806</t>
+        </is>
+      </c>
+      <c r="F5" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G5" s="159" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="H5" s="159" t="inlineStr">
         <is>
           <t>COMSEE_SC7_06102020173604</t>
         </is>
       </c>
-      <c r="D5" s="1" t="inlineStr">
+      <c r="I5" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="E5" s="159" t="inlineStr">
+      <c r="J5" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM06102020174507</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="K5" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G5" s="159" t="inlineStr">
+      <c r="L5" s="159" t="inlineStr">
         <is>
           <t>100,000.00</t>
         </is>
       </c>
-      <c r="H5" s="159" t="inlineStr">
+      <c r="M5" s="159" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="I5" s="26" t="inlineStr">
+      <c r="N5" s="26" t="inlineStr">
         <is>
           <t>ESPS11810226</t>
         </is>
       </c>
-      <c r="J5" s="1" t="inlineStr">
+      <c r="O5" s="1" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="K5" s="159" t="inlineStr">
+      <c r="P5" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="Q5" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM17092020214046</t>
         </is>
       </c>
-      <c r="L5" s="159" t="inlineStr">
+      <c r="R5" s="159" t="inlineStr">
         <is>
           <t>60000242</t>
         </is>
       </c>
-      <c r="M5" s="1" t="inlineStr">
+      <c r="S5" s="159" t="inlineStr">
+        <is>
+          <t>60000242</t>
+        </is>
+      </c>
+      <c r="T5" s="1" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="N5" s="1" t="inlineStr">
+      <c r="V5" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="O5" s="1" t="inlineStr">
+      <c r="W5" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="X5" s="1" t="inlineStr">
         <is>
           <t>10000.00</t>
         </is>
       </c>
-      <c r="P5" s="1" t="inlineStr">
+      <c r="AD5" s="1" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="Q5" s="26" t="inlineStr">
+      <c r="AE5" s="26" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="R5" s="159" t="inlineStr">
+      <c r="AF5" s="26" t="n"/>
+      <c r="AG5" s="159" t="inlineStr">
         <is>
           <t>21-Feb-2021</t>
         </is>
       </c>
-      <c r="S5" s="1" t="inlineStr">
+      <c r="AH5" s="159" t="n"/>
+      <c r="AI5" s="159" t="n"/>
+      <c r="AJ5" s="159" t="n"/>
+      <c r="AK5" s="1" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="T5" s="1" t="inlineStr">
+      <c r="AL5" s="1" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
-      <c r="U5" s="1" t="inlineStr">
+      <c r="AM5" s="1" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="V5" s="1" t="inlineStr">
+      <c r="AN5" s="1" t="inlineStr">
         <is>
           <t>Weeks</t>
         </is>
       </c>
-      <c r="W5" s="1" t="inlineStr">
+      <c r="AO5" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="X5" s="26" t="inlineStr">
+      <c r="AP5" s="26" t="inlineStr">
         <is>
           <t>27-Dec-2018</t>
         </is>
       </c>
-      <c r="Y5" s="1" t="inlineStr">
+      <c r="AQ5" s="1" t="inlineStr">
         <is>
           <t>Next Business Day</t>
         </is>
       </c>
-      <c r="Z5" s="26" t="inlineStr">
+      <c r="AR5" s="26" t="inlineStr">
         <is>
           <t>Outstandings</t>
         </is>
       </c>
-      <c r="AA5" s="26" t="inlineStr">
+      <c r="AS5" s="26" t="inlineStr">
         <is>
           <t>Awaiting Approval</t>
         </is>
       </c>
-      <c r="AB5" s="26" t="inlineStr">
+      <c r="AT5" s="26" t="inlineStr">
         <is>
           <t>Loan Initial Drawdown</t>
         </is>
       </c>
-      <c r="AC5" s="1" t="inlineStr">
+      <c r="AU5" s="1" t="inlineStr">
         <is>
           <t>Awaiting Rate Approval</t>
         </is>
       </c>
-      <c r="AD5" s="1" t="inlineStr">
+      <c r="AV5" s="1" t="inlineStr">
         <is>
           <t>Awaiting Release Cashflows</t>
         </is>
       </c>
-      <c r="AE5" s="1" t="inlineStr">
+      <c r="AW5" s="1" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="AF5" s="26" t="inlineStr">
+      <c r="AX5" s="26" t="inlineStr">
         <is>
           <t>195</t>
         </is>
       </c>
-      <c r="AG5" s="1" t="inlineStr">
+      <c r="AY5" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AH5" s="26" t="inlineStr">
+      <c r="AZ5" s="26" t="inlineStr">
         <is>
           <t>DOIT</t>
         </is>
       </c>
-      <c r="AI5" s="26" t="inlineStr">
+      <c r="BA5" s="26" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AJ5" s="26" t="inlineStr">
+      <c r="BB5" s="26" t="inlineStr">
         <is>
           <t>RTGSAUD1-0736</t>
         </is>
       </c>
-      <c r="AK5" s="73" t="inlineStr">
+      <c r="BC5" s="73" t="inlineStr">
         <is>
           <t>12001001836</t>
         </is>
       </c>
-      <c r="AL5" s="73" t="inlineStr">
+      <c r="BD5" s="73" t="inlineStr">
         <is>
           <t>18567000000</t>
         </is>
       </c>
-      <c r="AM5" s="26" t="inlineStr">
-        <is>
-          <t>CB001/Hold for Investment - Australia/BP_CML</t>
-        </is>
-      </c>
-      <c r="AN5" s="26" t="inlineStr">
+      <c r="BE5" s="159" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_COL</t>
+        </is>
+      </c>
+      <c r="BF5" s="26" t="inlineStr">
         <is>
           <t>Awaiting release</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="108" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C6" s="165" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D6" s="140" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V1</t>
+        </is>
+      </c>
+      <c r="E6" s="159" t="inlineStr">
+        <is>
+          <t>3000848</t>
+        </is>
+      </c>
+      <c r="F6" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G6" s="159" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="H6" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="J6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L6" s="159" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="M6" s="159" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N6" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="O6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="P6" s="1" t="inlineStr">
+        <is>
+          <t>Fixed Rate Loan</t>
+        </is>
+      </c>
+      <c r="Q6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM07102020202530</t>
+        </is>
+      </c>
+      <c r="R6" s="159" t="inlineStr">
+        <is>
+          <t>60001160</t>
+        </is>
+      </c>
+      <c r="S6" s="159" t="inlineStr">
+        <is>
+          <t>60001160</t>
+        </is>
+      </c>
+      <c r="T6" s="1" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>FIXED/Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="V6" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="W6" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="X6" s="1" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="AD6" s="1" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="AE6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="AF6" s="26" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="AG6" s="159" t="inlineStr">
+        <is>
+          <t>27-Feb-2022</t>
+        </is>
+      </c>
+      <c r="AH6" s="159" t="inlineStr">
+        <is>
+          <t>2022-02-27</t>
+        </is>
+      </c>
+      <c r="AI6" s="159" t="inlineStr">
+        <is>
+          <t>Pay in Arrears</t>
+        </is>
+      </c>
+      <c r="AJ6" s="159" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="AK6" s="1" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="AL6" s="1" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="AM6" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AN6" s="1" t="inlineStr">
+        <is>
+          <t>Weeks</t>
+        </is>
+      </c>
+      <c r="AO6" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AP6" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="AQ6" s="1" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AR6" s="26" t="inlineStr">
+        <is>
+          <t>Outstandings</t>
+        </is>
+      </c>
+      <c r="AS6" s="26" t="inlineStr">
+        <is>
+          <t>Awaiting Approval</t>
+        </is>
+      </c>
+      <c r="AT6" s="26" t="inlineStr">
+        <is>
+          <t>Loan Initial Drawdown</t>
+        </is>
+      </c>
+      <c r="AU6" s="1" t="inlineStr">
+        <is>
+          <t>Awaiting Rate Approval</t>
+        </is>
+      </c>
+      <c r="AV6" s="1" t="inlineStr">
+        <is>
+          <t>Awaiting Release Cashflows</t>
+        </is>
+      </c>
+      <c r="AW6" s="1" t="inlineStr">
+        <is>
+          <t>Borrower</t>
+        </is>
+      </c>
+      <c r="AX6" s="26" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="AY6" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="AZ6" s="26" t="inlineStr">
+        <is>
+          <t>DOIT</t>
+        </is>
+      </c>
+      <c r="BA6" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BB6" s="159" t="inlineStr">
+        <is>
+          <t>RTGS1</t>
+        </is>
+      </c>
+      <c r="BC6" s="73" t="inlineStr">
+        <is>
+          <t>12001001836</t>
+        </is>
+      </c>
+      <c r="BD6" s="73" t="inlineStr">
+        <is>
+          <t>18567000000</t>
+        </is>
+      </c>
+      <c r="BE6" s="159" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_COL</t>
+        </is>
+      </c>
+      <c r="BF6" s="26" t="inlineStr">
+        <is>
+          <t>Awaiting release</t>
+        </is>
+      </c>
+      <c r="BG6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BH6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BI6" t="inlineStr">
+        <is>
+          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -28664,11 +30241,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI5"/>
+  <dimension ref="A1:CI6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -29189,6 +30766,81 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="108" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C6" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="D6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="E6" s="26" t="inlineStr">
+        <is>
+          <t>ESPS11810226</t>
+        </is>
+      </c>
+      <c r="F6" s="26" t="inlineStr">
+        <is>
+          <t>Deal/Facility</t>
+        </is>
+      </c>
+      <c r="G6" s="26" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="H6" s="159" t="inlineStr">
+        <is>
+          <t>60001160</t>
+        </is>
+      </c>
+      <c r="I6" s="26" t="inlineStr">
+        <is>
+          <t>RTGSAUD1-0736</t>
+        </is>
+      </c>
+      <c r="J6" s="26" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="K6" s="159" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="L6" s="26" t="inlineStr">
+        <is>
+          <t>Principal Payment</t>
+        </is>
+      </c>
+      <c r="M6" s="82" t="inlineStr">
+        <is>
+          <t>10,000.00</t>
+        </is>
+      </c>
+      <c r="N6" s="73" t="n">
+        <v>100</v>
+      </c>
+      <c r="O6" s="26" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -29728,6 +31380,106 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C6" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="D6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="E6" s="159" t="inlineStr">
+        <is>
+          <t>60001160</t>
+        </is>
+      </c>
+      <c r="F6" s="159" t="inlineStr">
+        <is>
+          <t>04-Feb-2021</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>FIXED Interest Due</t>
+        </is>
+      </c>
+      <c r="H6" s="26" t="inlineStr">
+        <is>
+          <t>ESPS11810226</t>
+        </is>
+      </c>
+      <c r="I6" s="26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J6" s="26" t="inlineStr">
+        <is>
+          <t>Projected Due</t>
+        </is>
+      </c>
+      <c r="K6" s="159" t="inlineStr">
+        <is>
+          <t>8.77</t>
+        </is>
+      </c>
+      <c r="L6" s="26" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="M6" s="26" t="inlineStr">
+        <is>
+          <t>Payments</t>
+        </is>
+      </c>
+      <c r="N6" s="26" t="inlineStr">
+        <is>
+          <t>Awaiting Approval</t>
+        </is>
+      </c>
+      <c r="O6" s="26" t="inlineStr">
+        <is>
+          <t>Interest Payment</t>
+        </is>
+      </c>
+      <c r="P6" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="Q6" s="26" t="inlineStr">
+        <is>
+          <t>RTGSAUD1-0736</t>
+        </is>
+      </c>
+      <c r="R6" s="73" t="n">
+        <v>100</v>
+      </c>
+      <c r="S6" s="26" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+      <c r="T6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM12102019171714</t>
+        </is>
+      </c>
+    </row>
     <row r="7">
       <c r="H7" s="86" t="n"/>
     </row>
@@ -29747,11 +31499,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -29979,9 +31731,9 @@
           <t>COMSEE_SC7_20092020192239</t>
         </is>
       </c>
-      <c r="H2" s="26" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-0736</t>
+      <c r="H2" s="159" t="inlineStr">
+        <is>
+          <t>RTGS1</t>
         </is>
       </c>
       <c r="I2" s="26" t="inlineStr">
@@ -30525,6 +32277,151 @@
       <c r="AD5" s="159" t="inlineStr">
         <is>
           <t>25-Jan-2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="157">
+      <c r="A6" s="108" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C6" s="159" t="inlineStr">
+        <is>
+          <t>05-Jan-2021</t>
+        </is>
+      </c>
+      <c r="D6" s="159" t="inlineStr">
+        <is>
+          <t>06-Mar-2021</t>
+        </is>
+      </c>
+      <c r="E6" s="148" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="F6" s="148" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="G6" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="H6" s="159" t="inlineStr">
+        <is>
+          <t>RTGS1</t>
+        </is>
+      </c>
+      <c r="I6" s="26" t="inlineStr">
+        <is>
+          <t>06000505</t>
+        </is>
+      </c>
+      <c r="J6" s="26" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="K6" s="26" t="inlineStr">
+        <is>
+          <t>DOIT</t>
+        </is>
+      </c>
+      <c r="L6" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="M6" s="26" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+      <c r="N6" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="O6" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="P6" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="Q6" s="26" t="inlineStr">
+        <is>
+          <t>ONG000000000213</t>
+        </is>
+      </c>
+      <c r="R6" s="26" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="S6" s="159" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="T6" s="159" t="inlineStr">
+        <is>
+          <t>FACI Fee Due</t>
+        </is>
+      </c>
+      <c r="U6" s="159" t="inlineStr">
+        <is>
+          <t>28-Jan-2021</t>
+        </is>
+      </c>
+      <c r="V6" s="26" t="inlineStr">
+        <is>
+          <t>04-Jun-2018</t>
+        </is>
+      </c>
+      <c r="W6" s="26" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="X6" s="26" t="n">
+        <v>9.859999999999999</v>
+      </c>
+      <c r="Z6" s="40" t="inlineStr">
+        <is>
+          <t>90,000.00</t>
+        </is>
+      </c>
+      <c r="AA6" s="40" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="AB6" s="26" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="AC6" s="26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD6" s="159" t="inlineStr">
+        <is>
+          <t>04-Feb-2021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-7816 CommSee Outstandings V2 Fixed Rate Loan
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="29" activeTab="34" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="29" activeTab="33" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -22558,11 +22558,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DC6"/>
+  <dimension ref="A1:DC7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BC6" sqref="BC6"/>
+      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -24737,7 +24737,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="26" t="inlineStr">
+      <c r="A5" s="159" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -25247,7 +25247,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="26" t="inlineStr">
+      <c r="A6" s="159" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -25750,6 +25750,515 @@
         </is>
       </c>
       <c r="DB6" s="143" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK AUST -DBU</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="162" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C7" s="159" t="inlineStr">
+        <is>
+          <t>3000848</t>
+        </is>
+      </c>
+      <c r="D7" s="165" t="inlineStr">
+        <is>
+          <t>rodel</t>
+        </is>
+      </c>
+      <c r="E7" s="141" t="inlineStr">
+        <is>
+          <t>\DataSet\API_DataSet\Input\ComSee\</t>
+        </is>
+      </c>
+      <c r="F7" s="141" t="inlineStr">
+        <is>
+          <t>COM_RES_07</t>
+        </is>
+      </c>
+      <c r="G7" s="159" t="inlineStr">
+        <is>
+          <t>2019-10-12</t>
+        </is>
+      </c>
+      <c r="H7" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="I7" s="159" t="inlineStr">
+        <is>
+          <t>1001040</t>
+        </is>
+      </c>
+      <c r="J7" s="159" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="K7" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="L7" s="165" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="M7" s="159" t="inlineStr">
+        <is>
+          <t>AUSNA</t>
+        </is>
+      </c>
+      <c r="N7" s="159" t="inlineStr">
+        <is>
+          <t>Non-Agency Australia</t>
+        </is>
+      </c>
+      <c r="O7" s="149" t="inlineStr">
+        <is>
+          <t>BP_CML</t>
+        </is>
+      </c>
+      <c r="P7" s="159" t="inlineStr">
+        <is>
+          <t>Commercial Lending</t>
+        </is>
+      </c>
+      <c r="Q7" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="U7" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="V7" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="W7" s="159" t="inlineStr">
+        <is>
+          <t>GLB</t>
+        </is>
+      </c>
+      <c r="X7" s="149" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="Y7" s="109" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_</t>
+        </is>
+      </c>
+      <c r="Z7" s="109" t="inlineStr">
+        <is>
+          <t>CS7</t>
+        </is>
+      </c>
+      <c r="AA7" s="26" t="inlineStr">
+        <is>
+          <t>S724062019190029CNO</t>
+        </is>
+      </c>
+      <c r="AB7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="AC7" s="149" t="inlineStr">
+        <is>
+          <t>Sales Group 1</t>
+        </is>
+      </c>
+      <c r="AD7" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="AE7" s="26" t="inlineStr">
+        <is>
+          <t>Melbourne, VIC,Australia</t>
+        </is>
+      </c>
+      <c r="AF7" s="149" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="AG7" s="149" t="inlineStr">
+        <is>
+          <t>GCP</t>
+        </is>
+      </c>
+      <c r="AH7" s="149" t="inlineStr">
+        <is>
+          <t>General Corp Purpose</t>
+        </is>
+      </c>
+      <c r="AI7" s="149" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="AJ7" s="149" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="AK7" s="149" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AL7" s="149" t="inlineStr">
+        <is>
+          <t>Lending,${SPACE}${SPACE}Operations</t>
+        </is>
+      </c>
+      <c r="AM7" s="149" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AN7" s="149" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="AO7" s="149" t="inlineStr">
+        <is>
+          <t>10,000,000.00</t>
+        </is>
+      </c>
+      <c r="AP7" s="149" t="inlineStr">
+        <is>
+          <t>Sydney, Australia</t>
+        </is>
+      </c>
+      <c r="AQ7" s="148" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AR7" s="149" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AS7" s="149" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AT7" s="149" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="AU7" s="149" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AV7" s="149" t="inlineStr">
+        <is>
+          <t>Start of current cycle</t>
+        </is>
+      </c>
+      <c r="AW7" s="26" t="inlineStr">
+        <is>
+          <t>Start of next interest cycle</t>
+        </is>
+      </c>
+      <c r="AX7" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY7" s="149" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="AZ7" s="149" t="inlineStr">
+        <is>
+          <t>Effective date of change</t>
+        </is>
+      </c>
+      <c r="BA7" s="149" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="BB7" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC7" s="26" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="BD7" s="149" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="BE7" s="149" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="BF7" s="149" t="inlineStr">
+        <is>
+          <t>IT_COL</t>
+        </is>
+      </c>
+      <c r="BG7" s="26" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="BH7" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="BI7" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="BJ7" s="26" t="inlineStr">
+        <is>
+          <t>Add Comment</t>
+        </is>
+      </c>
+      <c r="BK7" s="149" t="inlineStr">
+        <is>
+          <t>Business Verification,${SPACE}${SPACE}BVT</t>
+        </is>
+      </c>
+      <c r="BL7" s="26" t="inlineStr">
+        <is>
+          <t>LENDING</t>
+        </is>
+      </c>
+      <c r="BM7" s="149" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="BN7" s="149" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="BO7" s="149" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="BP7" s="149" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="BQ7" s="159" t="inlineStr">
+        <is>
+          <t>28-Jan-2022</t>
+        </is>
+      </c>
+      <c r="BR7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="BT7" s="143" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia -DBU</t>
+        </is>
+      </c>
+      <c r="BU7" s="143" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="BV7" s="143" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BW7" s="143" t="inlineStr">
+        <is>
+          <t>ZOE</t>
+        </is>
+      </c>
+      <c r="BX7" s="143" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="BY7" s="143" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="BZ7" s="143" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+      <c r="CA7" s="143" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank Australia - DBU</t>
+        </is>
+      </c>
+      <c r="CB7" s="69" t="inlineStr">
+        <is>
+          <t>FJAPR01</t>
+        </is>
+      </c>
+      <c r="CC7" s="1" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CD7" s="69" t="inlineStr">
+        <is>
+          <t>FJUSR01</t>
+        </is>
+      </c>
+      <c r="CE7" s="1" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CF7" s="69" t="inlineStr">
+        <is>
+          <t>FJMGR01</t>
+        </is>
+      </c>
+      <c r="CG7" s="69" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+      <c r="CH7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CI7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CJ7" s="143" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH% DBU</t>
+        </is>
+      </c>
+      <c r="CK7" s="143" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK OF AUSTRALIA - DBU</t>
+        </is>
+      </c>
+      <c r="CL7" s="143" t="inlineStr">
+        <is>
+          <t>Bank Guarantee/Letter of Credit/Synd Fronted Bank</t>
+        </is>
+      </c>
+      <c r="CM7" s="143" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="CN7" s="143" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="CO7" s="143" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="CP7" s="143" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="CQ7" s="143" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="CR7" s="143" t="inlineStr">
+        <is>
+          <t>BLOGGS</t>
+        </is>
+      </c>
+      <c r="CS7" s="143" t="inlineStr">
+        <is>
+          <t>Bloggs,  John</t>
+        </is>
+      </c>
+      <c r="CT7" s="143" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="CU7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CV7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CW7" s="109" t="n"/>
+      <c r="CX7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="CY7" s="143" t="inlineStr">
+        <is>
+          <t>JB</t>
+        </is>
+      </c>
+      <c r="CZ7" s="143" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="DA7" s="143" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="DB7" s="143" t="inlineStr">
         <is>
           <t>COMMONWEALTH BANK AUST -DBU</t>
         </is>
@@ -25768,13 +26277,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY6"/>
+  <dimension ref="A1:AY7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -26796,7 +27305,7 @@
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="157">
-      <c r="A5" s="26" t="inlineStr">
+      <c r="A5" s="159" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -27041,7 +27550,7 @@
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="157">
-      <c r="A6" s="108" t="inlineStr">
+      <c r="A6" s="162" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -27279,6 +27788,250 @@
         </is>
       </c>
       <c r="AY6" s="35" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="157">
+      <c r="A7" s="159" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="D7" s="159" t="inlineStr">
+        <is>
+          <t>3000848</t>
+        </is>
+      </c>
+      <c r="E7" s="159" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="F7" s="159" t="inlineStr">
+        <is>
+          <t>2022-02-27</t>
+        </is>
+      </c>
+      <c r="G7" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="H7" s="159" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="26" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="J7" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="K7" s="159" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="L7" s="159" t="inlineStr">
+        <is>
+          <t>90000.00</t>
+        </is>
+      </c>
+      <c r="M7" s="159" t="inlineStr">
+        <is>
+          <t>IT_COL|Corporate Lending</t>
+        </is>
+      </c>
+      <c r="N7" s="159" t="inlineStr">
+        <is>
+          <t>AUSNA</t>
+        </is>
+      </c>
+      <c r="O7" s="159" t="inlineStr">
+        <is>
+          <t>Non-Agency Australia</t>
+        </is>
+      </c>
+      <c r="P7" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="T7" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="U7" s="159" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="V7" s="159" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="W7" s="159" t="inlineStr">
+        <is>
+          <t>90000.00</t>
+        </is>
+      </c>
+      <c r="X7" s="159" t="inlineStr">
+        <is>
+          <t>HFIAU</t>
+        </is>
+      </c>
+      <c r="Y7" s="159" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="Z7" s="159" t="inlineStr">
+        <is>
+          <t>CB001</t>
+        </is>
+      </c>
+      <c r="AA7" s="159" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="AB7" s="159" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AC7" s="159" t="inlineStr">
+        <is>
+          <t>Australian (Sydney)</t>
+        </is>
+      </c>
+      <c r="AD7" s="159" t="inlineStr">
+        <is>
+          <t>2022-01-28</t>
+        </is>
+      </c>
+      <c r="AE7" s="109" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM</t>
+        </is>
+      </c>
+      <c r="AF7" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="AG7" s="26" t="inlineStr">
+        <is>
+          <t>S124062019191047FMB</t>
+        </is>
+      </c>
+      <c r="AH7" s="150" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AI7" s="150" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="AK7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="AL7" s="26" t="inlineStr">
+        <is>
+          <t>16-Aug-2019</t>
+        </is>
+      </c>
+      <c r="AM7" s="26" t="inlineStr">
+        <is>
+          <t>15-Sep-2019</t>
+        </is>
+      </c>
+      <c r="AN7" s="149" t="inlineStr">
+        <is>
+          <t>BUSINESS VERIFICATION</t>
+        </is>
+      </c>
+      <c r="AO7" s="149" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+      <c r="AP7" s="150" t="inlineStr">
+        <is>
+          <t>Fixed Rate Loan</t>
+        </is>
+      </c>
+      <c r="AQ7" s="150" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AR7" s="150" t="inlineStr">
+        <is>
+          <t>Acquisitions</t>
+        </is>
+      </c>
+      <c r="AS7" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AT7" s="26" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia</t>
+        </is>
+      </c>
+      <c r="AU7" s="26" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="AV7" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="AW7" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AX7" s="26" t="inlineStr">
+        <is>
+          <t>BLOGGS</t>
+        </is>
+      </c>
+      <c r="AY7" s="35" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
@@ -27297,13 +28050,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -27311,24 +28064,24 @@
     <col width="6.140625" customWidth="1" style="26" min="1" max="1"/>
     <col width="21.7109375" customWidth="1" style="26" min="2" max="7"/>
     <col width="27.85546875" customWidth="1" style="26" min="8" max="8"/>
-    <col width="21.7109375" customWidth="1" style="26" min="9" max="20"/>
-    <col width="22.85546875" customWidth="1" style="26" min="21" max="21"/>
-    <col width="22.7109375" customWidth="1" style="26" min="22" max="22"/>
-    <col width="27.140625" customWidth="1" style="26" min="23" max="23"/>
-    <col width="23.42578125" customWidth="1" style="26" min="24" max="24"/>
-    <col width="21.85546875" customWidth="1" style="26" min="25" max="25"/>
-    <col width="26.42578125" customWidth="1" style="26" min="26" max="26"/>
-    <col width="23.5703125" customWidth="1" style="26" min="27" max="28"/>
-    <col width="21.85546875" customWidth="1" style="26" min="29" max="29"/>
-    <col width="15.7109375" customWidth="1" style="26" min="30" max="30"/>
-    <col width="24.7109375" customWidth="1" style="26" min="31" max="32"/>
-    <col width="16.42578125" customWidth="1" style="26" min="33" max="33"/>
-    <col width="21.42578125" customWidth="1" style="26" min="34" max="34"/>
-    <col width="17.85546875" customWidth="1" style="26" min="35" max="35"/>
-    <col width="21" customWidth="1" style="26" min="36" max="37"/>
-    <col width="22" customWidth="1" style="26" min="38" max="38"/>
-    <col width="25.42578125" customWidth="1" style="26" min="39" max="39"/>
-    <col width="26.5703125" bestFit="1" customWidth="1" style="157" min="40" max="40"/>
+    <col width="21.7109375" customWidth="1" style="26" min="9" max="21"/>
+    <col width="22.85546875" customWidth="1" style="26" min="22" max="22"/>
+    <col width="22.7109375" customWidth="1" style="26" min="23" max="23"/>
+    <col width="27.140625" customWidth="1" style="26" min="24" max="24"/>
+    <col width="23.42578125" customWidth="1" style="26" min="25" max="25"/>
+    <col width="21.85546875" customWidth="1" style="26" min="26" max="26"/>
+    <col width="26.42578125" customWidth="1" style="26" min="27" max="27"/>
+    <col width="23.5703125" customWidth="1" style="26" min="28" max="29"/>
+    <col width="21.85546875" customWidth="1" style="26" min="30" max="30"/>
+    <col width="15.7109375" customWidth="1" style="26" min="31" max="31"/>
+    <col width="24.7109375" customWidth="1" style="26" min="32" max="33"/>
+    <col width="16.42578125" customWidth="1" style="26" min="34" max="34"/>
+    <col width="21.42578125" customWidth="1" style="26" min="35" max="35"/>
+    <col width="17.85546875" customWidth="1" style="26" min="36" max="36"/>
+    <col width="21" customWidth="1" style="26" min="37" max="38"/>
+    <col width="22" customWidth="1" style="26" min="39" max="39"/>
+    <col width="25.42578125" customWidth="1" style="26" min="40" max="40"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" style="157" min="41" max="41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="135">
@@ -27429,105 +28182,110 @@
       </c>
       <c r="T1" s="129" t="inlineStr">
         <is>
+          <t>Fee_CycleDue</t>
+        </is>
+      </c>
+      <c r="U1" s="129" t="inlineStr">
+        <is>
           <t>Fee_PaidToDate</t>
         </is>
       </c>
-      <c r="U1" s="135" t="inlineStr">
+      <c r="V1" s="135" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="V1" s="135" t="inlineStr">
+      <c r="W1" s="135" t="inlineStr">
         <is>
           <t>OngoingFee_Category1</t>
         </is>
       </c>
-      <c r="W1" s="135" t="inlineStr">
+      <c r="X1" s="135" t="inlineStr">
         <is>
           <t>OngoingFee_Type1</t>
         </is>
       </c>
-      <c r="X1" s="135" t="inlineStr">
+      <c r="Y1" s="135" t="inlineStr">
         <is>
           <t>OngoingFee_RateBasis1</t>
         </is>
       </c>
-      <c r="Y1" s="135" t="inlineStr">
+      <c r="Z1" s="135" t="inlineStr">
         <is>
           <t>OngoingFee_AfterItem</t>
         </is>
       </c>
-      <c r="Z1" s="135" t="inlineStr">
+      <c r="AA1" s="135" t="inlineStr">
         <is>
           <t>OngoingFee_AfterItemType</t>
         </is>
       </c>
-      <c r="AA1" s="135" t="inlineStr">
+      <c r="AB1" s="135" t="inlineStr">
         <is>
           <t>Facility_PercentWhole</t>
         </is>
       </c>
-      <c r="AB1" s="135" t="inlineStr">
+      <c r="AC1" s="135" t="inlineStr">
         <is>
           <t>Facility_Percent</t>
         </is>
       </c>
-      <c r="AC1" s="135" t="inlineStr">
+      <c r="AD1" s="135" t="inlineStr">
         <is>
           <t>OngoingFee_SpreadType1</t>
         </is>
       </c>
-      <c r="AD1" s="135" t="inlineStr">
+      <c r="AE1" s="135" t="inlineStr">
         <is>
           <t>OngoingFee_SpreadType2</t>
         </is>
       </c>
-      <c r="AE1" s="135" t="inlineStr">
+      <c r="AF1" s="135" t="inlineStr">
         <is>
           <t>Interest_AddItem</t>
         </is>
       </c>
-      <c r="AF1" s="135" t="inlineStr">
+      <c r="AG1" s="135" t="inlineStr">
         <is>
           <t>Interest_OptionName1</t>
         </is>
       </c>
-      <c r="AG1" s="135" t="inlineStr">
+      <c r="AH1" s="135" t="inlineStr">
         <is>
           <t>Interest_RateBasis</t>
         </is>
       </c>
-      <c r="AH1" s="135" t="inlineStr">
+      <c r="AI1" s="135" t="inlineStr">
         <is>
           <t>Interest_SpreadType1</t>
         </is>
       </c>
-      <c r="AI1" s="135" t="inlineStr">
+      <c r="AJ1" s="135" t="inlineStr">
         <is>
           <t>Interest_SpreadType2</t>
         </is>
       </c>
-      <c r="AJ1" s="135" t="inlineStr">
+      <c r="AK1" s="135" t="inlineStr">
         <is>
           <t>Interest_SpreadValue1</t>
         </is>
       </c>
-      <c r="AK1" s="135" t="inlineStr">
+      <c r="AL1" s="135" t="inlineStr">
         <is>
           <t>Interest_SpreadAmt1</t>
         </is>
       </c>
-      <c r="AL1" s="135" t="inlineStr">
+      <c r="AM1" s="135" t="inlineStr">
         <is>
           <t>Interest_BaseRateCode1</t>
         </is>
       </c>
-      <c r="AM1" s="135" t="inlineStr">
+      <c r="AN1" s="135" t="inlineStr">
         <is>
           <t>Facility_PricingRuleOption1</t>
         </is>
       </c>
-      <c r="AN1" s="128" t="inlineStr">
+      <c r="AO1" s="128" t="inlineStr">
         <is>
           <t>AccrualRule_PayInAdvance</t>
         </is>
@@ -27629,107 +28387,108 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="T2" s="159" t="inlineStr">
+      <c r="T2" s="159" t="n"/>
+      <c r="U2" s="159" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="U2" s="159" t="inlineStr">
+      <c r="V2" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM20092020193010</t>
         </is>
       </c>
-      <c r="V2" s="150" t="inlineStr">
+      <c r="W2" s="150" t="inlineStr">
         <is>
           <t>Facility Ongoing Fee</t>
         </is>
       </c>
-      <c r="W2" s="150" t="inlineStr">
+      <c r="X2" s="150" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="X2" s="37" t="inlineStr">
+      <c r="Y2" s="37" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="Y2" s="150" t="inlineStr">
+      <c r="Z2" s="150" t="inlineStr">
         <is>
           <t>FormulaCategory</t>
         </is>
       </c>
-      <c r="Z2" s="150" t="inlineStr">
+      <c r="AA2" s="150" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="AA2" s="150" t="inlineStr">
+      <c r="AB2" s="150" t="inlineStr">
         <is>
           <t>4%</t>
         </is>
       </c>
-      <c r="AB2" s="150" t="inlineStr">
+      <c r="AC2" s="150" t="inlineStr">
         <is>
           <t>4.000000</t>
         </is>
       </c>
-      <c r="AC2" s="149" t="inlineStr">
+      <c r="AD2" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AD2" s="148" t="inlineStr">
+      <c r="AE2" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AE2" s="26" t="inlineStr">
+      <c r="AF2" s="26" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
       </c>
-      <c r="AF2" s="150" t="inlineStr">
+      <c r="AG2" s="150" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AG2" s="38" t="inlineStr">
+      <c r="AH2" s="38" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AH2" s="149" t="inlineStr">
+      <c r="AI2" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AI2" s="148" t="inlineStr">
+      <c r="AJ2" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AJ2" s="26" t="inlineStr">
+      <c r="AK2" s="26" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AK2" s="26" t="inlineStr">
+      <c r="AL2" s="26" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AL2" s="26" t="inlineStr">
+      <c r="AM2" s="26" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="AM2" s="26" t="inlineStr">
+      <c r="AN2" s="26" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AN2" s="148" t="inlineStr">
+      <c r="AO2" s="148" t="inlineStr">
         <is>
           <t>Pay In Arrears</t>
         </is>
@@ -27831,107 +28590,108 @@
           <t>460.26</t>
         </is>
       </c>
-      <c r="T3" s="159" t="inlineStr">
+      <c r="T3" s="159" t="n"/>
+      <c r="U3" s="159" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="U3" s="159" t="inlineStr">
+      <c r="V3" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM20092020200906</t>
         </is>
       </c>
-      <c r="V3" s="150" t="inlineStr">
+      <c r="W3" s="150" t="inlineStr">
         <is>
           <t>Facility Ongoing Fee</t>
         </is>
       </c>
-      <c r="W3" s="150" t="inlineStr">
+      <c r="X3" s="150" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="X3" s="37" t="inlineStr">
+      <c r="Y3" s="37" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="Y3" s="150" t="inlineStr">
+      <c r="Z3" s="150" t="inlineStr">
         <is>
           <t>FormulaCategory</t>
         </is>
       </c>
-      <c r="Z3" s="150" t="inlineStr">
+      <c r="AA3" s="150" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="AA3" s="150" t="inlineStr">
+      <c r="AB3" s="150" t="inlineStr">
         <is>
           <t>4%</t>
         </is>
       </c>
-      <c r="AB3" s="150" t="inlineStr">
+      <c r="AC3" s="150" t="inlineStr">
         <is>
           <t>4.000000</t>
         </is>
       </c>
-      <c r="AC3" s="149" t="inlineStr">
+      <c r="AD3" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AD3" s="148" t="inlineStr">
+      <c r="AE3" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AE3" s="159" t="inlineStr">
+      <c r="AF3" s="159" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
       </c>
-      <c r="AF3" s="150" t="inlineStr">
+      <c r="AG3" s="150" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AG3" s="98" t="inlineStr">
+      <c r="AH3" s="98" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AH3" s="149" t="inlineStr">
+      <c r="AI3" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AI3" s="148" t="inlineStr">
+      <c r="AJ3" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AJ3" s="159" t="inlineStr">
+      <c r="AK3" s="159" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AK3" s="159" t="inlineStr">
+      <c r="AL3" s="159" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AL3" s="159" t="inlineStr">
+      <c r="AM3" s="159" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="AM3" s="159" t="inlineStr">
+      <c r="AN3" s="159" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AN3" s="148" t="inlineStr">
+      <c r="AO3" s="148" t="inlineStr">
         <is>
           <t>Pay In Arrears</t>
         </is>
@@ -28033,107 +28793,108 @@
           <t>10.96</t>
         </is>
       </c>
-      <c r="T4" s="159" t="inlineStr">
+      <c r="T4" s="159" t="n"/>
+      <c r="U4" s="159" t="inlineStr">
         <is>
           <t>10.96</t>
         </is>
       </c>
-      <c r="U4" s="159" t="inlineStr">
+      <c r="V4" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM02102020204739</t>
         </is>
       </c>
-      <c r="V4" s="150" t="inlineStr">
+      <c r="W4" s="150" t="inlineStr">
         <is>
           <t>Facility Ongoing Fee</t>
         </is>
       </c>
-      <c r="W4" s="150" t="inlineStr">
+      <c r="X4" s="150" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="X4" s="37" t="inlineStr">
+      <c r="Y4" s="37" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="Y4" s="150" t="inlineStr">
+      <c r="Z4" s="150" t="inlineStr">
         <is>
           <t>FormulaCategory</t>
         </is>
       </c>
-      <c r="Z4" s="150" t="inlineStr">
+      <c r="AA4" s="150" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="AA4" s="150" t="inlineStr">
+      <c r="AB4" s="150" t="inlineStr">
         <is>
           <t>4%</t>
         </is>
       </c>
-      <c r="AB4" s="150" t="inlineStr">
+      <c r="AC4" s="150" t="inlineStr">
         <is>
           <t>4.000000</t>
         </is>
       </c>
-      <c r="AC4" s="149" t="inlineStr">
+      <c r="AD4" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AD4" s="148" t="inlineStr">
+      <c r="AE4" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AE4" s="159" t="inlineStr">
+      <c r="AF4" s="159" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
       </c>
-      <c r="AF4" s="150" t="inlineStr">
+      <c r="AG4" s="150" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AG4" s="98" t="inlineStr">
+      <c r="AH4" s="98" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AH4" s="149" t="inlineStr">
+      <c r="AI4" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AI4" s="148" t="inlineStr">
+      <c r="AJ4" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AJ4" s="159" t="inlineStr">
+      <c r="AK4" s="159" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AK4" s="159" t="inlineStr">
+      <c r="AL4" s="159" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AL4" s="159" t="inlineStr">
+      <c r="AM4" s="159" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="AM4" s="159" t="inlineStr">
+      <c r="AN4" s="159" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AN4" s="148" t="inlineStr">
+      <c r="AO4" s="148" t="inlineStr">
         <is>
           <t>Pay In Arrears</t>
         </is>
@@ -28235,114 +28996,115 @@
           <t>10.96</t>
         </is>
       </c>
-      <c r="T5" s="159" t="inlineStr">
+      <c r="T5" s="159" t="n"/>
+      <c r="U5" s="159" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="U5" s="159" t="inlineStr">
+      <c r="V5" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM06102020174507</t>
         </is>
       </c>
-      <c r="V5" s="150" t="inlineStr">
+      <c r="W5" s="150" t="inlineStr">
         <is>
           <t>Facility Ongoing Fee</t>
         </is>
       </c>
-      <c r="W5" s="150" t="inlineStr">
+      <c r="X5" s="150" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="X5" s="37" t="inlineStr">
+      <c r="Y5" s="37" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="Y5" s="150" t="inlineStr">
+      <c r="Z5" s="150" t="inlineStr">
         <is>
           <t>FormulaCategory</t>
         </is>
       </c>
-      <c r="Z5" s="150" t="inlineStr">
+      <c r="AA5" s="150" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="AA5" s="150" t="inlineStr">
+      <c r="AB5" s="150" t="inlineStr">
         <is>
           <t>4%</t>
         </is>
       </c>
-      <c r="AB5" s="150" t="inlineStr">
+      <c r="AC5" s="150" t="inlineStr">
         <is>
           <t>4.000000</t>
         </is>
       </c>
-      <c r="AC5" s="149" t="inlineStr">
+      <c r="AD5" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AD5" s="148" t="inlineStr">
+      <c r="AE5" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AE5" s="159" t="inlineStr">
+      <c r="AF5" s="159" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
       </c>
-      <c r="AF5" s="150" t="inlineStr">
+      <c r="AG5" s="150" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AG5" s="98" t="inlineStr">
+      <c r="AH5" s="98" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AH5" s="149" t="inlineStr">
+      <c r="AI5" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AI5" s="148" t="inlineStr">
+      <c r="AJ5" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AJ5" s="159" t="inlineStr">
+      <c r="AK5" s="159" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AK5" s="159" t="inlineStr">
+      <c r="AL5" s="159" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AL5" s="159" t="inlineStr">
+      <c r="AM5" s="159" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="AM5" s="159" t="inlineStr">
+      <c r="AN5" s="159" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AN5" s="148" t="inlineStr">
+      <c r="AO5" s="148" t="inlineStr">
         <is>
           <t>Pay In Arrears</t>
         </is>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="157">
-      <c r="A6" s="108" t="inlineStr">
+      <c r="A6" s="162" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -28437,107 +29199,315 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="T6" s="159" t="inlineStr">
+      <c r="T6" s="159" t="n"/>
+      <c r="U6" s="159" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="U6" s="159" t="inlineStr">
+      <c r="V6" s="159" t="inlineStr">
         <is>
           <t>CSSC7_TERM09102020115930</t>
         </is>
       </c>
-      <c r="V6" s="150" t="inlineStr">
+      <c r="W6" s="150" t="inlineStr">
         <is>
           <t>Facility Ongoing Fee</t>
         </is>
       </c>
-      <c r="W6" s="150" t="inlineStr">
+      <c r="X6" s="150" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="X6" s="37" t="inlineStr">
+      <c r="Y6" s="37" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="Y6" s="150" t="inlineStr">
+      <c r="Z6" s="150" t="inlineStr">
         <is>
           <t>FormulaCategory</t>
         </is>
       </c>
-      <c r="Z6" s="150" t="inlineStr">
+      <c r="AA6" s="150" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="AA6" s="150" t="inlineStr">
+      <c r="AB6" s="150" t="inlineStr">
         <is>
           <t>4%</t>
         </is>
       </c>
-      <c r="AB6" s="150" t="inlineStr">
+      <c r="AC6" s="150" t="inlineStr">
         <is>
           <t>4.000000</t>
         </is>
       </c>
-      <c r="AC6" s="149" t="inlineStr">
+      <c r="AD6" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AD6" s="148" t="inlineStr">
+      <c r="AE6" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AE6" s="26" t="inlineStr">
+      <c r="AF6" s="26" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
       </c>
-      <c r="AF6" s="150" t="inlineStr">
+      <c r="AG6" s="150" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AG6" s="38" t="inlineStr">
+      <c r="AH6" s="38" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AH6" s="149" t="inlineStr">
+      <c r="AI6" s="149" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AI6" s="148" t="inlineStr">
+      <c r="AJ6" s="148" t="inlineStr">
         <is>
           <t>Basis Points</t>
         </is>
       </c>
-      <c r="AJ6" s="26" t="inlineStr">
+      <c r="AK6" s="26" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AK6" s="26" t="inlineStr">
+      <c r="AL6" s="26" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AL6" s="26" t="inlineStr">
+      <c r="AM6" s="26" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="AM6" s="26" t="inlineStr">
+      <c r="AN6" s="26" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
       </c>
-      <c r="AN6" s="148" t="inlineStr">
+      <c r="AO6" s="148" t="inlineStr">
+        <is>
+          <t>Pay In Arrears</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="157">
+      <c r="A7" s="162" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C7" s="140" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D7" s="140" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V2</t>
+        </is>
+      </c>
+      <c r="E7" s="159" t="inlineStr">
+        <is>
+          <t>3000848</t>
+        </is>
+      </c>
+      <c r="F7" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G7" s="159" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="H7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="I7" s="159" t="inlineStr">
+        <is>
+          <t>ONG000000000604</t>
+        </is>
+      </c>
+      <c r="J7" s="159" t="inlineStr">
+        <is>
+          <t>Released</t>
+        </is>
+      </c>
+      <c r="K7" s="159" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="L7" s="159" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="M7" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="N7" s="159" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="O7" s="159" t="inlineStr">
+        <is>
+          <t>2022-02-27</t>
+        </is>
+      </c>
+      <c r="P7" s="159" t="inlineStr">
+        <is>
+          <t>2021-02-04</t>
+        </is>
+      </c>
+      <c r="Q7" s="159" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="R7" s="159" t="inlineStr">
+        <is>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="S7" s="159" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="T7" s="159" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="U7" s="159" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="V7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="W7" s="150" t="inlineStr">
+        <is>
+          <t>Facility Ongoing Fee</t>
+        </is>
+      </c>
+      <c r="X7" s="150" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="Y7" s="37" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="Z7" s="150" t="inlineStr">
+        <is>
+          <t>FormulaCategory</t>
+        </is>
+      </c>
+      <c r="AA7" s="150" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="AB7" s="150" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="AC7" s="150" t="inlineStr">
+        <is>
+          <t>4.000000</t>
+        </is>
+      </c>
+      <c r="AD7" s="149" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+      <c r="AE7" s="148" t="inlineStr">
+        <is>
+          <t>Basis Points</t>
+        </is>
+      </c>
+      <c r="AF7" s="26" t="inlineStr">
+        <is>
+          <t>Option</t>
+        </is>
+      </c>
+      <c r="AG7" s="150" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AH7" s="38" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="AI7" s="149" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
+      <c r="AJ7" s="148" t="inlineStr">
+        <is>
+          <t>Basis Points</t>
+        </is>
+      </c>
+      <c r="AK7" s="26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AL7" s="26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AM7" s="26" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="AN7" s="26" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="AO7" s="148" t="inlineStr">
         <is>
           <t>Pay In Arrears</t>
         </is>
@@ -28556,10 +29526,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BN6"/>
+  <dimension ref="A1:BN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -30228,6 +31198,323 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C7" s="165" t="inlineStr">
+        <is>
+          <t>\DataSet\Integration_DataSet\CommSee\Output\</t>
+        </is>
+      </c>
+      <c r="D7" s="140" t="inlineStr">
+        <is>
+          <t>COM_RES_07_V2</t>
+        </is>
+      </c>
+      <c r="E7" s="159" t="inlineStr">
+        <is>
+          <t>3000848</t>
+        </is>
+      </c>
+      <c r="F7" s="159" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G7" s="159" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="H7" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="J7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L7" s="159" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="M7" s="159" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N7" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="O7" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="P7" s="1" t="inlineStr">
+        <is>
+          <t>Fixed Rate Loan</t>
+        </is>
+      </c>
+      <c r="Q7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM07102020202530</t>
+        </is>
+      </c>
+      <c r="R7" s="159" t="inlineStr">
+        <is>
+          <t>60001160</t>
+        </is>
+      </c>
+      <c r="S7" s="159" t="inlineStr">
+        <is>
+          <t>60001160</t>
+        </is>
+      </c>
+      <c r="T7" s="1" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>FIXED/Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="V7" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="W7" s="1" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="X7" s="1" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="AD7" s="1" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="AE7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="AF7" s="26" t="inlineStr">
+        <is>
+          <t>2021-01-28</t>
+        </is>
+      </c>
+      <c r="AG7" s="159" t="inlineStr">
+        <is>
+          <t>27-Feb-2022</t>
+        </is>
+      </c>
+      <c r="AH7" s="159" t="inlineStr">
+        <is>
+          <t>2022-02-27</t>
+        </is>
+      </c>
+      <c r="AI7" s="159" t="inlineStr">
+        <is>
+          <t>Pay in Arrears</t>
+        </is>
+      </c>
+      <c r="AJ7" s="159" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="AK7" s="1" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="AL7" s="1" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="AM7" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AN7" s="1" t="inlineStr">
+        <is>
+          <t>Weeks</t>
+        </is>
+      </c>
+      <c r="AO7" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AP7" s="26" t="inlineStr">
+        <is>
+          <t>27-Dec-2018</t>
+        </is>
+      </c>
+      <c r="AQ7" s="1" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AR7" s="26" t="inlineStr">
+        <is>
+          <t>Outstandings</t>
+        </is>
+      </c>
+      <c r="AS7" s="26" t="inlineStr">
+        <is>
+          <t>Awaiting Approval</t>
+        </is>
+      </c>
+      <c r="AT7" s="26" t="inlineStr">
+        <is>
+          <t>Loan Initial Drawdown</t>
+        </is>
+      </c>
+      <c r="AU7" s="1" t="inlineStr">
+        <is>
+          <t>Awaiting Rate Approval</t>
+        </is>
+      </c>
+      <c r="AV7" s="1" t="inlineStr">
+        <is>
+          <t>Awaiting Release Cashflows</t>
+        </is>
+      </c>
+      <c r="AW7" s="1" t="inlineStr">
+        <is>
+          <t>Borrower</t>
+        </is>
+      </c>
+      <c r="AX7" s="26" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="AY7" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="AZ7" s="26" t="inlineStr">
+        <is>
+          <t>DOIT</t>
+        </is>
+      </c>
+      <c r="BA7" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BB7" s="159" t="inlineStr">
+        <is>
+          <t>RTGS1</t>
+        </is>
+      </c>
+      <c r="BC7" s="73" t="inlineStr">
+        <is>
+          <t>12001001836</t>
+        </is>
+      </c>
+      <c r="BD7" s="73" t="inlineStr">
+        <is>
+          <t>18567000000</t>
+        </is>
+      </c>
+      <c r="BE7" s="159" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_COL</t>
+        </is>
+      </c>
+      <c r="BF7" s="26" t="inlineStr">
+        <is>
+          <t>Awaiting release</t>
+        </is>
+      </c>
+      <c r="BG7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BH7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BI7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BM7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BN7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -30241,11 +31528,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI6"/>
+  <dimension ref="A1:CI7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B6" sqref="B6"/>
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B7" sqref="B7:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -30841,6 +32128,81 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C7" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="D7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="E7" s="26" t="inlineStr">
+        <is>
+          <t>ESPS11810226</t>
+        </is>
+      </c>
+      <c r="F7" s="26" t="inlineStr">
+        <is>
+          <t>Deal/Facility</t>
+        </is>
+      </c>
+      <c r="G7" s="26" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="H7" s="159" t="inlineStr">
+        <is>
+          <t>60001160</t>
+        </is>
+      </c>
+      <c r="I7" s="26" t="inlineStr">
+        <is>
+          <t>RTGSAUD1-0736</t>
+        </is>
+      </c>
+      <c r="J7" s="26" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="K7" s="159" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="L7" s="26" t="inlineStr">
+        <is>
+          <t>Principal Payment</t>
+        </is>
+      </c>
+      <c r="M7" s="82" t="inlineStr">
+        <is>
+          <t>10,000.00</t>
+        </is>
+      </c>
+      <c r="N7" s="73" t="n">
+        <v>100</v>
+      </c>
+      <c r="O7" s="26" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -30856,8 +32218,8 @@
   </sheetPr>
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -31481,7 +32843,104 @@
       </c>
     </row>
     <row r="7">
-      <c r="H7" s="86" t="n"/>
+      <c r="A7" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C7" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="D7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="E7" s="159" t="inlineStr">
+        <is>
+          <t>60001160</t>
+        </is>
+      </c>
+      <c r="F7" s="159" t="inlineStr">
+        <is>
+          <t>04-Feb-2021</t>
+        </is>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>FIXED Interest Due</t>
+        </is>
+      </c>
+      <c r="H7" s="26" t="inlineStr">
+        <is>
+          <t>ESPS11810226</t>
+        </is>
+      </c>
+      <c r="I7" s="26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J7" s="26" t="inlineStr">
+        <is>
+          <t>Projected Due</t>
+        </is>
+      </c>
+      <c r="K7" s="159" t="inlineStr">
+        <is>
+          <t>8.77</t>
+        </is>
+      </c>
+      <c r="L7" s="26" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="M7" s="26" t="inlineStr">
+        <is>
+          <t>Payments</t>
+        </is>
+      </c>
+      <c r="N7" s="26" t="inlineStr">
+        <is>
+          <t>Awaiting Approval</t>
+        </is>
+      </c>
+      <c r="O7" s="26" t="inlineStr">
+        <is>
+          <t>Interest Payment</t>
+        </is>
+      </c>
+      <c r="P7" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="Q7" s="26" t="inlineStr">
+        <is>
+          <t>RTGSAUD1-0736</t>
+        </is>
+      </c>
+      <c r="R7" s="73" t="n">
+        <v>100</v>
+      </c>
+      <c r="S7" s="26" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+      <c r="T7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM12102019171714</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="H8" s="86" t="n"/>
@@ -31499,11 +32958,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B6" sqref="B6"/>
+      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B7" sqref="B7:AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -32420,6 +33879,151 @@
         </is>
       </c>
       <c r="AD6" s="159" t="inlineStr">
+        <is>
+          <t>04-Feb-2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="157">
+      <c r="A7" s="108" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="165" t="inlineStr">
+        <is>
+          <t>COMSEE_SCENARIO_07</t>
+        </is>
+      </c>
+      <c r="C7" s="159" t="inlineStr">
+        <is>
+          <t>05-Jan-2021</t>
+        </is>
+      </c>
+      <c r="D7" s="159" t="inlineStr">
+        <is>
+          <t>06-Mar-2021</t>
+        </is>
+      </c>
+      <c r="E7" s="148" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="F7" s="148" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="G7" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="H7" s="159" t="inlineStr">
+        <is>
+          <t>RTGS1</t>
+        </is>
+      </c>
+      <c r="I7" s="26" t="inlineStr">
+        <is>
+          <t>06000505</t>
+        </is>
+      </c>
+      <c r="J7" s="26" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="K7" s="26" t="inlineStr">
+        <is>
+          <t>DOIT</t>
+        </is>
+      </c>
+      <c r="L7" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="M7" s="26" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+        </is>
+      </c>
+      <c r="N7" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="O7" s="159" t="inlineStr">
+        <is>
+          <t>CSSC7_TERM09102020115930</t>
+        </is>
+      </c>
+      <c r="P7" s="159" t="inlineStr">
+        <is>
+          <t>COMSEE_SC7_09102020115127</t>
+        </is>
+      </c>
+      <c r="Q7" s="26" t="inlineStr">
+        <is>
+          <t>ONG000000000213</t>
+        </is>
+      </c>
+      <c r="R7" s="26" t="inlineStr">
+        <is>
+          <t>Commitment Fee</t>
+        </is>
+      </c>
+      <c r="S7" s="159" t="inlineStr">
+        <is>
+          <t>Line Fee</t>
+        </is>
+      </c>
+      <c r="T7" s="159" t="inlineStr">
+        <is>
+          <t>FACI Fee Due</t>
+        </is>
+      </c>
+      <c r="U7" s="159" t="inlineStr">
+        <is>
+          <t>28-Jan-2021</t>
+        </is>
+      </c>
+      <c r="V7" s="26" t="inlineStr">
+        <is>
+          <t>04-Jun-2018</t>
+        </is>
+      </c>
+      <c r="W7" s="26" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="X7" s="26" t="n">
+        <v>9.859999999999999</v>
+      </c>
+      <c r="Z7" s="40" t="inlineStr">
+        <is>
+          <t>90,000.00</t>
+        </is>
+      </c>
+      <c r="AA7" s="40" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="AB7" s="26" t="inlineStr">
+        <is>
+          <t>Actual/365</t>
+        </is>
+      </c>
+      <c r="AC7" s="26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD7" s="159" t="inlineStr">
         <is>
           <t>04-Feb-2021</t>
         </is>

</xml_diff>

<commit_message>
GDE-7319 Test Case for CommSee Outstanding V2 for Fixed Rate Loan with Non Zero Cycle Due
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -31501,12 +31501,12 @@
       </c>
       <c r="BI7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="BM7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="BN7" t="inlineStr">

</xml_diff>

<commit_message>
GDE-7323 CommSee Outstanding V2 for Fixed Rate Loan with Multiple Accruals
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -29384,27 +29384,27 @@
       </c>
       <c r="P7" s="159" t="inlineStr">
         <is>
-          <t>2021-02-04</t>
+          <t>2021-03-04</t>
         </is>
       </c>
       <c r="Q7" s="159" t="inlineStr">
         <is>
-          <t>2021-01-28</t>
+          <t>2021-02-25</t>
         </is>
       </c>
       <c r="R7" s="159" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-03-03</t>
         </is>
       </c>
       <c r="S7" s="159" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>339.72</t>
         </is>
       </c>
       <c r="T7" s="159" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>339.72</t>
         </is>
       </c>
       <c r="U7" s="159" t="inlineStr">
@@ -31501,12 +31501,12 @@
       </c>
       <c r="BI7" t="inlineStr">
         <is>
-          <t>2.19</t>
+          <t>67.94</t>
         </is>
       </c>
       <c r="BM7" t="inlineStr">
         <is>
-          <t>2.19</t>
+          <t>67.94</t>
         </is>
       </c>
       <c r="BN7" t="inlineStr">

</xml_diff>

<commit_message>
GDE-7321 CommSee Outstanding V2 Paid To Date
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="29" activeTab="33" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="32" activeTab="36" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -22561,8 +22561,8 @@
   <dimension ref="A1:DC7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V6" sqref="V6"/>
+      <pane xSplit="2" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -25768,7 +25768,7 @@
       </c>
       <c r="C7" s="159" t="inlineStr">
         <is>
-          <t>3000848</t>
+          <t>3000864</t>
         </is>
       </c>
       <c r="D7" s="165" t="inlineStr">
@@ -25793,17 +25793,17 @@
       </c>
       <c r="H7" s="159" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_09102020115127</t>
+          <t>COMSEE_SC7_12102020154722</t>
         </is>
       </c>
       <c r="I7" s="159" t="inlineStr">
         <is>
-          <t>1001040</t>
+          <t>1001075</t>
         </is>
       </c>
       <c r="J7" s="159" t="inlineStr">
         <is>
-          <t>2021-01-28</t>
+          <t>2021-02-28</t>
         </is>
       </c>
       <c r="K7" s="159" t="inlineStr">
@@ -25887,7 +25887,7 @@
       </c>
       <c r="AB7" s="159" t="inlineStr">
         <is>
-          <t>CSSC7_TERM09102020115930</t>
+          <t>CSSC7_TERM12102020155623</t>
         </is>
       </c>
       <c r="AC7" s="149" t="inlineStr">
@@ -26084,7 +26084,7 @@
       </c>
       <c r="BQ7" s="159" t="inlineStr">
         <is>
-          <t>28-Jan-2022</t>
+          <t>28-Feb-2022</t>
         </is>
       </c>
       <c r="BR7" s="26" t="inlineStr">
@@ -27806,22 +27806,22 @@
       </c>
       <c r="C7" s="159" t="inlineStr">
         <is>
-          <t>CSSC7_TERM09102020115930</t>
+          <t>CSSC7_TERM12102020155623</t>
         </is>
       </c>
       <c r="D7" s="159" t="inlineStr">
         <is>
-          <t>3000848</t>
+          <t>3000864</t>
         </is>
       </c>
       <c r="E7" s="159" t="inlineStr">
         <is>
-          <t>2021-01-28</t>
+          <t>2021-02-28</t>
         </is>
       </c>
       <c r="F7" s="159" t="inlineStr">
         <is>
-          <t>2022-02-27</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="G7" s="26" t="inlineStr">
@@ -27933,7 +27933,7 @@
       </c>
       <c r="AD7" s="159" t="inlineStr">
         <is>
-          <t>2022-01-28</t>
+          <t>2022-02-28</t>
         </is>
       </c>
       <c r="AE7" s="109" t="inlineStr">
@@ -27943,7 +27943,7 @@
       </c>
       <c r="AF7" s="159" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_09102020115127</t>
+          <t>COMSEE_SC7_12102020154722</t>
         </is>
       </c>
       <c r="AG7" s="26" t="inlineStr">
@@ -28052,7 +28052,7 @@
   </sheetPr>
   <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
@@ -29329,7 +29329,7 @@
       </c>
       <c r="E7" s="159" t="inlineStr">
         <is>
-          <t>3000848</t>
+          <t>3000864</t>
         </is>
       </c>
       <c r="F7" s="159" t="inlineStr">
@@ -29344,12 +29344,12 @@
       </c>
       <c r="H7" s="159" t="inlineStr">
         <is>
-          <t>CSSC7_TERM09102020115930</t>
+          <t>CSSC7_TERM12102020155623</t>
         </is>
       </c>
       <c r="I7" s="159" t="inlineStr">
         <is>
-          <t>ONG000000000604</t>
+          <t>ONG000000000618</t>
         </is>
       </c>
       <c r="J7" s="159" t="inlineStr">
@@ -29374,37 +29374,37 @@
       </c>
       <c r="N7" s="159" t="inlineStr">
         <is>
-          <t>2021-01-28</t>
+          <t>2021-02-28</t>
         </is>
       </c>
       <c r="O7" s="159" t="inlineStr">
         <is>
-          <t>2022-02-27</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="P7" s="159" t="inlineStr">
         <is>
-          <t>2021-03-04</t>
+          <t>2021-05-28</t>
         </is>
       </c>
       <c r="Q7" s="159" t="inlineStr">
         <is>
-          <t>2021-02-25</t>
+          <t>2021-02-28</t>
         </is>
       </c>
       <c r="R7" s="159" t="inlineStr">
         <is>
-          <t>2021-03-03</t>
+          <t>2021-05-27</t>
         </is>
       </c>
       <c r="S7" s="159" t="inlineStr">
         <is>
-          <t>339.72</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="T7" s="159" t="inlineStr">
         <is>
-          <t>339.72</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="U7" s="159" t="inlineStr">
@@ -29414,7 +29414,7 @@
       </c>
       <c r="V7" s="159" t="inlineStr">
         <is>
-          <t>CSSC7_TERM09102020115930</t>
+          <t>CSSC7_TERM12102020155623</t>
         </is>
       </c>
       <c r="W7" s="150" t="inlineStr">
@@ -29529,7 +29529,7 @@
   <dimension ref="A1:BN7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -31221,7 +31221,7 @@
       </c>
       <c r="E7" s="159" t="inlineStr">
         <is>
-          <t>3000848</t>
+          <t>3000864</t>
         </is>
       </c>
       <c r="F7" s="159" t="inlineStr">
@@ -31236,7 +31236,7 @@
       </c>
       <c r="H7" s="159" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_09102020115127</t>
+          <t>COMSEE_SC7_12102020154722</t>
         </is>
       </c>
       <c r="I7" s="1" t="inlineStr">
@@ -31246,7 +31246,7 @@
       </c>
       <c r="J7" s="159" t="inlineStr">
         <is>
-          <t>CSSC7_TERM09102020115930</t>
+          <t>CSSC7_TERM12102020155623</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
@@ -31286,12 +31286,12 @@
       </c>
       <c r="R7" s="159" t="inlineStr">
         <is>
-          <t>60001160</t>
+          <t>60001177</t>
         </is>
       </c>
       <c r="S7" s="159" t="inlineStr">
         <is>
-          <t>60001160</t>
+          <t>60001177</t>
         </is>
       </c>
       <c r="T7" s="1" t="inlineStr">
@@ -31356,17 +31356,17 @@
       </c>
       <c r="AF7" s="26" t="inlineStr">
         <is>
-          <t>2021-01-28</t>
+          <t>2021-02-28</t>
         </is>
       </c>
       <c r="AG7" s="159" t="inlineStr">
         <is>
-          <t>27-Feb-2022</t>
+          <t>30-Mar-2022</t>
         </is>
       </c>
       <c r="AH7" s="159" t="inlineStr">
         <is>
-          <t>2022-02-27</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="AI7" s="159" t="inlineStr">
@@ -31501,17 +31501,17 @@
       </c>
       <c r="BI7" t="inlineStr">
         <is>
-          <t>67.94</t>
+          <t>4.38</t>
         </is>
       </c>
       <c r="BM7" t="inlineStr">
         <is>
-          <t>67.94</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="BN7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>4.38</t>
         </is>
       </c>
     </row>
@@ -32141,12 +32141,12 @@
       </c>
       <c r="C7" s="159" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_09102020115127</t>
+          <t>COMSEE_SC7_12102020154722</t>
         </is>
       </c>
       <c r="D7" s="159" t="inlineStr">
         <is>
-          <t>CSSC7_TERM09102020115930</t>
+          <t>CSSC7_TERM12102020155623</t>
         </is>
       </c>
       <c r="E7" s="26" t="inlineStr">
@@ -32166,7 +32166,7 @@
       </c>
       <c r="H7" s="159" t="inlineStr">
         <is>
-          <t>60001160</t>
+          <t>60001177</t>
         </is>
       </c>
       <c r="I7" s="26" t="inlineStr">
@@ -32218,8 +32218,8 @@
   </sheetPr>
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:T7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -32855,22 +32855,22 @@
       </c>
       <c r="C7" s="159" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_09102020115127</t>
+          <t>COMSEE_SC7_12102020154722</t>
         </is>
       </c>
       <c r="D7" s="159" t="inlineStr">
         <is>
-          <t>CSSC7_TERM09102020115930</t>
+          <t>CSSC7_TERM12102020155623</t>
         </is>
       </c>
       <c r="E7" s="159" t="inlineStr">
         <is>
-          <t>60001160</t>
+          <t>60001177</t>
         </is>
       </c>
       <c r="F7" s="159" t="inlineStr">
         <is>
-          <t>04-Feb-2021</t>
+          <t>08-Mar-2021</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
@@ -32878,9 +32878,9 @@
           <t>FIXED Interest Due</t>
         </is>
       </c>
-      <c r="H7" s="26" t="inlineStr">
-        <is>
-          <t>ESPS11810226</t>
+      <c r="H7" s="159" t="inlineStr">
+        <is>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="I7" s="26" t="inlineStr">
@@ -32895,7 +32895,7 @@
       </c>
       <c r="K7" s="159" t="inlineStr">
         <is>
-          <t>8.77</t>
+          <t>4.38</t>
         </is>
       </c>
       <c r="L7" s="26" t="inlineStr">
@@ -32923,17 +32923,17 @@
           <t>RTGS</t>
         </is>
       </c>
-      <c r="Q7" s="26" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-0736</t>
+      <c r="Q7" s="159" t="inlineStr">
+        <is>
+          <t>RTGS1</t>
         </is>
       </c>
       <c r="R7" s="73" t="n">
         <v>100</v>
       </c>
-      <c r="S7" s="26" t="inlineStr">
-        <is>
-          <t>CB001/Hold for Investment - Australia/BP_CML</t>
+      <c r="S7" s="159" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/IT_COL</t>
         </is>
       </c>
       <c r="T7" s="159" t="inlineStr">
@@ -33897,12 +33897,12 @@
       </c>
       <c r="C7" s="159" t="inlineStr">
         <is>
-          <t>05-Jan-2021</t>
+          <t>06-Feb-2021</t>
         </is>
       </c>
       <c r="D7" s="159" t="inlineStr">
         <is>
-          <t>06-Mar-2021</t>
+          <t>07-Apr-2021</t>
         </is>
       </c>
       <c r="E7" s="148" t="inlineStr">
@@ -33917,7 +33917,7 @@
       </c>
       <c r="G7" s="159" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_09102020115127</t>
+          <t>COMSEE_SC7_12102020154722</t>
         </is>
       </c>
       <c r="H7" s="159" t="inlineStr">
@@ -33957,12 +33957,12 @@
       </c>
       <c r="O7" s="159" t="inlineStr">
         <is>
-          <t>CSSC7_TERM09102020115930</t>
+          <t>CSSC7_TERM12102020155623</t>
         </is>
       </c>
       <c r="P7" s="159" t="inlineStr">
         <is>
-          <t>COMSEE_SC7_09102020115127</t>
+          <t>COMSEE_SC7_12102020154722</t>
         </is>
       </c>
       <c r="Q7" s="26" t="inlineStr">
@@ -33987,7 +33987,7 @@
       </c>
       <c r="U7" s="159" t="inlineStr">
         <is>
-          <t>28-Jan-2021</t>
+          <t>28-Feb-2021</t>
         </is>
       </c>
       <c r="V7" s="26" t="inlineStr">
@@ -34025,7 +34025,7 @@
       </c>
       <c r="AD7" s="159" t="inlineStr">
         <is>
-          <t>04-Feb-2021</t>
+          <t>08-Mar-2021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add tc and keyword-GDE-7324
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\CommSee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC37C97-7177-44CE-A987-84512C85BE97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA9142-EC02-4D84-972B-E7A68E46AED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6603,8 +6603,8 @@
   </sheetPr>
   <dimension ref="A1:BI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB23" sqref="BB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>